<commit_message>
Final Version Revisi 1
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070"/>
+    <workbookView windowWidth="18530" windowHeight="7070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -86,10 +86,10 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Williandy</t>
-  </si>
-  <si>
-    <t>Edgar</t>
+    <t>WILLIANDY</t>
+  </si>
+  <si>
+    <t>EDGAR</t>
   </si>
   <si>
     <t>Industry</t>
@@ -107,10 +107,10 @@
     <t>Jabatan</t>
   </si>
   <si>
-    <t>Section Head</t>
-  </si>
-  <si>
-    <t>Section Leg</t>
+    <t>SECTION HEAD</t>
+  </si>
+  <si>
+    <t>SECTION LEG</t>
   </si>
   <si>
     <t>Value DDL</t>
@@ -121,9 +121,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -150,15 +150,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,45 +164,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -219,6 +172,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -234,6 +218,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -249,31 +265,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,187 +301,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,15 +534,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -554,6 +545,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,17 +586,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -595,152 +595,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -751,7 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1074,7 +1073,7 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1173,8 +1172,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" s="6" customFormat="1" spans="1:1">
-      <c r="A12" s="7"/>
+    <row r="12" s="3" customFormat="1" spans="1:1">
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="3"/>
@@ -1220,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Version Code Review 2
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="7070"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Status</t>
   </si>
@@ -41,22 +41,37 @@
     <t>$Email registrasi</t>
   </si>
   <si>
-    <t>kevin.edgar@ad-ins.com</t>
+    <t>KVNEDGAR@GGG.COM</t>
+  </si>
+  <si>
+    <t>BOCCHITHERCK@ANIME.COM</t>
   </si>
   <si>
     <t>$Username registrasi</t>
   </si>
   <si>
-    <t>KevinKevini</t>
+    <t>PenggunaTrail</t>
+  </si>
+  <si>
+    <t>Bocchi</t>
   </si>
   <si>
     <t>$Pass registrasi</t>
   </si>
   <si>
-    <t>Xavier123!</t>
+    <t>Xavier1234!</t>
+  </si>
+  <si>
+    <t>GuitarHero111!!</t>
   </si>
   <si>
     <t>$Pass_confirm registrasi</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Done well</t>
   </si>
   <si>
     <t>Data Edit Profile</t>
@@ -121,9 +136,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -142,6 +157,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,8 +165,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,6 +219,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -172,17 +272,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,92 +286,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,187 +316,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,9 +512,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,6 +541,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,26 +584,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -595,7 +610,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -616,127 +631,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1073,14 +1088,15 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="20.0909090909091" customWidth="1"/>
-    <col min="2" max="3" width="21.7272727272727" customWidth="1"/>
+    <col min="2" max="2" width="21.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="28.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1136,40 +1152,40 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:1">
@@ -1219,7 +1235,7 @@
   <sheetPr/>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1234,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1245,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1271,67 +1287,67 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B13" s="4">
         <v>123456789012</v>
@@ -1342,18 +1358,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5">
         <v>99</v>

</xml_diff>

<commit_message>
Code Review 4 Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070"/>
+    <workbookView windowWidth="18530" windowHeight="7070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <t>Username Login</t>
   </si>
   <si>
-    <t>willis.wy@ad-ins.com</t>
+    <t>WILLIS.WY@AD-INS.COM</t>
   </si>
   <si>
     <t>Password Login</t>
@@ -136,10 +136,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -157,6 +157,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -164,6 +172,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -171,16 +219,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,31 +251,29 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,30 +281,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,39 +294,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,49 +316,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,61 +478,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,67 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,8 +513,53 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,52 +583,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,8 +591,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,15 +610,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -628,130 +628,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1088,7 +1088,7 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1221,14 +1221,14 @@
   <sheetPr/>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
-    <col min="2" max="3" width="20.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="24.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1280,10 +1280,10 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Review null + API Paging On progress
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="7070" windowWidth="18530"/>
+    <workbookView windowWidth="18530" windowHeight="7070" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" r:id="rId1" sheetId="1"/>
-    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Status</t>
   </si>
@@ -23,9 +24,15 @@
     <t>Unexecuted</t>
   </si>
   <si>
+    <t>Failed</t>
+  </si>
+  <si>
     <t>Reason failed</t>
   </si>
   <si>
+    <t>;Submit Gagal</t>
+  </si>
+  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -74,19 +81,19 @@
     <t>Data Edit Profile</t>
   </si>
   <si>
-    <t>Username Login</t>
+    <t>$Username Login</t>
   </si>
   <si>
     <t>KVNEDGAR@ADIN.COM</t>
   </si>
   <si>
-    <t>Password Login</t>
+    <t>$Password Login</t>
   </si>
   <si>
     <t>Xavier123!</t>
   </si>
   <si>
-    <t>Nama Depan</t>
+    <t>$Nama Depan</t>
   </si>
   <si>
     <t>WILLIS</t>
@@ -95,7 +102,7 @@
     <t>KEPIN</t>
   </si>
   <si>
-    <t>Last Name</t>
+    <t>$Last Name</t>
   </si>
   <si>
     <t>WILLIANDY</t>
@@ -104,7 +111,7 @@
     <t>EDGAR</t>
   </si>
   <si>
-    <t>Nama Tenant</t>
+    <t>$Nama Tenant</t>
   </si>
   <si>
     <t>AD-INS</t>
@@ -113,7 +120,7 @@
     <t>ADIN</t>
   </si>
   <si>
-    <t>Industry</t>
+    <t>$Industry</t>
   </si>
   <si>
     <t>QA</t>
@@ -149,16 +156,28 @@
     <t>SECTION LEG</t>
   </si>
   <si>
-    <t>Kode Negara</t>
+    <t>$Kode Negara</t>
   </si>
   <si>
     <t>Indonesia +62</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>;Submit Gagal</t>
+    <t>$Nama API KEY</t>
+  </si>
+  <si>
+    <t>SIAPA</t>
+  </si>
+  <si>
+    <t>PACARKU_?</t>
+  </si>
+  <si>
+    <t>$Tipe API KEY</t>
+  </si>
+  <si>
+    <t>PRODUCTION</t>
+  </si>
+  <si>
+    <t>TRIAL</t>
   </si>
 </sst>
 </file>
@@ -187,11 +206,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,6 +283,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -212,118 +299,50 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -346,127 +365,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,49 +539,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,11 +559,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,17 +598,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,239 +656,219 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="10" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="4" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="17" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="21" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="21" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
-    <cellStyle builtinId="10" name="Note" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -863,10 +882,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1030,21 +1049,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1061,7 +1080,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1114,20 +1133,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7272727272727" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.0909090909091" collapsed="true"/>
+    <col min="1" max="1" width="20.0909090909091" customWidth="1"/>
+    <col min="2" max="2" width="21.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="22.7272727272727" customWidth="1"/>
+    <col min="4" max="4" width="21.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1138,28 +1157,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <f>COUNTIFS(Register!A8:A20,"*$*",Register!B8:B20,"")</f>
@@ -1174,54 +1193,54 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row customFormat="1" r="12" s="3" spans="1:1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:1">
       <c r="A12" s="6"/>
     </row>
     <row r="13" spans="2:3">
@@ -1257,26 +1276,26 @@
       <c r="C20" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.9090909090909" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.5454545454545" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="27.9090909090909" customWidth="1"/>
+    <col min="3" max="3" width="29.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1292,17 +1311,17 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <f>COUNTIFS(Register!A8:A20,"*$*",Register!B8:B20,"")</f>
@@ -1313,102 +1332,102 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4">
         <v>123456789012</v>
@@ -1419,28 +1438,143 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="23.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="22.7272727272727" customWidth="1"/>
+    <col min="4" max="4" width="21.0909090909091" customWidth="1"/>
+    <col min="5" max="6" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIFS(Register!A8:A20,"*$*",Register!B8:B20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>IF(ISBLANK(Register!C8:C11),1,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ATEENDIGO 17 18 19 20 Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070"/>
+    <workbookView windowWidth="18530" windowHeight="7070" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>Status</t>
   </si>
@@ -198,7 +198,7 @@
     <t>$Nama API KEY</t>
   </si>
   <si>
-    <t>SEKUYGEMING</t>
+    <t>BOLEHHH</t>
   </si>
   <si>
     <t>PACARKU_?</t>
@@ -210,16 +210,16 @@
     <t>$Tipe API KEY</t>
   </si>
   <si>
+    <t>TRIAL</t>
+  </si>
+  <si>
     <t>PRODUCTION</t>
   </si>
   <si>
-    <t>TRIAL</t>
-  </si>
-  <si>
     <t>$Edit Nama API</t>
   </si>
   <si>
-    <t>BAGAIMANA</t>
+    <t>YAUDAHHH</t>
   </si>
   <si>
     <t>DEMI</t>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>INACTIVE</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
   </si>
 </sst>
 </file>
@@ -240,8 +243,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -260,6 +263,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -268,83 +355,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,17 +371,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,7 +400,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -419,49 +422,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,133 +578,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,6 +627,41 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,53 +698,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -725,18 +719,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,130 +749,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1209,17 +1212,17 @@
   <sheetPr/>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.0909090909091" customWidth="1"/>
-    <col min="2" max="2" width="21.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="28.4545454545455" customWidth="1"/>
-    <col min="4" max="4" width="21.0909090909091" customWidth="1"/>
-    <col min="5" max="5" width="21.9090909090909" customWidth="1"/>
+    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.9090909090909" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1641,17 +1644,17 @@
   <sheetPr/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="23" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="23.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="22.7272727272727" customWidth="1"/>
+    <col min="4" max="4" width="21.0909090909091" customWidth="1"/>
+    <col min="5" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1755,7 +1758,7 @@
         <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1780,7 +1783,7 @@
         <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Code Review API Key 1 Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="89">
   <si>
     <t>Status</t>
   </si>
@@ -195,10 +195,33 @@
     <t>Indonesia +62</t>
   </si>
   <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Done well</t>
+  </si>
+  <si>
+    <t>;FailedStoreDB;FailedStoreDB</t>
+  </si>
+  <si>
+    <t>Sukses 100%</t>
+  </si>
+  <si>
+    <t>Controller berhasil</t>
+  </si>
+  <si>
+    <t>Add gagal production 
+sudah aktif</t>
+  </si>
+  <si>
+    <t>Add gagal karena trial 
+sudah aktif</t>
+  </si>
+  <si>
     <t>$Nama API KEY</t>
   </si>
   <si>
-    <t>BOLEHHH</t>
+    <t>ITSTIME</t>
   </si>
   <si>
     <t>PACARKU_?</t>
@@ -207,6 +230,9 @@
     <t>SIUUU</t>
   </si>
   <si>
+    <t>WINWIN</t>
+  </si>
+  <si>
     <t>$Tipe API KEY</t>
   </si>
   <si>
@@ -219,13 +245,16 @@
     <t>$Edit Nama API</t>
   </si>
   <si>
-    <t>YAUDAHHH</t>
+    <t>KURENGGG</t>
   </si>
   <si>
     <t>DEMI</t>
   </si>
   <si>
-    <t>KENAPA</t>
+    <t>RUNNN</t>
+  </si>
+  <si>
+    <t>HOTDAMN</t>
   </si>
   <si>
     <t>$Edit Status API</t>
@@ -235,6 +264,27 @@
   </si>
   <si>
     <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>SearchTipeAPI</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>SearchStatusAPI</t>
+  </si>
+  <si>
+    <t>TC Add &amp; Edit Controller</t>
+  </si>
+  <si>
+    <t>Add API KEY?(Yes/No)</t>
+  </si>
+  <si>
+    <t>Edit API KEY?(Yes/No)</t>
+  </si>
+  <si>
+    <t>Copy API Link?(Yes/No)</t>
   </si>
 </sst>
 </file>
@@ -242,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -260,6 +310,59 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -279,52 +382,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -340,21 +397,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -363,6 +405,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -371,20 +442,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -399,13 +456,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -422,31 +472,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,151 +646,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,26 +681,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -662,6 +692,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,6 +722,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -692,6 +742,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,27 +778,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -749,136 +799,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1274,7 +1327,7 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1344,111 +1397,111 @@
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="8">
         <v>999999</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="10">
         <v>1</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="10">
         <v>2</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="10">
         <v>2</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:1">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,7 +1567,7 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1533,10 +1586,10 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1544,7 +1597,7 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1552,7 +1605,7 @@
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1560,10 +1613,10 @@
       <c r="A12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1571,10 +1624,10 @@
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1582,10 +1635,10 @@
       <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1604,10 +1657,10 @@
       <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1615,10 +1668,10 @@
       <c r="A17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1626,10 +1679,10 @@
       <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1642,10 +1695,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1653,57 +1706,88 @@
     <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
     <col min="2" max="2" width="23.3636363636364" customWidth="1"/>
     <col min="3" max="3" width="22.7272727272727" customWidth="1"/>
-    <col min="4" max="4" width="21.0909090909091" customWidth="1"/>
-    <col min="5" max="6" width="23" customWidth="1"/>
+    <col min="4" max="5" width="27.9090909090909" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <f>COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f>COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f>COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIFS($A$8:$A$20,"*$*",D8:D20,"")</f>
+        <f>COUNTIFS($A$8:$A$22,"*$*",D8:D22,"")</f>
         <v>0</v>
       </c>
+      <c r="E4">
+        <f>COUNTIFS($A$8:$A$22,"*$*",E8:E22,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1714,6 +1798,9 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1721,72 +1808,176 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:5">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="D13" t="s">
-        <v>71</v>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:5">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Review Ko Fen Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="117">
   <si>
     <t>Status</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>Delete File ?(Yes/No)</t>
+  </si>
+  <si>
+    <t>Berhasil Save tapi mandatory tidak lengkap</t>
   </si>
 </sst>
 </file>
@@ -414,75 +417,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -497,11 +433,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -513,16 +494,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,7 +540,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,7 +548,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,37 +575,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,139 +719,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,17 +778,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,11 +802,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,19 +835,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,16 +867,18 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="5" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
@@ -893,130 +896,130 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="7" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="17" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="5" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="5" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="14" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="15" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="8" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="7" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="7" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="6" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="27" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="27" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1792,8 +1795,8 @@
   <sheetPr/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1873,7 +1876,7 @@
         <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="K2" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Review 2 OCR KK Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="2" activeTab="5"/>
+    <workbookView activeTab="5" firstSheet="2" windowHeight="7070" windowWidth="18530"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" sheetId="1" r:id="rId1"/>
-    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
-    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
-    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
-    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
-    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
-    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
-    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
+    <sheet name="Register" r:id="rId1" sheetId="1"/>
+    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
+    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
+    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
+    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
+    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
+    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
+    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="211">
   <si>
     <t>Status</t>
   </si>
@@ -539,6 +539,10 @@
     <t>Unexecited</t>
   </si>
   <si>
+    <t>Eksekusi berhasil, karena KK valid 
+dan parameter terpenuhi</t>
+  </si>
+  <si>
     <t>Eksekusi berhasil, tapi data yang dibaca tidak akan punya confidence level tinggi</t>
   </si>
   <si>
@@ -552,6 +556,9 @@
 kecil tidak berpengaruh</t>
   </si>
   <si>
+    <t>Eksekusi akan tetap berhasil, karena rotasi seharusnya tidak berpengaruh</t>
+  </si>
+  <si>
     <t>Punya 50% tingkat eksekusi berhasil karena gambar tidak tajam</t>
   </si>
   <si>
@@ -561,10 +568,13 @@
     <t>Gambar tidak bisa dibaca oleh robot karena gambar terlalu pecah</t>
   </si>
   <si>
-    <t>KK tida terbaca karena semua teks dalam keadaan terbalik/mirror</t>
-  </si>
-  <si>
-    <t>Eksekusi akan tetap berhasil, karena rotasi seharusnya tidak berpengaruh</t>
+    <t>KK tidak terbaca karena semua teks dalam keadaan terbalik/mirror</t>
+  </si>
+  <si>
+    <t>Eksekusi gagal, karena resolusi dan ukuran file terlalu besar</t>
+  </si>
+  <si>
+    <t>Eksekusi gagal, karena resolusi terlalu rendah</t>
   </si>
   <si>
     <t>Object Repository/ImageFolder/KK/KKWorks1.jpg</t>
@@ -582,6 +592,9 @@
     <t>Object Repository/ImageFolder/KK/KKblackwhiterotated.jpg</t>
   </si>
   <si>
+    <t>Object Repository/ImageFolder/KK/KKupsidedown1.jpg</t>
+  </si>
+  <si>
     <t>Object Repository/ImageFolder/KK/KKblurlevel1.jpg</t>
   </si>
   <si>
@@ -594,7 +607,16 @@
     <t>Object Repository/ImageFolder/KK/KKreverse1.jpg</t>
   </si>
   <si>
-    <t>Object Repository/ImageFolder/KK/KKupsidedown1.jpg</t>
+    <t>Object Repository/ImageFolder/KK/KKrestoobig1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/KK/KKrestoobig2.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/KK/KKrestoosmall1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/KK/KKrestoosmall2.jpg</t>
   </si>
   <si>
     <t>hxycaczn-ybfe-mmd9-9b5d-pwj7kibgacny</t>
@@ -656,10 +678,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -690,16 +712,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -713,6 +735,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -723,9 +753,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -746,15 +776,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -783,11 +805,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -798,15 +819,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -842,13 +864,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,13 +888,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,43 +924,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,7 +942,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -944,19 +978,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,25 +1020,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,13 +1032,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1016,13 +1044,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,15 +1073,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1071,6 +1084,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1090,15 +1121,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1110,6 +1132,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1131,15 +1162,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1150,224 +1172,224 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="10" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="11" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="26" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="7" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="7" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
+    <cellStyle builtinId="10" name="Note" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1381,10 +1403,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1548,21 +1570,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1579,7 +1601,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1632,9 +1654,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
@@ -1642,11 +1664,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1688,7 +1710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:7">
+    <row ht="43.5" r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1716,31 +1738,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1834,7 +1856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1929,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1974,19 +1996,19 @@
       <c r="C21" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C14:D14 F14:G14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1994,10 +2016,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2025,7 +2047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -2247,18 +2269,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C16" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -2266,16 +2288,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2307,7 +2329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="29" spans="1:9">
+    <row ht="29" r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2336,7 +2358,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:9">
+    <row ht="29" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2370,39 +2392,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2636,7 +2658,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="3" t="s">
         <v>111</v>
       </c>
@@ -2759,7 +2781,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -2770,15 +2792,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -2786,16 +2808,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2853,7 +2875,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:11">
+    <row ht="43.5" r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2893,35 +2915,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>119</v>
       </c>
@@ -2986,19 +3008,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:J12"/>
@@ -3006,10 +3028,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3052,7 +3074,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:10">
+    <row ht="29" r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3089,43 +3111,43 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -3290,7 +3312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="13" s="1" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>154</v>
       </c>
@@ -3360,37 +3382,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1"/>
-    <col min="7" max="9" width="45.1818181818182" customWidth="1"/>
-    <col min="10" max="10" width="42.3636363636364" customWidth="1"/>
-    <col min="11" max="11" width="48.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>166</v>
@@ -3419,48 +3443,75 @@
       <c r="K1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="29" spans="1:11">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row ht="29" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>176</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3469,31 +3520,31 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f>COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",D8:D20,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",E8:E20,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",F8:F20,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",G8:G20,"")</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",H8:H20,"")</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$20,"*$*",I8:I20,"")</f>
         <v>0</v>
       </c>
       <c r="J4">
@@ -3502,55 +3553,83 @@
       </c>
       <c r="K4">
         <f>COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",L8:L20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",M8:M20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",N8:N20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",O8:O20,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G8" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="K8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>188</v>
+      </c>
+      <c r="L8" t="s">
+        <v>189</v>
+      </c>
+      <c r="M8" t="s">
+        <v>190</v>
+      </c>
+      <c r="N8" t="s">
+        <v>191</v>
+      </c>
+      <c r="O8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>149</v>
@@ -3579,8 +3658,20 @@
       <c r="K9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>149</v>
+      </c>
+      <c r="M9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9" t="s">
+        <v>149</v>
+      </c>
+      <c r="O9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -3614,8 +3705,20 @@
       <c r="K10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -3646,8 +3749,23 @@
       <c r="J11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -3678,13 +3796,28 @@
       <c r="J12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row customFormat="1" r="13" s="1" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -3707,19 +3840,31 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
         <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -3739,31 +3884,43 @@
         <v>161</v>
       </c>
       <c r="G15" t="s">
+        <v>193</v>
+      </c>
+      <c r="H15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>164</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>165</v>
       </c>
-      <c r="K15" t="s">
-        <v>186</v>
+      <c r="L15" t="s">
+        <v>157</v>
+      </c>
+      <c r="M15" t="s">
+        <v>158</v>
+      </c>
+      <c r="N15" t="s">
+        <v>163</v>
+      </c>
+      <c r="O15" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="A11:O12"/>
@@ -3771,17 +3928,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="38.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="10" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="40.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3839,43 +3996,43 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
         <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="H2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="I2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="J2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="L2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="M2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="N2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="O2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3906,35 +4063,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -3958,56 +4115,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" ht="43.5" spans="1:15">
+    <row ht="43.5" r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -4198,7 +4355,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="13" s="1" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>154</v>
       </c>
@@ -4282,7 +4439,7 @@
         <v>165</v>
       </c>
       <c r="K15" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="L15" t="s">
         <v>157</v>
@@ -4298,15 +4455,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -4314,16 +4471,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5454545454545" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4363,7 +4520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:10">
+    <row ht="29" r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4404,39 +4561,39 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -4513,7 +4670,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="13" s="1" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>154</v>
       </c>
@@ -4583,7 +4740,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
APIAAS Basic Feature + TC OCR KTP KK STNK Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="2" windowHeight="7070" windowWidth="18530"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" r:id="rId1" sheetId="1"/>
-    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
-    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
-    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
-    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
-    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
-    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
-    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
+    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
+    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
+    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
+    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
+    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="212">
   <si>
     <t>Status</t>
   </si>
@@ -485,9 +485,6 @@
     <t>$SearchTipeSaldo</t>
   </si>
   <si>
-    <t>IDR</t>
-  </si>
-  <si>
     <t>$SearchTipeTransaksi</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>Unexecited</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
   <si>
     <t>Eksekusi berhasil, karena KK valid 
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>Object Repository/ImageFolder/STNK/STNKberbayang.png</t>
+  </si>
+  <si>
+    <t>IDR</t>
   </si>
 </sst>
 </file>
@@ -678,10 +681,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -706,6 +709,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -713,7 +723,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -735,19 +768,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -761,45 +831,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -812,38 +844,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,19 +867,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,13 +891,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,31 +921,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -942,43 +933,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,13 +969,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,7 +981,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,25 +1005,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,6 +1076,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1084,24 +1096,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1139,8 +1133,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1162,6 +1156,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1172,224 +1175,224 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="10" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="11" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="26" fontId="17" numFmtId="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="7" fontId="18" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="7" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="16" numFmtId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="20" numFmtId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="21" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="12" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
-    <cellStyle builtinId="10" name="Note" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1403,10 +1406,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1570,21 +1573,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1601,7 +1604,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1654,9 +1657,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
@@ -1664,11 +1667,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
+    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1710,7 +1713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:7">
+    <row r="3" ht="43.5" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1738,31 +1741,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:1">
+    <row r="12" s="1" customFormat="1" spans="1:1">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:1">
+    <row r="17" s="1" customFormat="1" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1996,19 +1999,19 @@
       <c r="C21" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C14:D14 F14:G14"/>
+    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -2016,10 +2019,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2047,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:5">
+    <row r="3" ht="29" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -2269,18 +2272,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C16"/>
+    <ignoredError sqref="C16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -2288,16 +2291,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
+    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2329,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:9">
+    <row r="2" ht="29" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:9">
+    <row r="3" ht="29" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2392,39 +2395,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="3" t="s">
         <v>111</v>
       </c>
@@ -2781,7 +2784,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -2792,15 +2795,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -2808,16 +2811,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2875,7 +2878,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:11">
+    <row r="3" ht="43.5" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2915,35 +2918,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>119</v>
       </c>
@@ -3008,30 +3011,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:J12"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
-    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3074,7 +3077,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:10">
+    <row r="3" ht="29" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3111,43 +3114,43 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -3189,68 +3192,68 @@
         <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3282,7 +3285,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3312,14 +3315,14 @@
         <v>26</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:1">
+    <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3351,62 +3354,62 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
         <v>156</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>160</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>161</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>164</v>
       </c>
-      <c r="J15" t="s">
-        <v>165</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3414,34 +3417,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
@@ -3461,10 +3464,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row ht="29" r="3" spans="1:15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3572,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -3632,95 +3635,95 @@
         <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="L9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="M9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="N9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="O9" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3767,7 +3770,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3812,14 +3815,14 @@
         <v>26</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:1">
+    <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3866,79 +3869,79 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
         <v>156</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>160</v>
-      </c>
-      <c r="F15" t="s">
-        <v>161</v>
       </c>
       <c r="G15" t="s">
         <v>193</v>
       </c>
       <c r="H15" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15" t="s">
         <v>162</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>163</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>164</v>
       </c>
-      <c r="K15" t="s">
-        <v>165</v>
-      </c>
       <c r="L15" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" t="s">
         <v>157</v>
       </c>
-      <c r="M15" t="s">
-        <v>158</v>
-      </c>
       <c r="N15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="A11:O12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
-    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="37.1818181818182" customWidth="1"/>
+    <col min="3" max="3" width="42.0909090909091" customWidth="1"/>
+    <col min="4" max="4" width="41.6363636363636" customWidth="1"/>
+    <col min="5" max="5" width="37.5454545454545" customWidth="1"/>
+    <col min="6" max="6" width="37.6363636363636" customWidth="1"/>
+    <col min="7" max="7" width="36.3636363636364" customWidth="1"/>
+    <col min="8" max="8" width="37.4545454545455" customWidth="1"/>
+    <col min="9" max="9" width="38.4545454545455" customWidth="1"/>
+    <col min="10" max="13" width="39.1818181818182" customWidth="1"/>
+    <col min="14" max="15" width="40.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4063,35 +4066,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -4115,12 +4118,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row ht="43.5" r="8" spans="1:15">
+    <row r="8" ht="43.5" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
@@ -4172,98 +4175,98 @@
         <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="L9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="M9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="N9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="O9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -4310,7 +4313,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -4355,14 +4358,14 @@
         <v>26</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:1">
+    <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -4409,61 +4412,61 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
         <v>156</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>160</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>161</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>164</v>
-      </c>
-      <c r="J15" t="s">
-        <v>165</v>
       </c>
       <c r="K15" t="s">
         <v>193</v>
       </c>
       <c r="L15" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" t="s">
         <v>157</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>158</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>159</v>
       </c>
-      <c r="O15" t="s">
-        <v>160</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -4471,16 +4474,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5454545454545" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4520,7 +4523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:10">
+    <row r="3" ht="29" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4561,39 +4564,39 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -4611,73 +4614,73 @@
         <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row customFormat="1" r="13" s="1" spans="1:1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -4709,38 +4712,38 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
         <v>156</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>160</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>161</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>164</v>
       </c>
-      <c r="J15" t="s">
-        <v>165</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
APIAAS Basic Feature + TC OCR KTP KK STNK (Path on progress)
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="252">
   <si>
     <t>Status</t>
   </si>
@@ -426,6 +426,12 @@
     <t>Delete File ?(Yes/No)</t>
   </si>
   <si>
+    <t>;null</t>
+  </si>
+  <si>
+    <t>;Invalid API key or tenant code</t>
+  </si>
+  <si>
     <t>Eksekusi berhasil, karena KTP valid 
 dan parameter terpenuhi</t>
   </si>
@@ -449,6 +455,9 @@
     <t>KTP sangat blur, FAILED</t>
   </si>
   <si>
+    <t>Insufficient Balance</t>
+  </si>
+  <si>
     <t>OCR Parameter</t>
   </si>
   <si>
@@ -531,6 +540,48 @@
   </si>
   <si>
     <t>hxycaczn-ybfe-mmd9-9b5d-pwj6kibgacny</t>
+  </si>
+  <si>
+    <t>ParameterOptional</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>loginId</t>
+  </si>
+  <si>
+    <t>MALVIN</t>
+  </si>
+  <si>
+    <t>referenceNumber</t>
+  </si>
+  <si>
+    <t>REF00001</t>
+  </si>
+  <si>
+    <t>officeCode</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>officeName</t>
+  </si>
+  <si>
+    <t>HEAD_OFFICE</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>Registrasi User Pertama</t>
+  </si>
+  <si>
+    <t>Source(MOBILE/WEB)</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
   </si>
   <si>
     <t>Unexecited</t>
@@ -622,13 +673,73 @@
     <t>hxycaczn-ybfe-mmd9-9b5d-pwj7kibgacny</t>
   </si>
   <si>
+    <t>Parameter Optional</t>
+  </si>
+  <si>
+    <t>custNo</t>
+  </si>
+  <si>
+    <t>refocrKK</t>
+  </si>
+  <si>
+    <t>TL Check</t>
+  </si>
+  <si>
+    <t>;Image is too dark; Image is out of focus/blurry;  Image is noisy; Image is unreadable;</t>
+  </si>
+  <si>
+    <t>;Image is too dark;   Image is noisy; Image is unreadable;</t>
+  </si>
+  <si>
     <t>;Unexpected Error</t>
   </si>
   <si>
-    <t>;Image is too dark; Image is out of focus/blurry;  Image is noisy; Image is unreadable;</t>
-  </si>
-  <si>
-    <t>;Invalid API key or tenant code</t>
+    <t>;Image is unreadable;</t>
+  </si>
+  <si>
+    <t>;Image is noisy; Image is unreadable;</t>
+  </si>
+  <si>
+    <t>Invalid API Key or Tenant Code</t>
+  </si>
+  <si>
+    <t>Sukses, foto STNK memenuhi requirement</t>
+  </si>
+  <si>
+    <t>STNK terlipat lipat dan tidak terbaca, error/failed</t>
+  </si>
+  <si>
+    <t>Blurry yang tidak terlalu parah, maka error atau failed</t>
+  </si>
+  <si>
+    <t>Blur parah, error atau failed</t>
+  </si>
+  <si>
+    <t>Banyak STNK dalam foto, server bingung dan error</t>
+  </si>
+  <si>
+    <t>Foto lumayan jelas, tapi ada yang terpotong, 50% kemungkinan success</t>
+  </si>
+  <si>
+    <t>STNK yang difoto tidak bolak balik, error</t>
+  </si>
+  <si>
+    <t>Resolusi diatas maksimal kapabilitas server, Error atau null</t>
+  </si>
+  <si>
+    <t>Resolusi dibawah minimum requirement, Error</t>
+  </si>
+  <si>
+    <t>50% kemungkinan terbaca, karena ada bagian yang terpotong dan blurry, tapi bagian tengah terbaca</t>
+  </si>
+  <si>
+    <t>Error, karena gambar buram, resolusi kecil, dan banyak tulisan yang di sensor</t>
+  </si>
+  <si>
+    <t>Gambar punya 50% kemungkinan sukses, karena resolusi kecil tapi tulisan yang di bold</t>
+  </si>
+  <si>
+    <t>Invalid API Key karena key salah</t>
   </si>
   <si>
     <t>Object Repository/ImageFolder/STNK/STNKWorks1.jpg</t>
@@ -674,6 +785,15 @@
   </si>
   <si>
     <t>IDR</t>
+  </si>
+  <si>
+    <t>$halaman1</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB</t>
+  </si>
+  <si>
+    <t>$halaman2</t>
   </si>
 </sst>
 </file>
@@ -681,10 +801,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -723,37 +843,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -768,23 +857,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,10 +881,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -829,16 +928,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -847,6 +952,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -867,7 +987,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,19 +1077,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,7 +1113,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,7 +1137,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,91 +1155,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1023,31 +1167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,23 +1199,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1111,6 +1231,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1140,25 +1269,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1176,13 +1296,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1194,134 +1314,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1329,6 +1449,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1865,92 +1989,92 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="10">
         <v>999999</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="9">
         <v>1</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="9">
         <v>2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="9">
         <v>2</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1960,22 +2084,22 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="B18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
@@ -1983,8 +2107,8 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
@@ -1995,8 +2119,8 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2190,16 +2314,16 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2224,16 +2348,16 @@
       <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="7">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="7">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="7">
         <v>123456788012</v>
       </c>
     </row>
@@ -2258,16 +2382,16 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="8" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3023,21 +3147,22 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:J9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="3" width="45.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="52.8181818181818" customWidth="1"/>
+    <col min="5" max="10" width="49.1818181818182" customWidth="1"/>
+    <col min="11" max="11" width="51.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3045,19 +3170,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>44</v>
@@ -3068,57 +3193,78 @@
       <c r="J1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" ht="29" spans="1:10">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>138</v>
+      </c>
+      <c r="K3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f>COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
@@ -3149,47 +3295,54 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="K4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>150</v>
+      </c>
+      <c r="K8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>128</v>
@@ -3218,42 +3371,48 @@
       <c r="J9" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>153</v>
+      </c>
+      <c r="K10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3282,10 +3441,13 @@
       <c r="J11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3312,17 +3474,20 @@
         <v>26</v>
       </c>
       <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3351,37 +3516,104 @@
       <c r="J14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F15" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G15" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I15" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J15" t="s">
-        <v>164</v>
+        <v>167</v>
+      </c>
+      <c r="K15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3393,23 +3625,23 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:O9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="A17:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="43.3636363636364" customWidth="1"/>
+    <col min="3" max="5" width="45.1818181818182" customWidth="1"/>
+    <col min="6" max="6" width="49.8181818181818" customWidth="1"/>
+    <col min="7" max="10" width="45.1818181818182" customWidth="1"/>
+    <col min="11" max="11" width="42.3636363636364" customWidth="1"/>
+    <col min="12" max="12" width="48.9090909090909" customWidth="1"/>
+    <col min="13" max="13" width="46.4545454545455" customWidth="1"/>
+    <col min="14" max="15" width="49.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3420,31 +3652,31 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="H1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="J1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="K1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
@@ -3464,7 +3696,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="29" spans="1:15">
@@ -3472,46 +3704,46 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3577,59 +3809,59 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="G8" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="H8" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="I8" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="K8" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="L8" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="M8" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="N8" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="O8" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>124</v>
@@ -3676,54 +3908,54 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="M10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="N10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3770,7 +4002,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3817,12 +4049,12 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3869,49 +4101,110 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" t="s">
+        <v>210</v>
+      </c>
+      <c r="H15" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J15" t="s">
+        <v>166</v>
+      </c>
+      <c r="K15" t="s">
+        <v>167</v>
+      </c>
+      <c r="L15" t="s">
         <v>159</v>
       </c>
-      <c r="F15" t="s">
+      <c r="M15" t="s">
         <v>160</v>
       </c>
-      <c r="G15" t="s">
-        <v>193</v>
-      </c>
-      <c r="H15" t="s">
-        <v>161</v>
-      </c>
-      <c r="I15" t="s">
-        <v>162</v>
-      </c>
-      <c r="J15" t="s">
-        <v>163</v>
-      </c>
-      <c r="K15" t="s">
-        <v>164</v>
-      </c>
-      <c r="L15" t="s">
-        <v>156</v>
-      </c>
-      <c r="M15" t="s">
-        <v>157</v>
-      </c>
       <c r="N15" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3923,10 +4216,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:O9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3955,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -3999,63 +4292,91 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="G2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="H2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="J2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="K2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="L2" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="M2" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="N2" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="O2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" ht="43.5" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
@@ -4120,153 +4441,153 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" ht="43.5" spans="1:15">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>204</v>
+        <v>241</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>206</v>
+        <v>243</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>208</v>
+        <v>245</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>209</v>
+        <v>246</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>210</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="G9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="H9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="I9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="J9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="K9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="L9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="M9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="N9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="O9" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="M10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="N10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -4313,7 +4634,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -4360,12 +4681,12 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -4383,78 +4704,139 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" t="s">
         <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+      <c r="J15" t="s">
+        <v>167</v>
+      </c>
+      <c r="K15" t="s">
+        <v>210</v>
+      </c>
+      <c r="L15" t="s">
         <v>159</v>
       </c>
-      <c r="F15" t="s">
+      <c r="M15" t="s">
         <v>160</v>
       </c>
-      <c r="G15" t="s">
+      <c r="N15" t="s">
         <v>161</v>
       </c>
-      <c r="H15" t="s">
+      <c r="O15" t="s">
         <v>162</v>
       </c>
-      <c r="I15" t="s">
-        <v>163</v>
-      </c>
-      <c r="J15" t="s">
-        <v>164</v>
-      </c>
-      <c r="K15" t="s">
-        <v>193</v>
-      </c>
-      <c r="L15" t="s">
-        <v>156</v>
-      </c>
-      <c r="M15" t="s">
-        <v>157</v>
-      </c>
-      <c r="N15" t="s">
-        <v>158</v>
-      </c>
-      <c r="O15" t="s">
-        <v>159</v>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:1">
+      <c r="A16" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4466,24 +4848,24 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="49.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
+    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
+    <col min="10" max="10" width="35.7272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4528,31 +4910,31 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4560,186 +4942,306 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f>COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f>COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
-        <v>1</v>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$21,"*$*",C8:C21,"")</f>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>249</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H8" t="s">
+        <v>250</v>
+      </c>
+      <c r="I8" t="s">
+        <v>250</v>
+      </c>
+      <c r="J8" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>251</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="G9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="H9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="I9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="J9" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="J10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>154</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>158</v>
       </c>
-      <c r="E15" t="s">
+      <c r="B16" t="s">
         <v>159</v>
       </c>
-      <c r="F15" t="s">
+      <c r="C16" t="s">
         <v>160</v>
       </c>
-      <c r="G15" t="s">
+      <c r="D16" t="s">
         <v>161</v>
       </c>
-      <c r="H15" t="s">
+      <c r="E16" t="s">
         <v>162</v>
       </c>
-      <c r="I15" t="s">
+      <c r="F16" t="s">
         <v>163</v>
       </c>
-      <c r="J15" t="s">
+      <c r="G16" t="s">
         <v>164</v>
+      </c>
+      <c r="H16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J16" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
APIAAS Basic Feature + TC OCR KTP KK STNK NPWP BPKB Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="2" activeTab="6"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
     <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
     <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
+    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="322">
   <si>
     <t>Status</t>
   </si>
@@ -446,6 +447,9 @@
     <t>Ukuran resolusi KTP terlalu besar melebihi 1920x1080, failed</t>
   </si>
   <si>
+    <t>Penggunaan Key salah, error atau failed</t>
+  </si>
+  <si>
     <t>Ukuran resolusi KTP terlalu kecil kurang dari 960x720, failed</t>
   </si>
   <si>
@@ -551,7 +555,7 @@
     <t>loginId</t>
   </si>
   <si>
-    <t>MALVIN</t>
+    <t>Q</t>
   </si>
   <si>
     <t>referenceNumber</t>
@@ -628,6 +632,9 @@
     <t>Eksekusi gagal, karena resolusi terlalu rendah</t>
   </si>
   <si>
+    <t>Penggunaan key yang salah, error atau failed</t>
+  </si>
+  <si>
     <t>Object Repository/ImageFolder/KK/KKWorks1.jpg</t>
   </si>
   <si>
@@ -787,13 +794,217 @@
     <t>IDR</t>
   </si>
   <si>
+    <t>;Failed to extract data from BPKB Hal 2</t>
+  </si>
+  <si>
+    <t>;BPKB Hal 2 or 3 not found</t>
+  </si>
+  <si>
+    <t>;BPKB Hal 2 : Image resolution is below 480 x 360 or above 2560 x 1920 (Document Only).</t>
+  </si>
+  <si>
+    <t>;BPKB Hal 2 or 3 not found;BPKB Hal 2 or 3 not found</t>
+  </si>
+  <si>
+    <t>Success, karena bpkb halaman 2 dan 3 sesuai requirement</t>
+  </si>
+  <si>
+    <t>Gagal karena tingkat blur yang mengganggu proses OCR</t>
+  </si>
+  <si>
+    <t>Gagal, karena pada foto halaman2 terdapat STNK di dalamnya</t>
+  </si>
+  <si>
+    <t>Gagal, karena bpkb dalam foto ada dua</t>
+  </si>
+  <si>
+    <t>50% kemungkinan berhasil karena versi lama mungkin cocok dengan OCR terkini</t>
+  </si>
+  <si>
+    <t>50% berhasil karena foto terlalu silau terkena flash</t>
+  </si>
+  <si>
+    <t>Gagal karena salah satu halaman memilki resolusi sangat tinggi</t>
+  </si>
+  <si>
+    <t>Gagal, API Key salah</t>
+  </si>
+  <si>
+    <t>Gagal karena salah satu halaman memiliki resolusi terlalu rendah</t>
+  </si>
+  <si>
+    <t>Dengan dikirim 1 parameter saja seharusnya success</t>
+  </si>
+  <si>
+    <t>Dengan dikirim parameter halaman 3 saja, maka kemungkinan bisa success</t>
+  </si>
+  <si>
     <t>$halaman1</t>
   </si>
   <si>
-    <t>Object Repository/ImageFolder/BPKB</t>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_cahayaMinim.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_blurlevel2.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_blurlevel1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_campurSTNK.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_double.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_old.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_old2.png</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_overexposure.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_restoohigh.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal2/BPKB_restoolow.png</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_works.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/decoy.txt</t>
   </si>
   <si>
     <t>$halaman2</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_blurlevel1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_blurlevel2.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_meetrequirement.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_oldVersion.png</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_shouldworks.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/BPKB/Hal3/BPKB_agak buram.jpg</t>
+  </si>
+  <si>
+    <t>Customer No.</t>
+  </si>
+  <si>
+    <t>OfficeCode</t>
+  </si>
+  <si>
+    <t>OfficeName</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>BPKB Hal 2 dan 3 (9)</t>
+  </si>
+  <si>
+    <t>LoginID</t>
+  </si>
+  <si>
+    <t>refNumber</t>
+  </si>
+  <si>
+    <t>MAL-001</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Sukses, NPWP memenuhi kriteria</t>
+  </si>
+  <si>
+    <t>Sukses, tampilan NPWP yang baru</t>
+  </si>
+  <si>
+    <t>Kemungkinan 50% berhasil gambar sedikit blur</t>
+  </si>
+  <si>
+    <t>Gagal, karena tingkat blur sangat parah</t>
+  </si>
+  <si>
+    <t>Kemungkinan 50% berhasil, gambar agak gelap</t>
+  </si>
+  <si>
+    <t>Kemungkinan 50% berhasil, gambar diambil dari monitor</t>
+  </si>
+  <si>
+    <t>Gagal, resolusi terlalu tinggi</t>
+  </si>
+  <si>
+    <t>Gagal, resolusi terlalu rendah</t>
+  </si>
+  <si>
+    <t>Kemungkinan 50%, gambar agak noisy</t>
+  </si>
+  <si>
+    <t>Sukses, sesuai kriteria</t>
+  </si>
+  <si>
+    <t>Kemungkinan 50% sukses, karena hanya sedikit terpotong di fotonya</t>
+  </si>
+  <si>
+    <t>Gagal, key yang digunakan salah</t>
+  </si>
+  <si>
+    <t>Mungkin gagal, karena gambar sangat grainy</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_belakang.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_blurlevel1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_blurlevel2.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_dark.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_monitor.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_restoohigh.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_restoolow.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP1.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP2.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_kepotong.jpg</t>
+  </si>
+  <si>
+    <t>Object Repository/ImageFolder/NPWP/NPWP_amatir.jpg</t>
+  </si>
+  <si>
+    <t>REF0001</t>
+  </si>
+  <si>
+    <t>check response header</t>
   </si>
 </sst>
 </file>
@@ -801,8 +1012,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -829,7 +1040,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -837,6 +1048,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,17 +1083,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -929,29 +1155,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,6 +1171,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -987,13 +1198,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,25 +1234,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1047,7 +1258,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,115 +1378,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,6 +1403,32 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1244,21 +1481,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1282,27 +1504,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1314,145 +1525,142 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1785,8 +1993,8 @@
   <sheetPr/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1825,8 +2033,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -1847,16 +2055,16 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1889,8 +2097,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1983,123 +2191,123 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
-      <c r="A12" s="3" t="s">
+    <row r="12" s="2" customFormat="1" spans="1:1">
+      <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>999999</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>2</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>2</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>2</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
-      <c r="A17" s="3" t="s">
+    <row r="17" s="2" customFormat="1" spans="1:1">
+      <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="B18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
@@ -2107,8 +2315,8 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
@@ -2119,15 +2327,15 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
+    <ignoredError sqref="C14:D14 F14:G14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2184,10 +2392,10 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2212,8 +2420,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2314,16 +2522,16 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2348,16 +2556,16 @@
       <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>123456788012</v>
       </c>
     </row>
@@ -2382,16 +2590,16 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2463,7 +2671,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D2" t="s">
@@ -2492,25 +2700,25 @@
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2551,8 +2759,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2785,8 +2993,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
-      <c r="A16" s="3" t="s">
+    <row r="16" s="2" customFormat="1" spans="1:1">
+      <c r="A16" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2878,7 +3086,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B20" t="s">
@@ -3006,32 +3214,32 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -3070,8 +3278,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3149,17 +3357,17 @@
   <sheetPr/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1"/>
-    <col min="11" max="11" width="51.5454545454545" customWidth="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="51.5454545454545" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3224,35 +3432,35 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>138</v>
       </c>
+      <c r="J3" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="K3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3300,49 +3508,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>140</v>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="4" t="s">
-        <v>141</v>
+      <c r="A8" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>128</v>
@@ -3377,42 +3585,42 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3447,7 +3655,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3480,14 +3688,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="3" t="s">
-        <v>156</v>
+    <row r="13" s="2" customFormat="1" spans="1:1">
+      <c r="A13" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3508,13 +3716,13 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
         <v>34</v>
@@ -3522,47 +3730,47 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
-      <c r="A16" s="3" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:1">
+      <c r="A16" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>123</v>
@@ -3570,50 +3778,50 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3625,26 +3833,27 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="A17:B23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1"/>
-    <col min="7" max="10" width="45.1818181818182" customWidth="1"/>
-    <col min="11" max="11" width="42.3636363636364" customWidth="1"/>
-    <col min="12" max="12" width="48.9090909090909" customWidth="1"/>
-    <col min="13" max="13" width="46.4545454545455" customWidth="1"/>
-    <col min="14" max="15" width="49.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="46" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3652,31 +3861,31 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
@@ -3688,6 +3897,9 @@
         <v>44</v>
       </c>
       <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3696,57 +3908,60 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" ht="29" spans="1:15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:16">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="N3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3806,62 +4021,69 @@
         <f>COUNTIFS($A$8:$A$20,"*$*",O8:O20,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="4" t="s">
+      <c r="P4">
+        <f>COUNTIFS($A$8:$A$20,"*$*",P8:P20,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
         <v>141</v>
       </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="K8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M8" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="O8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>211</v>
+      </c>
+      <c r="P8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>124</v>
@@ -3905,57 +4127,63 @@
       <c r="O9" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>154</v>
+      </c>
+      <c r="P10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3999,10 +4227,13 @@
       <c r="O11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -4046,15 +4277,18 @@
       <c r="O12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:1">
+      <c r="A13" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -4072,88 +4306,94 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" t="s">
         <v>35</v>
       </c>
-      <c r="H14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" t="s">
-        <v>34</v>
-      </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+      <c r="J15" t="s">
+        <v>167</v>
+      </c>
+      <c r="K15" t="s">
+        <v>168</v>
+      </c>
+      <c r="L15" t="s">
         <v>160</v>
       </c>
-      <c r="D15" t="s">
+      <c r="M15" t="s">
         <v>161</v>
       </c>
-      <c r="E15" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" t="s">
-        <v>163</v>
-      </c>
-      <c r="G15" t="s">
-        <v>210</v>
-      </c>
-      <c r="H15" t="s">
-        <v>164</v>
-      </c>
-      <c r="I15" t="s">
-        <v>165</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="N15" t="s">
         <v>166</v>
       </c>
-      <c r="K15" t="s">
-        <v>167</v>
-      </c>
-      <c r="L15" t="s">
-        <v>159</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>160</v>
       </c>
-      <c r="N15" t="s">
-        <v>165</v>
-      </c>
-      <c r="O15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
-      <c r="A16" s="3" t="s">
-        <v>211</v>
+      <c r="P15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:1">
+      <c r="A16" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4161,50 +4401,50 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4218,23 +4458,23 @@
   <sheetPr/>
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="37.1818181818182" customWidth="1"/>
-    <col min="3" max="3" width="42.0909090909091" customWidth="1"/>
-    <col min="4" max="4" width="41.6363636363636" customWidth="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1"/>
-    <col min="9" max="9" width="38.4545454545455" customWidth="1"/>
-    <col min="10" max="13" width="39.1818181818182" customWidth="1"/>
-    <col min="14" max="15" width="40.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="38.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="40.2727272727273" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4292,16 +4532,16 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4319,63 +4559,63 @@
         <v>131</v>
       </c>
       <c r="L2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="N2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="O2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" ht="43.5" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="I3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>233</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -4439,155 +4679,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>140</v>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" ht="43.5" spans="1:15">
-      <c r="A8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="A8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="L8" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="M8" s="3" t="s">
         <v>247</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="J9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="K9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="L9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="M9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="O9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -4634,7 +4874,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -4679,14 +4919,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="3" t="s">
-        <v>156</v>
+    <row r="13" s="2" customFormat="1" spans="1:1">
+      <c r="A13" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -4733,59 +4973,59 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" t="s">
+        <v>168</v>
+      </c>
+      <c r="K15" t="s">
+        <v>212</v>
+      </c>
+      <c r="L15" t="s">
         <v>160</v>
       </c>
-      <c r="D15" t="s">
+      <c r="M15" t="s">
         <v>161</v>
       </c>
-      <c r="E15" t="s">
+      <c r="N15" t="s">
         <v>162</v>
       </c>
-      <c r="F15" t="s">
+      <c r="O15" t="s">
         <v>163</v>
       </c>
-      <c r="G15" t="s">
-        <v>164</v>
-      </c>
-      <c r="H15" t="s">
-        <v>165</v>
-      </c>
-      <c r="I15" t="s">
-        <v>166</v>
-      </c>
-      <c r="J15" t="s">
-        <v>167</v>
-      </c>
-      <c r="K15" t="s">
-        <v>210</v>
-      </c>
-      <c r="L15" t="s">
-        <v>159</v>
-      </c>
-      <c r="M15" t="s">
-        <v>160</v>
-      </c>
-      <c r="N15" t="s">
-        <v>161</v>
-      </c>
-      <c r="O15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
-      <c r="A16" s="6" t="s">
-        <v>211</v>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:1">
+      <c r="A16" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4793,50 +5033,50 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4848,32 +5088,679 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:I15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="49.5454545454545" customWidth="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="40.8181818181818" customWidth="1"/>
+    <col min="3" max="3" width="52.6363636363636" customWidth="1"/>
+    <col min="4" max="4" width="54.6363636363636" customWidth="1"/>
+    <col min="5" max="5" width="58" customWidth="1"/>
+    <col min="6" max="6" width="51.6363636363636" customWidth="1"/>
     <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
     <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
     <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
     <col min="10" max="10" width="35.7272727272727" customWidth="1"/>
+    <col min="11" max="11" width="31.6363636363636" customWidth="1"/>
+    <col min="12" max="14" width="39.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
+        <v>254</v>
+      </c>
+      <c r="M2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" ht="43.5" spans="1:14">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$21,"*$*",C8:C21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",K8:K21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",L8:L21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",M8:M21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",N8:N21,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" ht="43.5" spans="1:14">
+      <c r="A8" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" ht="43.5" spans="1:14">
+      <c r="A9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L11" t="s">
+        <v>154</v>
+      </c>
+      <c r="M11" t="s">
+        <v>154</v>
+      </c>
+      <c r="N11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:1">
+      <c r="A14" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" t="s">
+        <v>168</v>
+      </c>
+      <c r="K16" t="s">
+        <v>168</v>
+      </c>
+      <c r="L16" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" t="s">
+        <v>168</v>
+      </c>
+      <c r="N16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" spans="1:1">
+      <c r="A17" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>286</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>288</v>
+      </c>
+      <c r="B20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>289</v>
+      </c>
+      <c r="B21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="36.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="34.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="35.5454545454545" customWidth="1"/>
+    <col min="5" max="5" width="37.5454545454545" customWidth="1"/>
+    <col min="6" max="6" width="37.6363636363636" customWidth="1"/>
+    <col min="7" max="7" width="36.3636363636364" customWidth="1"/>
+    <col min="8" max="8" width="37.4545454545455" customWidth="1"/>
+    <col min="9" max="9" width="40.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="39.1818181818182" customWidth="1"/>
+    <col min="11" max="11" width="37.4545454545455" customWidth="1"/>
+    <col min="12" max="12" width="40.0909090909091" customWidth="1"/>
+    <col min="13" max="13" width="39.1818181818182" customWidth="1"/>
+    <col min="14" max="14" width="40.0909090909091" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -4899,45 +5786,72 @@
       <c r="J1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="29" spans="1:10">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:14">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="B3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -4946,78 +5860,107 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$21,"*$*",C8:C21,"")</f>
+        <f>COUNTIFS($A$8:$A$21,"*$*",C8:C21,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",D8:D21,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",G8:G21,"")</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",H8:H21,"")</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f>COUNTIFS($A$8:$A$21,"*$*",I8:I21,"")</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" t="s">
-        <v>250</v>
-      </c>
-      <c r="D8" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" t="s">
-        <v>250</v>
-      </c>
-      <c r="F8" t="s">
-        <v>250</v>
-      </c>
-      <c r="G8" t="s">
-        <v>250</v>
-      </c>
-      <c r="H8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I8" t="s">
-        <v>250</v>
-      </c>
-      <c r="J8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <f>COUNTIFS($A$8:$A$21,"*$*",J8:J21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",K8:K21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",L8:L21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",M8:M21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",N8:N21,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1"/>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" ht="58" spans="1:14">
+      <c r="A8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>250</v>
@@ -5046,202 +5989,303 @@
       <c r="J9" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="s">
+        <v>250</v>
+      </c>
+      <c r="L9" t="s">
+        <v>250</v>
+      </c>
+      <c r="M9" t="s">
+        <v>250</v>
+      </c>
+      <c r="N9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="G10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="I10" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="J10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>154</v>
+      </c>
+      <c r="K10" t="s">
+        <v>154</v>
+      </c>
+      <c r="L10" t="s">
+        <v>154</v>
+      </c>
+      <c r="M10" t="s">
+        <v>154</v>
+      </c>
+      <c r="N10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:1">
-      <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:14">
+      <c r="A12" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:1">
+      <c r="A13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:14">
+      <c r="A15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" t="s">
-        <v>162</v>
-      </c>
-      <c r="F16" t="s">
-        <v>163</v>
-      </c>
-      <c r="G16" t="s">
-        <v>164</v>
-      </c>
-      <c r="H16" t="s">
-        <v>165</v>
-      </c>
-      <c r="I16" t="s">
+        <v>168</v>
+      </c>
+      <c r="K15" t="s">
         <v>166</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L15" t="s">
         <v>167</v>
+      </c>
+      <c r="M15" t="s">
+        <v>168</v>
+      </c>
+      <c r="N15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:1">
+      <c r="A16" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balikan AT 46 Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="375">
   <si>
     <t>Status</t>
   </si>
@@ -1133,6 +1133,9 @@
   </si>
   <si>
     <t>Sukses karena rekening koran digital resmi</t>
+  </si>
+  <si>
+    <t>Gagal, tidak image untuk OCR</t>
   </si>
   <si>
     <t>ImageFolder/RKBCA/RKBCA1.pdf</t>
@@ -1171,9 +1174,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1197,9 +1200,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1213,7 +1215,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1227,17 +1229,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1245,36 +1238,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1288,14 +1252,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1311,8 +1291,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1320,22 +1301,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1356,7 +1359,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1368,19 +1401,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1392,7 +1431,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1404,19 +1473,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1428,7 +1491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1440,31 +1503,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,49 +1527,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1530,13 +1539,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1576,24 +1579,35 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1613,17 +1627,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1651,21 +1665,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1683,40 +1686,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1725,88 +1728,88 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2492,7 +2495,7 @@
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C14:D14 F14:G14" numberStoredAsText="1"/>
+    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2502,7 +2505,7 @@
   <sheetPr/>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -3099,10 +3102,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="$A24:$XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3117,9 +3120,10 @@
     <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
     <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
     <col min="10" max="12" width="35.7272727272727" customWidth="1"/>
+    <col min="13" max="13" width="35.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3154,6 +3158,9 @@
         <v>44</v>
       </c>
       <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3162,7 +3169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:12">
+    <row r="3" ht="29" spans="1:13">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3199,8 +3206,11 @@
       <c r="L3" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3247,6 +3257,10 @@
       <c r="L4">
         <f>COUNTIFS($A$8:$A$21,"*$*",L8:L21,"")</f>
         <v>0</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIFS($A$8:$A$21,"*$*",M8:M21,"")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
@@ -3254,83 +3268,87 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="L8" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>365</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="I9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="L9" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>374</v>
+      </c>
+      <c r="M9" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -3365,6 +3383,9 @@
         <v>155</v>
       </c>
       <c r="L10" t="s">
+        <v>155</v>
+      </c>
+      <c r="M10" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3373,7 +3394,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -3410,8 +3431,11 @@
       <c r="L12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -3448,8 +3472,11 @@
       <c r="L13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>160</v>
       </c>
@@ -3486,8 +3513,11 @@
       <c r="L14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>161</v>
       </c>
@@ -3522,6 +3552,9 @@
         <v>170</v>
       </c>
       <c r="L15" t="s">
+        <v>170</v>
+      </c>
+      <c r="M15" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Isi Saldo , Flag Excel Failed Done (AT49+AT50)
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,29 +4,29 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="4" activeTab="8"/>
+    <workbookView activeTab="12" firstSheet="8" windowHeight="7070" windowWidth="18530"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" sheetId="1" r:id="rId1"/>
-    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
-    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
-    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
-    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
-    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
-    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
-    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
-    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
-    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
-    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
-    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
-    <sheet name="APIAAS-Saldo" sheetId="13" r:id="rId13"/>
+    <sheet name="Register" r:id="rId1" sheetId="1"/>
+    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
+    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
+    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
+    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
+    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
+    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
+    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
+    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
+    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
+    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
+    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
+    <sheet name="APIAAS-Saldo" r:id="rId13" sheetId="13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="431">
   <si>
     <t>Status</t>
   </si>
@@ -1280,7 +1280,16 @@
     <t>1980-01-01</t>
   </si>
   <si>
-    <t>Success tambah saldo</t>
+    <t>Success tambah saldo IDR</t>
+  </si>
+  <si>
+    <t>Success tambah saldo OCR KTP</t>
+  </si>
+  <si>
+    <t>Success tambah saldo OCR KK</t>
+  </si>
+  <si>
+    <t>Gagal topup karena tipe saldo kosong</t>
   </si>
   <si>
     <t>$Username Billing</t>
@@ -1320,6 +1329,9 @@
   </si>
   <si>
     <t>2023-04-19</t>
+  </si>
+  <si>
+    <t>Filter Saldo</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1340,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1355,16 +1367,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1378,7 +1389,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1394,15 +1421,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1417,23 +1451,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1441,7 +1459,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1455,20 +1473,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -1477,8 +1481,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1514,7 +1526,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1526,7 +1538,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1538,7 +1598,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,7 +1646,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1562,61 +1676,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,37 +1688,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,31 +1700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1723,32 +1735,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1777,6 +1768,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1801,11 +1807,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1822,238 +1834,238 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="12" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="14" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="25" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="27" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="27" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="18">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
+    <cellStyle builtinId="10" name="Note" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2067,10 +2079,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2234,21 +2246,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2265,7 +2277,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2318,9 +2330,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -2328,11 +2340,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2374,7 +2386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:7">
+    <row ht="43.5" r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2402,31 +2414,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -2615,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -2660,19 +2672,19 @@
       <c r="C21" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -2680,20 +2692,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="47.9090909090909" customWidth="1"/>
-    <col min="4" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="34.2727272727273" customWidth="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1"/>
-    <col min="12" max="13" width="57.1818181818182" customWidth="1"/>
-    <col min="14" max="14" width="37.2727272727273" customWidth="1"/>
-    <col min="15" max="15" width="36.5454545454545" customWidth="1"/>
-    <col min="16" max="16" width="35.7272727272727" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.9090909090909" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="57.1818181818182" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="37.2727272727273" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2781,7 +2793,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:15">
+    <row ht="29" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2845,31 +2857,31 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
+        <f ref="E4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -2889,12 +2901,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:15">
+    <row ht="29" r="8" spans="1:15">
       <c r="A8" s="11" t="s">
         <v>144</v>
       </c>
@@ -3035,7 +3047,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -3228,7 +3240,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>231</v>
       </c>
@@ -3326,15 +3338,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3342,18 +3354,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="6" width="34.2727272727273" customWidth="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1"/>
-    <col min="11" max="13" width="35.7272727272727" customWidth="1"/>
-    <col min="14" max="14" width="35.3636363636364" customWidth="1"/>
-    <col min="15" max="15" width="34.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="35.3636363636364" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.6363636363636" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3408,7 +3420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:15">
+    <row ht="43.5" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3476,27 +3488,27 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
+        <f ref="F4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3516,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
@@ -3662,7 +3674,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -3855,7 +3867,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>231</v>
       </c>
@@ -3916,7 +3928,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="4" t="s">
         <v>189</v>
       </c>
@@ -3938,15 +3950,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
@@ -3954,20 +3966,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
-    <col min="10" max="10" width="75.9090909090909" customWidth="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1"/>
-    <col min="12" max="12" width="45.1818181818182" customWidth="1"/>
-    <col min="13" max="16" width="35.7272727272727" customWidth="1"/>
-    <col min="17" max="17" width="35.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="75.9090909090909" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="35.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -4028,7 +4040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:17">
+    <row ht="43.5" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4094,55 +4106,55 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:P4" si="0">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f ref="D4:P4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>4</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="Q4">
@@ -4150,12 +4162,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="11" t="s">
         <v>405</v>
       </c>
@@ -4361,7 +4373,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>160</v>
       </c>
@@ -4578,7 +4590,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="21" s="1" spans="1:1">
       <c r="A21" s="4" t="s">
         <v>175</v>
       </c>
@@ -4615,7 +4627,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="26" s="1" spans="1:1">
       <c r="A26" s="4" t="s">
         <v>189</v>
       </c>
@@ -4637,28 +4649,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B9" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="B9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="5" width="27" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7272727272727" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4678,7 +4690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4686,7 +4698,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4694,13 +4706,13 @@
         <v>413</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>414</v>
+      </c>
+      <c r="D3" t="s">
+        <v>415</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4713,54 +4725,54 @@
       </c>
       <c r="C4">
         <f>COUNTIFS($A$10:$A$22,"*$*",C10:C22,"")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f>COUNTIFS($A$10:$A$22,"*$*",D10:D22,"")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f>COUNTIFS($A$10:$A$22,"*$*",E10:E22,"")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" spans="1:5">
+    <row customFormat="1" r="8" s="2" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" s="2" customFormat="1" spans="1:5">
+        <v>418</v>
+      </c>
+    </row>
+    <row customFormat="1" r="9" s="2" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4797,85 +4809,176 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>422</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="6" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B15">
         <v>100</v>
       </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B16" s="7">
         <v>1111</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="7">
+        <v>1112</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1113</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B17" s="6" t="str">
         <f>CONCATENATE("Isiulang ",B14)</f>
         <v>Isiulang IDR</v>
       </c>
-    </row>
-    <row r="18" ht="29" spans="1:5">
+      <c r="C17" s="6" t="str">
+        <f>CONCATENATE("Isiulang ",C14)</f>
+        <v>Isiulang OCR KTP</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f>CONCATENATE("Isiulang ",D14)</f>
+        <v>Isiulang OCR KK</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f>CONCATENATE("Isiulang ",E14)</f>
+        <v>Isiulang </v>
+      </c>
+    </row>
+    <row ht="29" r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+        <v>429</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row customFormat="1" r="19" s="1" spans="1:1">
+      <c r="A19" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="10" t="str">
+        <f>B14</f>
+        <v>IDR</v>
+      </c>
+      <c r="C20" s="10" t="str">
+        <f>C14</f>
+        <v>OCR KTP</v>
+      </c>
+      <c r="D20" s="10" t="str">
+        <f>D14</f>
+        <v>OCR KK</v>
+      </c>
       <c r="E20" s="10"/>
     </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" t="str">
+        <f>CONCATENATE("Top Up ",B20)</f>
+        <v>Top Up IDR</v>
+      </c>
+      <c r="C21" t="str">
+        <f>CONCATENATE("Top Up ",C20)</f>
+        <v>Top Up OCR KTP</v>
+      </c>
+      <c r="D21" t="str">
+        <f>CONCATENATE("Top Up ",D20)</f>
+        <v>Top Up OCR KK</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:E18"/>
@@ -4883,10 +4986,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4914,7 +5017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4952,7 +5055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -5136,18 +5239,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C16" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -5155,16 +5258,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5196,7 +5299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="29" spans="1:9">
+    <row ht="29" r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5225,7 +5328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:9">
+    <row ht="29" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5259,39 +5362,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -5525,7 +5628,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>111</v>
       </c>
@@ -5648,7 +5751,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -5659,15 +5762,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -5675,16 +5778,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5742,7 +5845,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:11">
+    <row ht="43.5" r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5782,35 +5885,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>119</v>
       </c>
@@ -5875,19 +5978,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
@@ -5895,14 +5998,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1"/>
-    <col min="11" max="11" width="51.5454545454545" customWidth="1"/>
-    <col min="12" max="12" width="43.7272727272727" customWidth="1"/>
-    <col min="13" max="13" width="35.2727272727273" customWidth="1"/>
-    <col min="14" max="14" width="36.8181818181818" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="51.5454545454545" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="35.2727272727273" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="36.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5963,7 +6066,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:14">
+    <row ht="29" r="3" spans="1:14">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -6016,35 +6119,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -6064,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
@@ -6201,7 +6304,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -6382,7 +6485,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>175</v>
       </c>
@@ -6443,7 +6546,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="4" t="s">
         <v>189</v>
       </c>
@@ -6465,15 +6568,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
@@ -6481,21 +6584,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1"/>
-    <col min="7" max="10" width="45.1818181818182" customWidth="1"/>
-    <col min="11" max="11" width="42.3636363636364" customWidth="1"/>
-    <col min="12" max="12" width="48.9090909090909" customWidth="1"/>
-    <col min="13" max="13" width="46.4545454545455" customWidth="1"/>
-    <col min="14" max="15" width="49.2727272727273" customWidth="1"/>
-    <col min="16" max="16" width="46.8181818181818" customWidth="1"/>
-    <col min="17" max="17" width="51.4545454545455" customWidth="1"/>
-    <col min="18" max="18" width="53.3636363636364" customWidth="1"/>
-    <col min="19" max="19" width="34.8181818181818" customWidth="1"/>
-    <col min="20" max="20" width="31.4545454545455" customWidth="1"/>
-    <col min="21" max="21" width="29.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="46.8181818181818" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="51.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="53.3636363636364" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.8181818181818" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="31.4545454545455" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="29.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -6616,7 +6719,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:20">
+    <row ht="29" r="3" spans="1:20">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6683,67 +6786,67 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:Q4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:Q4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="R4">
@@ -6759,7 +6862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
@@ -6950,7 +7053,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -7203,7 +7306,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>231</v>
       </c>
@@ -7264,7 +7367,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="4" t="s">
         <v>189</v>
       </c>
@@ -7286,39 +7389,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="R1" activePane="topLeft"/>
+      <pane activePane="topLeft" topLeftCell="R1" xSplit="18280"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="37.1818181818182" customWidth="1"/>
-    <col min="3" max="3" width="42.0909090909091" customWidth="1"/>
-    <col min="4" max="4" width="41.6363636363636" customWidth="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1"/>
-    <col min="9" max="9" width="38.4545454545455" customWidth="1"/>
-    <col min="10" max="13" width="39.1818181818182" customWidth="1"/>
-    <col min="14" max="15" width="40.2727272727273" customWidth="1"/>
-    <col min="16" max="16" width="37.5454545454545" customWidth="1"/>
-    <col min="17" max="17" width="34.4545454545455" customWidth="1"/>
-    <col min="18" max="18" width="43.6363636363636" customWidth="1"/>
-    <col min="19" max="19" width="34.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="43.6363636363636" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -7436,7 +7539,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:19">
+    <row ht="43.5" r="3" spans="1:19">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7504,59 +7607,59 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -7572,12 +7675,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:19">
+    <row ht="29" r="8" spans="1:19">
       <c r="A8" s="11" t="s">
         <v>144</v>
       </c>
@@ -7754,7 +7857,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -7995,7 +8098,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>231</v>
       </c>
@@ -8056,7 +8159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="4" t="s">
         <v>189</v>
       </c>
@@ -8078,15 +8181,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -8094,20 +8197,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="40.8181818181818" customWidth="1"/>
-    <col min="3" max="3" width="52.6363636363636" customWidth="1"/>
-    <col min="4" max="4" width="54.6363636363636" customWidth="1"/>
-    <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="51.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
-    <col min="10" max="10" width="35.7272727272727" customWidth="1"/>
-    <col min="11" max="11" width="31.6363636363636" customWidth="1"/>
-    <col min="12" max="15" width="39.1818181818182" customWidth="1"/>
-    <col min="16" max="16" width="43" customWidth="1"/>
-    <col min="17" max="17" width="34.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="54.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.6363636363636" collapsed="true"/>
+    <col min="12" max="15" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -8210,7 +8313,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:17">
+    <row ht="43.5" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8276,55 +8379,55 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:J4" si="0">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
+        <f ref="D4:J4" si="0" t="shared">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -8332,12 +8435,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="11" t="s">
         <v>288</v>
       </c>
@@ -8390,7 +8493,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" ht="29" spans="1:17">
+    <row ht="29" r="9" spans="1:17">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -8549,7 +8652,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="4" t="s">
         <v>160</v>
       </c>
@@ -8766,7 +8869,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="4" t="s">
         <v>175</v>
       </c>
@@ -8827,7 +8930,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="25" s="1" spans="1:1">
       <c r="A25" s="4" t="s">
         <v>189</v>
       </c>
@@ -8849,41 +8952,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="T1" activePane="topLeft"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <pane activePane="topLeft" topLeftCell="T1" xSplit="18280"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="36.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="34.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="35.5454545454545" customWidth="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1"/>
-    <col min="9" max="9" width="40.0909090909091" customWidth="1"/>
-    <col min="10" max="10" width="39.1818181818182" customWidth="1"/>
-    <col min="11" max="11" width="37.4545454545455" customWidth="1"/>
-    <col min="12" max="12" width="40.0909090909091" customWidth="1"/>
-    <col min="13" max="13" width="39.1818181818182" customWidth="1"/>
-    <col min="14" max="15" width="40.0909090909091" customWidth="1"/>
-    <col min="16" max="16" width="43.7272727272727" customWidth="1"/>
-    <col min="17" max="17" width="34.5454545454545" customWidth="1"/>
-    <col min="18" max="18" width="30.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.2727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.5454545454545" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.5454545454545" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -8992,7 +9095,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:18">
+    <row ht="43.5" r="3" spans="1:18">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9053,59 +9156,59 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:O4" si="0">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <f ref="B4:O4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -9121,12 +9224,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:18">
+    <row ht="29" r="8" spans="1:18">
       <c r="A8" s="11" t="s">
         <v>144</v>
       </c>
@@ -9294,7 +9397,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -9523,7 +9626,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>231</v>
       </c>
@@ -9584,7 +9687,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="4" t="s">
         <v>189</v>
       </c>
@@ -9606,7 +9709,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AT49 Isi Saldo + AT73 Saldo
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="12"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
     <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
     <sheet name="Tenant" sheetId="14" r:id="rId14"/>
-    <sheet name="APIAAS-Saldo" sheetId="15" r:id="rId15"/>
+    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
     <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="560">
   <si>
     <t>Status</t>
   </si>
@@ -1220,9 +1220,6 @@
     <t>OCR Rek. Koran BCA</t>
   </si>
   <si>
-    <t>;Insufficient balance</t>
-  </si>
-  <si>
     <t>Success, karena bpkb halaman 2 dan 3 sesuai requirement</t>
   </si>
   <si>
@@ -1286,6 +1283,12 @@
     <t>1980-01-01</t>
   </si>
   <si>
+    <t>;Done well</t>
+  </si>
+  <si>
+    <t>;Topup terjadi failure</t>
+  </si>
+  <si>
     <t>Success tambah saldo IDR</t>
   </si>
   <si>
@@ -1355,12 +1358,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>-;Mandatory is incomplete</t>
-  </si>
-  <si>
-    <t>-;Fungsi pencarian gagal, no result</t>
-  </si>
-  <si>
     <t>Success create tenant</t>
   </si>
   <si>
@@ -1445,7 +1442,7 @@
     <t>API Key</t>
   </si>
   <si>
-    <t>ox7BrO</t>
+    <t>pnDRcU</t>
   </si>
   <si>
     <t>EfXHMQ</t>
@@ -1661,18 +1658,33 @@
     <t>Verifikasi Identitas Dukcapil</t>
   </si>
   <si>
+    <t>;Fungsi pencarian gagal, no result</t>
+  </si>
+  <si>
+    <t>Success search with all criteria and all function active</t>
+  </si>
+  <si>
+    <t>Success search dengan field pengguna dan nama dokumen tidak terisi</t>
+  </si>
+  <si>
+    <t>Success search dengan mengisi field mandatory saja</t>
+  </si>
+  <si>
     <t>Tipe Transaksi</t>
   </si>
   <si>
     <t>Tanggal Transaksi Dari</t>
   </si>
   <si>
-    <t>2023-04-28</t>
+    <t>2023-05-01</t>
   </si>
   <si>
     <t>Pengguna</t>
   </si>
   <si>
+    <t>ADMIN ESIGN</t>
+  </si>
+  <si>
     <t>Hasil Proses</t>
   </si>
   <si>
@@ -1685,6 +1697,9 @@
     <t>Tanggal Transaksi hingga</t>
   </si>
   <si>
+    <t>2023-05-03</t>
+  </si>
+  <si>
     <t>Kantor</t>
   </si>
   <si>
@@ -1694,16 +1709,16 @@
     <t>Username</t>
   </si>
   <si>
+    <t>Success verifikasi</t>
+  </si>
+  <si>
+    <t>Data Login</t>
+  </si>
+  <si>
     <t>USERA@GMAIL.COM</t>
   </si>
   <si>
     <t>P@ssw0rd123</t>
-  </si>
-  <si>
-    <t>Success verifikasi</t>
-  </si>
-  <si>
-    <t>Data Login</t>
   </si>
   <si>
     <t>PT A</t>
@@ -1714,11 +1729,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1750,8 +1765,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1764,9 +1788,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1787,16 +1810,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1827,38 +1857,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1871,8 +1871,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1886,9 +1895,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1909,19 +1924,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1933,25 +1942,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1963,37 +1966,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2005,25 +1978,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2041,7 +2002,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2053,7 +2020,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2065,31 +2080,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2176,16 +2191,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2195,6 +2219,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2214,30 +2247,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2253,11 +2262,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2275,13 +2290,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2293,137 +2308,143 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2456,9 +2477,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2837,8 +2855,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -2859,16 +2877,16 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3001,92 +3019,92 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="29">
         <v>999999</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28" t="s">
+      <c r="E14" s="29"/>
+      <c r="F14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="6">
         <v>2</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="6">
         <v>2</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3096,22 +3114,22 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
@@ -3119,8 +3137,8 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
@@ -3131,15 +3149,15 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
+    <ignoredError sqref="C14:D14 F14:G14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3260,46 +3278,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3370,49 +3388,49 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3887,46 +3905,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3997,49 +4015,49 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4423,26 +4441,26 @@
   <sheetPr/>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="75.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="35.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
+    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
+    <col min="10" max="10" width="75.9090909090909" customWidth="1"/>
+    <col min="11" max="11" width="35.7272727272727" customWidth="1"/>
+    <col min="12" max="12" width="45.1818181818182" customWidth="1"/>
+    <col min="13" max="16" width="35.7272727272727" customWidth="1"/>
+    <col min="17" max="17" width="35.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -4450,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -4498,64 +4516,61 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="3" ht="43.5" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>394</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="P3" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4634,102 +4649,102 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:17">
-      <c r="A8" s="24" t="s">
-        <v>406</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
+        <v>406</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>407</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>409</v>
-      </c>
-      <c r="B10" s="26">
+        <v>408</v>
+      </c>
+      <c r="B10" s="27">
         <v>7183259386136510</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>409</v>
+      </c>
+      <c r="B11" t="s">
         <v>410</v>
-      </c>
-      <c r="B11" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>411</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>412</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -5127,15 +5142,15 @@
   <sheetPr/>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="B1:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="5" width="27" customWidth="1"/>
+    <col min="1" max="1" width="18.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="27" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5143,10 +5158,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>44</v>
@@ -5155,9 +5170,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="3" ht="29" spans="1:5">
@@ -5165,16 +5186,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
-        <v>416</v>
-      </c>
-      <c r="E3" s="21" t="s">
         <v>417</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5205,36 +5226,36 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5242,16 +5263,16 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5259,38 +5280,38 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -5307,7 +5328,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B14" t="s">
         <v>269</v>
@@ -5321,7 +5342,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -5338,24 +5359,24 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>429</v>
-      </c>
-      <c r="B16" s="22">
-        <v>1113</v>
-      </c>
-      <c r="C16" s="22">
-        <v>1115</v>
-      </c>
-      <c r="D16" s="22">
+        <v>430</v>
+      </c>
+      <c r="B16" s="23">
+        <v>1130</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1131</v>
+      </c>
+      <c r="D16" s="23">
         <v>1121</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="23">
         <v>1116</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B17" t="str">
         <f>CONCATENATE("Isiulang ",B14)</f>
@@ -5375,44 +5396,44 @@
       </c>
     </row>
     <row r="18" ht="29" spans="1:5">
-      <c r="A18" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>433</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="23" t="str">
+      <c r="B20" s="24" t="str">
         <f>B14</f>
         <v>IDR</v>
       </c>
-      <c r="C20" s="23" t="str">
+      <c r="C20" s="24" t="str">
         <f>C14</f>
         <v>OCR BPKB</v>
       </c>
-      <c r="D20" s="23" t="str">
+      <c r="D20" s="24" t="str">
         <f>D14</f>
         <v>OCR STNK</v>
       </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
@@ -5441,726 +5462,726 @@
   <sheetPr/>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="30.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="32.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.1818181818182" customWidth="1"/>
+    <col min="2" max="2" width="42.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="21.8181818181818" customWidth="1"/>
+    <col min="4" max="5" width="32.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="36.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="26.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
+      <c r="C1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="G3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="6">
         <f>IF(C7="New",COUNTIFS($A$12:$A$23,"*$*",C12:C23,""),IF(C7="Service",COUNTIFS($A$9:$A$10,"*$*",C9:C10,""),IF(C7="Edit",COUNTIFS($A$9:$A$21,"*$*",C9:C21,""),0)))</f>
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <f>IF(D7="New",COUNTIFS($A$12:$A$23,"*$*",D12:D23,""),IF(D7="Service",COUNTIFS($A$9:$A$10,"*$*",D9:D10,""),IF(D7="Edit",COUNTIFS($A$9:$A$21,"*$*",D9:D21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
         <f>IF(E7="New",COUNTIFS($A$12:$A$23,"*$*",E12:E23,""),IF(E7="Service",COUNTIFS($A$9:$A$10,"*$*",E9:E10,""),IF(E7="Edit",COUNTIFS($A$9:$A$21,"*$*",E9:E21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <f>IF(F7="New",COUNTIFS($A$12:$A$23,"*$*",F12:F23,""),IF(F7="Service",COUNTIFS($A$9:$A$10,"*$*",F9:F10,""),IF(F7="Edit",COUNTIFS($A$9:$A$21,"*$*",F9:F21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="6">
         <f>IF(G7="New",COUNTIFS($A$12:$A$23,"*$*",G12:G23,""),IF(G7="Service",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),IF(G7="Edit",COUNTIFS($A$9:$A$21,"*$*",G9:G21,""),IF(G7="ChargeType",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),0))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="G7" s="4" t="s">
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:7">
+      <c r="A8" s="7" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:7">
+      <c r="A11" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:7">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="10">
+        <v>202304426</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>463</v>
       </c>
-      <c r="B14" s="8">
-        <v>202304426</v>
-      </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10">
+        <v>202304277</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8">
-        <v>202304277</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="B15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="7" t="s">
+      <c r="B16" t="s">
         <v>466</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" t="s">
         <v>467</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" t="s">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="1:7">
+      <c r="A17" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:7">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" ht="29" spans="1:7">
+      <c r="A18" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" ht="29" spans="1:7">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:7">
+      <c r="A20" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B21" t="s">
+        <v>475</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="B22" t="s">
+        <v>478</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:7">
+      <c r="A24" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" ht="29" spans="1:7">
+      <c r="A27" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" spans="1:7">
+      <c r="A30" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:3">
+      <c r="A31" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:7">
-      <c r="A20" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B21" t="s">
-        <v>476</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="B22" t="s">
-        <v>479</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="1:7">
-      <c r="A24" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" ht="29" spans="1:7">
-      <c r="A27" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>490</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="30" customFormat="1" spans="1:7">
-      <c r="A30" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="31" s="1" customFormat="1" spans="1:3">
-      <c r="A31" s="17" t="s">
+      <c r="B32" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="C32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="C33" s="4" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="6" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="C34" s="4" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="4" t="s">
+      <c r="B35" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="C35" s="4" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="4" t="s">
+      <c r="B36" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="C36" s="4" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="4" t="s">
+      <c r="B37" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
+      <c r="B38" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="4" t="s">
+      <c r="B39" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="4" t="s">
+      <c r="B40" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="4" t="s">
+      <c r="B41" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="4" t="s">
+      <c r="B42" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="4" t="s">
+      <c r="B43" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="4" t="s">
+      <c r="B45" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="4" t="s">
+      <c r="B47" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="4" t="s">
+      <c r="B48" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4" t="s">
+      <c r="B50" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="4" t="s">
+      <c r="B51" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="4" t="s">
+      <c r="B52" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" spans="3:3">
-      <c r="C54" s="20"/>
+      <c r="C54" s="22"/>
     </row>
     <row r="55" spans="3:3">
-      <c r="C55" s="20"/>
+      <c r="C55" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
+      <formula1>"Edit, Service, New,ChargeType"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
       <formula1>"Active, Inactive"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
-      <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
       <formula1>"Edit, New"</formula1>
@@ -6174,47 +6195,57 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="22.8181818181818" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="31.7272727272727" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="29.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.0909090909091" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" ht="43.5" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>414</v>
-      </c>
-      <c r="C3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6224,93 +6255,148 @@
       </c>
       <c r="C4">
         <f>COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIFS($A$8:$A$22,"*$*",D8:D22,"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>540</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>543</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>545</v>
+      </c>
+      <c r="B11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="C12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>548</v>
+      </c>
+      <c r="B13">
+        <v>1234</v>
+      </c>
+      <c r="C13">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>549</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B8</f>
+        <v>OCR BPKB</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>550</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:1">
@@ -6320,10 +6406,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="B24" t="s">
-        <v>550</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6331,15 +6417,15 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>551</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6353,7 +6439,7 @@
   <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -6381,7 +6467,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6395,23 +6481,23 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6419,7 +6505,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6427,12 +6513,12 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -6440,15 +6526,15 @@
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>453</v>
+      </c>
+      <c r="B16" t="s">
         <v>454</v>
-      </c>
-      <c r="B16" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -6509,10 +6595,10 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6639,16 +6725,16 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6673,16 +6759,16 @@
       <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="23">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="23">
         <v>123456788012</v>
       </c>
     </row>
@@ -6707,16 +6793,16 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="24" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6788,7 +6874,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D2" t="s">
@@ -6817,25 +6903,25 @@
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7203,7 +7289,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="25" t="s">
         <v>115</v>
       </c>
       <c r="B20" t="s">
@@ -7331,32 +7417,32 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -7552,43 +7638,43 @@
       <c r="A3" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -7655,7 +7741,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -7691,7 +7777,7 @@
       <c r="L8" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>155</v>
       </c>
       <c r="N8" t="s">
@@ -8205,61 +8291,61 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="3" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8350,7 +8436,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -8401,10 +8487,10 @@
       <c r="Q8" t="s">
         <v>229</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="3" t="s">
         <v>155</v>
       </c>
       <c r="T8" t="s">
@@ -9025,58 +9111,58 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -9163,61 +9249,61 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:19">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="3" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9799,52 +9885,52 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -9923,55 +10009,55 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:17">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -9979,52 +10065,52 @@
       <c r="A9" t="s">
         <v>300</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="O9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10581,55 +10667,55 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -10712,58 +10798,58 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:18">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="3" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AT49 Isi Saldo + AT73 Saldo + AT48 Dukcapil Dummy + AT72 Tenant
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="11"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="561">
   <si>
     <t>Status</t>
   </si>
@@ -1283,6 +1283,18 @@
     <t>1980-01-01</t>
   </si>
   <si>
+    <t>Verifikasi Identitas Dukcapil</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>CHECKFINANCE@GM.COM</t>
+  </si>
+  <si>
+    <t>Check1234!</t>
+  </si>
+  <si>
     <t>;Done well</t>
   </si>
   <si>
@@ -1313,12 +1325,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>CHECKFINANCE@GM.COM</t>
-  </si>
-  <si>
-    <t>Check1234!</t>
-  </si>
-  <si>
     <t>$Tenant</t>
   </si>
   <si>
@@ -1442,7 +1448,7 @@
     <t>API Key</t>
   </si>
   <si>
-    <t>pnDRcU</t>
+    <t>kyP4ih</t>
   </si>
   <si>
     <t>EfXHMQ</t>
@@ -1653,9 +1659,6 @@
   </si>
   <si>
     <t>DUKCAPIL_VIDA</t>
-  </si>
-  <si>
-    <t>Verifikasi Identitas Dukcapil</t>
   </si>
   <si>
     <t>;Fungsi pencarian gagal, no result</t>
@@ -1729,9 +1732,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
@@ -1765,17 +1768,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1788,40 +1782,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1833,32 +1798,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1866,6 +1815,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1881,7 +1838,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1895,15 +1875,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1924,67 +1927,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1996,103 +1945,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2105,6 +1958,156 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2190,17 +2193,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2210,24 +2207,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2242,6 +2221,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2263,16 +2257,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2290,7 +2293,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2308,130 +2311,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4441,7 +4444,7 @@
   <sheetPr/>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
@@ -4468,7 +4471,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -4516,9 +4519,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" ht="43.5" spans="1:17">
@@ -4752,7 +4758,7 @@
         <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>269</v>
+        <v>413</v>
       </c>
       <c r="C13" t="s">
         <v>121</v>
@@ -5080,7 +5086,7 @@
         <v>312</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5117,7 +5123,7 @@
         <v>316</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5125,7 +5131,7 @@
         <v>317</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -5175,10 +5181,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C2" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" ht="29" spans="1:5">
@@ -5186,16 +5192,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C3" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5226,36 +5232,36 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C9" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D9" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="E9" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5263,16 +5269,16 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C10" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="D10" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="E10" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5280,38 +5286,38 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C11" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D11" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E11" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B12" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C12" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D12" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E12" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -5328,7 +5334,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B14" t="s">
         <v>269</v>
@@ -5342,7 +5348,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -5359,7 +5365,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B16" s="23">
         <v>1130</v>
@@ -5376,7 +5382,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B17" t="str">
         <f>CONCATENATE("Isiulang ",B14)</f>
@@ -5397,24 +5403,24 @@
     </row>
     <row r="18" ht="29" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5463,7 +5469,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -5501,25 +5507,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5527,27 +5533,27 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B4" s="6">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
@@ -5594,30 +5600,30 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -5628,45 +5634,45 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -5677,49 +5683,49 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B14" s="10">
         <v>202304426</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -5730,7 +5736,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>34</v>
@@ -5745,22 +5751,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B16" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="G16" s="6"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -5771,37 +5777,37 @@
     </row>
     <row r="18" ht="29" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="11" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="9" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:7">
       <c r="A20" s="7" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -5812,52 +5818,52 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B21" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="6" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B22" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="6" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:7">
       <c r="A24" s="7" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -5867,67 +5873,67 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" ht="29" spans="1:7">
       <c r="A27" s="6" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="6" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5935,12 +5941,12 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:7">
       <c r="A30" s="6" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -5948,74 +5954,74 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:3">
       <c r="A31" s="19" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="6" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>128</v>
@@ -6024,16 +6030,16 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>121</v>
@@ -6042,7 +6048,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>124</v>
@@ -6051,25 +6057,25 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="6" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>126</v>
@@ -6078,82 +6084,82 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="6" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>537</v>
+        <v>413</v>
       </c>
       <c r="C52" s="6"/>
     </row>
@@ -6177,11 +6183,11 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
+      <formula1>"Active, Inactive"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
-      <formula1>"Active, Inactive"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
       <formula1>"Edit, New"</formula1>
@@ -6197,16 +6203,16 @@
   <sheetPr/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.8181818181818" customWidth="1"/>
+    <col min="2" max="2" width="31.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="29.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="26.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6220,7 +6226,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6228,7 +6234,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" ht="43.5" spans="1:4">
@@ -6236,13 +6242,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6264,12 +6270,12 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B8" t="s">
         <v>121</v>
@@ -6283,7 +6289,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B9" t="s">
         <v>159</v>
@@ -6294,27 +6300,27 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B11" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B12" t="s">
         <v>159</v>
@@ -6325,7 +6331,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B13">
         <v>1234</v>
@@ -6336,7 +6342,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B14" t="str">
         <f>B8</f>
@@ -6345,19 +6351,19 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B16" t="s">
         <v>159</v>
@@ -6368,7 +6374,7 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -6406,10 +6412,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6417,7 +6423,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -6467,7 +6473,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6481,23 +6487,23 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6505,7 +6511,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6513,12 +6519,12 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -6526,15 +6532,15 @@
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B16" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AT 77 Layanan Saya Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="14"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="560">
   <si>
     <t>Status</t>
   </si>
@@ -1718,13 +1718,10 @@
     <t>Data Login</t>
   </si>
   <si>
-    <t>USERA@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>P@ssw0rd123</t>
-  </si>
-  <si>
-    <t>PT A</t>
+    <t>API KEY controller</t>
+  </si>
+  <si>
+    <t>Tipe API KEY</t>
   </si>
 </sst>
 </file>
@@ -1733,9 +1730,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="23">
@@ -1768,6 +1765,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1775,26 +1773,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1806,6 +1796,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1820,6 +1818,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1829,10 +1835,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1844,8 +1850,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1853,30 +1860,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1891,15 +1874,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1907,6 +1882,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1927,7 +1924,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1939,31 +1972,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1975,49 +2002,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2035,7 +2050,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2047,67 +2098,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2195,33 +2192,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2242,6 +2217,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2256,17 +2246,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2282,18 +2281,16 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2311,136 +2308,137 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2858,8 +2856,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -2880,16 +2878,16 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3022,92 +3020,92 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="30">
         <v>999999</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29" t="s">
+      <c r="E14" s="30"/>
+      <c r="F14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
         <v>2</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="7">
         <v>2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3117,22 +3115,22 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
@@ -3140,8 +3138,8 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
@@ -3152,15 +3150,15 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C14:D14 F14:G14" numberStoredAsText="1"/>
+    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3281,46 +3279,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3391,49 +3389,49 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:15">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3908,46 +3906,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4018,49 +4016,49 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4531,52 +4529,52 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4655,55 +4653,55 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:17">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>405</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4711,29 +4709,29 @@
       <c r="A9" t="s">
         <v>406</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>408</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="28">
         <v>7183259386136510</v>
       </c>
     </row>
@@ -4749,7 +4747,7 @@
       <c r="A12" t="s">
         <v>411</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="29" t="s">
         <v>412</v>
       </c>
     </row>
@@ -5200,7 +5198,7 @@
       <c r="D3" t="s">
         <v>421</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>422</v>
       </c>
     </row>
@@ -5367,16 +5365,16 @@
       <c r="A16" t="s">
         <v>432</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="24">
         <v>1130</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="24">
         <v>1131</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="24">
         <v>1121</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="24">
         <v>1116</v>
       </c>
     </row>
@@ -5402,19 +5400,19 @@
       </c>
     </row>
     <row r="18" ht="29" spans="1:5">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>436</v>
       </c>
     </row>
@@ -5427,19 +5425,19 @@
       <c r="A20" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="24" t="str">
+      <c r="B20" s="25" t="str">
         <f>B14</f>
         <v>IDR</v>
       </c>
-      <c r="C20" s="24" t="str">
+      <c r="C20" s="25" t="str">
         <f>C14</f>
         <v>OCR BPKB</v>
       </c>
-      <c r="D20" s="24" t="str">
+      <c r="D20" s="25" t="str">
         <f>D14</f>
         <v>OCR STNK</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
@@ -5483,714 +5481,714 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <f>IF(C7="New",COUNTIFS($A$12:$A$23,"*$*",C12:C23,""),IF(C7="Service",COUNTIFS($A$9:$A$10,"*$*",C9:C10,""),IF(C7="Edit",COUNTIFS($A$9:$A$21,"*$*",C9:C21,""),0)))</f>
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <f>IF(D7="New",COUNTIFS($A$12:$A$23,"*$*",D12:D23,""),IF(D7="Service",COUNTIFS($A$9:$A$10,"*$*",D9:D10,""),IF(D7="Edit",COUNTIFS($A$9:$A$21,"*$*",D9:D21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <f>IF(E7="New",COUNTIFS($A$12:$A$23,"*$*",E12:E23,""),IF(E7="Service",COUNTIFS($A$9:$A$10,"*$*",E9:E10,""),IF(E7="Edit",COUNTIFS($A$9:$A$21,"*$*",E9:E21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <f>IF(F7="New",COUNTIFS($A$12:$A$23,"*$*",F12:F23,""),IF(F7="Service",COUNTIFS($A$9:$A$10,"*$*",F9:F10,""),IF(F7="Edit",COUNTIFS($A$9:$A$21,"*$*",F9:F21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <f>IF(G7="New",COUNTIFS($A$12:$A$23,"*$*",G12:G23,""),IF(G7="Service",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),IF(G7="Edit",COUNTIFS($A$9:$A$21,"*$*",G9:G21,""),IF(G7="ChargeType",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),0))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:7">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="11">
         <v>202304426</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="32" t="s">
         <v>465</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11">
         <v>202304277</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="9"/>
+      <c r="B15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>467</v>
       </c>
       <c r="B16" t="s">
         <v>468</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
       <c r="F16" t="s">
         <v>469</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:7">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" ht="29" spans="1:7">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="11" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="G18" s="6"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:7">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>476</v>
       </c>
       <c r="B21" t="s">
         <v>477</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="6" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>479</v>
       </c>
       <c r="B22" t="s">
         <v>480</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="6" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="G23" s="6"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:7">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="14"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" ht="29" spans="1:7">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="14"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:7">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="7" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="6"/>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="7" t="s">
         <v>519</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="6"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="C46" s="6"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="C47" s="6"/>
+      <c r="C47" s="7"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="C48" s="6"/>
+      <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="7"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="C50" s="6"/>
+      <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="C51" s="6"/>
+      <c r="C51" s="7"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="C52" s="6"/>
+      <c r="C52" s="7"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C53" s="6"/>
+      <c r="C53" s="7"/>
     </row>
     <row r="54" spans="3:3">
-      <c r="C54" s="22"/>
+      <c r="C54" s="23"/>
     </row>
     <row r="55" spans="3:3">
-      <c r="C55" s="22"/>
+      <c r="C55" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
-      <formula1>"Active, Inactive"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
+      <formula1>"Edit, New"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
-      <formula1>"Edit, New"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
+      <formula1>"Active, Inactive"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6203,7 +6201,7 @@
   <sheetPr/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -6241,13 +6239,13 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6302,13 +6300,13 @@
       <c r="A10" t="s">
         <v>544</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>545</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>545</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
@@ -6353,13 +6351,13 @@
       <c r="A15" t="s">
         <v>551</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
@@ -6443,16 +6441,16 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="40.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6481,7 +6479,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f>COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f>COUNTIFS($A$8:$A$14,"*$*",B8:B14,"")</f>
         <v>0</v>
       </c>
     </row>
@@ -6492,58 +6490,39 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>423</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>425</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:1">
+      <c r="A11" s="3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:1">
-      <c r="A14" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>455</v>
-      </c>
-      <c r="B16" t="s">
-        <v>456</v>
+      <c r="B12" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>"PRODUCTION,TRIAL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -6601,10 +6580,10 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6731,16 +6710,16 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="24" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6765,16 +6744,16 @@
       <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="24">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="24">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="24">
         <v>123456788012</v>
       </c>
     </row>
@@ -6799,16 +6778,16 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6880,7 +6859,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D2" t="s">
@@ -6909,25 +6888,25 @@
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7295,7 +7274,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>115</v>
       </c>
       <c r="B20" t="s">
@@ -7423,32 +7402,32 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -7644,43 +7623,43 @@
       <c r="A3" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -7747,7 +7726,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -7783,7 +7762,7 @@
       <c r="L8" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>155</v>
       </c>
       <c r="N8" t="s">
@@ -8297,61 +8276,61 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="4" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8442,7 +8421,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -8493,10 +8472,10 @@
       <c r="Q8" t="s">
         <v>229</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="4" t="s">
         <v>155</v>
       </c>
       <c r="T8" t="s">
@@ -9117,58 +9096,58 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>253</v>
       </c>
     </row>
@@ -9255,61 +9234,61 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:19">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="4" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9891,52 +9870,52 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -10015,55 +9994,55 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:17">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10071,52 +10050,52 @@
       <c r="A9" t="s">
         <v>300</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="Q9" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10673,55 +10652,55 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>332</v>
       </c>
     </row>
@@ -10804,58 +10783,58 @@
       </c>
     </row>
     <row r="8" ht="29" spans="1:18">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="4" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AT 77 re-update Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,32 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="15"/>
+    <workbookView activeTab="15" firstSheet="11" windowHeight="7070" windowWidth="18530"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" sheetId="1" r:id="rId1"/>
-    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
-    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
-    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
-    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
-    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
-    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
-    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
-    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
-    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
-    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
-    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
-    <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
-    <sheet name="Tenant" sheetId="14" r:id="rId14"/>
-    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
-    <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
+    <sheet name="Register" r:id="rId1" sheetId="1"/>
+    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
+    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
+    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
+    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
+    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
+    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
+    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
+    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
+    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
+    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
+    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
+    <sheet name="IsiSaldo" r:id="rId13" sheetId="13"/>
+    <sheet name="Tenant" r:id="rId14" sheetId="14"/>
+    <sheet name="Saldo" r:id="rId15" sheetId="15"/>
+    <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="561">
   <si>
     <t>Status</t>
   </si>
@@ -1722,6 +1722,9 @@
   </si>
   <si>
     <t>Tipe API KEY</t>
+  </si>
+  <si>
+    <t>;Table error/tidak muncul</t>
   </si>
 </sst>
 </file>
@@ -1729,10 +1732,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="23">
@@ -2289,265 +2292,265 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="16" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="5" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="25" fontId="22" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="3" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="3" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="33">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="7"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
+    <cellStyle builtinId="10" name="Note" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2561,10 +2564,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2728,21 +2731,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2759,7 +2762,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2812,9 +2815,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -2822,11 +2825,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2868,7 +2871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:7">
+    <row ht="43.5" r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2896,31 +2899,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3014,7 +3017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -3154,19 +3157,19 @@
       <c r="C21" s="25"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -3174,20 +3177,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="57.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="37.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.9090909090909" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="57.1818181818182" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="37.2727272727273" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3275,7 +3278,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:15">
+    <row ht="29" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3339,31 +3342,31 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
+        <f ref="E4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3383,12 +3386,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:15">
+    <row ht="29" r="8" spans="1:15">
       <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
@@ -3529,7 +3532,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -3722,7 +3725,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -3820,15 +3823,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3836,18 +3839,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="35.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="35.3636363636364" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.6363636363636" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3902,7 +3905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:15">
+    <row ht="43.5" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3970,27 +3973,27 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
+        <f ref="F4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -4010,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -4156,7 +4159,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -4349,7 +4352,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -4410,7 +4413,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -4432,15 +4435,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="B1:C2"/>
@@ -4448,20 +4451,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
-    <col min="10" max="10" width="75.9090909090909" customWidth="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1"/>
-    <col min="12" max="12" width="45.1818181818182" customWidth="1"/>
-    <col min="13" max="16" width="35.7272727272727" customWidth="1"/>
-    <col min="17" max="17" width="35.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="75.9090909090909" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="35.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -4525,7 +4528,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:17">
+    <row ht="43.5" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4591,55 +4594,55 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:P4" si="0">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f ref="D4:P4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>4</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
       <c r="Q4">
@@ -4647,12 +4650,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="26" t="s">
         <v>405</v>
       </c>
@@ -4857,7 +4860,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>160</v>
       </c>
@@ -5074,7 +5077,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="21" s="1" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>175</v>
       </c>
@@ -5111,7 +5114,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="26" s="1" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>189</v>
       </c>
@@ -5133,18 +5136,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B9" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="B9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -5152,9 +5155,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="27" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7272727272727" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5185,7 +5188,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5223,7 +5226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>Isiulang </v>
       </c>
     </row>
-    <row r="18" ht="29" spans="1:5">
+    <row ht="29" r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>434</v>
       </c>
@@ -5416,7 +5419,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="19" s="1" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>437</v>
       </c>
@@ -5456,15 +5459,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -5472,12 +5475,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="30.1818181818182" customWidth="1"/>
-    <col min="2" max="2" width="42.3636363636364" customWidth="1"/>
-    <col min="3" max="3" width="21.8181818181818" customWidth="1"/>
-    <col min="4" max="5" width="32.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="36.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="26.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.8181818181818" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="32.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5619,7 +5622,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="8" s="1" spans="1:7">
       <c r="A8" s="8" t="s">
         <v>451</v>
       </c>
@@ -5668,7 +5671,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="11" s="1" spans="1:7">
       <c r="A11" s="8" t="s">
         <v>457</v>
       </c>
@@ -5762,7 +5765,7 @@
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="17" s="1" spans="1:7">
       <c r="A17" s="8" t="s">
         <v>470</v>
       </c>
@@ -5773,7 +5776,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" ht="29" spans="1:7">
+    <row ht="29" r="18" spans="1:7">
       <c r="A18" s="7" t="s">
         <v>471</v>
       </c>
@@ -5803,7 +5806,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="20" s="1" spans="1:7">
       <c r="A20" s="8" t="s">
         <v>475</v>
       </c>
@@ -5859,7 +5862,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="24" s="1" spans="1:7">
       <c r="A24" s="8" t="s">
         <v>485</v>
       </c>
@@ -5899,7 +5902,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" ht="29" spans="1:7">
+    <row ht="29" r="27" spans="1:7">
       <c r="A27" s="7" t="s">
         <v>490</v>
       </c>
@@ -5942,7 +5945,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="30" customFormat="1" spans="1:7">
+    <row customFormat="1" r="30" spans="1:7">
       <c r="A30" s="7" t="s">
         <v>497</v>
       </c>
@@ -5955,7 +5958,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" spans="1:3">
+    <row customFormat="1" r="31" s="1" spans="1:3">
       <c r="A31" s="20" t="s">
         <v>499</v>
       </c>
@@ -6181,25 +6184,25 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
       <formula1>"Edit, New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10 E10 F10 G10" type="list">
       <formula1>"Active, Inactive"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -6207,10 +6210,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.8181818181818" customWidth="1"/>
-    <col min="2" max="2" width="31.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="29.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="26.0909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.8181818181818" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.2727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.0909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6235,7 +6238,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:4">
+    <row ht="43.5" r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6266,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>437</v>
       </c>
@@ -6370,7 +6373,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="18" s="1" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>554</v>
       </c>
@@ -6403,7 +6406,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="23" s="1" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>189</v>
       </c>
@@ -6426,22 +6429,22 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -6449,8 +6452,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="40.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.6363636363636" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6458,13 +6461,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -6483,7 +6489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>557</v>
       </c>
@@ -6504,7 +6510,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="3" t="s">
         <v>558</v>
       </c>
@@ -6519,19 +6525,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12" type="list">
       <formula1>"PRODUCTION,TRIAL"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:B9"/>
@@ -6539,10 +6545,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6570,7 +6576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6608,7 +6614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -6792,18 +6798,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C16" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -6811,16 +6817,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6852,7 +6858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="29" spans="1:9">
+    <row ht="29" r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6881,7 +6887,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:9">
+    <row ht="29" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6915,39 +6921,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -7181,7 +7187,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
@@ -7304,7 +7310,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -7315,15 +7321,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:B9"/>
@@ -7331,16 +7337,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7398,7 +7404,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:11">
+    <row ht="43.5" r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7438,35 +7444,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>119</v>
       </c>
@@ -7531,19 +7537,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -7551,14 +7557,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="51.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="43.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="35.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="36.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="51.5454545454545" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="35.2727272727273" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="36.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7619,7 +7625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:14">
+    <row ht="29" r="3" spans="1:14">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -7672,35 +7678,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -7720,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -7857,7 +7863,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -8038,7 +8044,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>175</v>
       </c>
@@ -8099,7 +8105,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -8121,15 +8127,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
@@ -8137,21 +8143,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="46.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="51.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="53.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="29.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="46.8181818181818" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="51.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="53.3636363636364" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.8181818181818" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="31.4545454545455" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="29.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -8272,7 +8278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:20">
+    <row ht="29" r="3" spans="1:20">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8339,67 +8345,67 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:Q4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:Q4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="R4">
@@ -8415,7 +8421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -8606,7 +8612,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -8859,7 +8865,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -8920,7 +8926,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -8942,39 +8948,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="R1" activePane="topLeft"/>
+      <pane activePane="topLeft" topLeftCell="R1" xSplit="18280"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="38.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="10" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="40.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="43.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="43.6363636363636" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9092,7 +9098,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:19">
+    <row ht="43.5" r="3" spans="1:19">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9160,59 +9166,59 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9228,12 +9234,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:19">
+    <row ht="29" r="8" spans="1:19">
       <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
@@ -9410,7 +9416,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -9651,7 +9657,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -9712,7 +9718,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -9734,15 +9740,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -9750,20 +9756,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="52.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="54.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="58" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="51.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="12" max="15" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="43" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="54.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.6363636363636" collapsed="true"/>
+    <col min="12" max="15" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -9866,7 +9872,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:17">
+    <row ht="43.5" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9932,55 +9938,55 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:J4" si="0">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
+        <f ref="D4:J4" si="0" t="shared">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9988,12 +9994,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="26" t="s">
         <v>288</v>
       </c>
@@ -10046,7 +10052,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" ht="29" spans="1:17">
+    <row ht="29" r="9" spans="1:17">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -10205,7 +10211,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>160</v>
       </c>
@@ -10422,7 +10428,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>175</v>
       </c>
@@ -10483,7 +10489,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="25" s="1" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>189</v>
       </c>
@@ -10505,41 +10511,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="T1" activePane="topLeft"/>
+      <pane activePane="topLeft" topLeftCell="T1" xSplit="18280"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="43.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="30.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.2727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.5454545454545" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.5454545454545" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10648,7 +10654,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:18">
+    <row ht="43.5" r="3" spans="1:18">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10709,59 +10715,59 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:O4" si="0">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <f ref="B4:O4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -10777,12 +10783,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:18">
+    <row ht="29" r="8" spans="1:18">
       <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
@@ -10950,7 +10956,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -11179,7 +11185,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -11240,7 +11246,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -11262,7 +11268,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AT 73 Saldo + AT 77 Layanan Saya balikan Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -1768,19 +1768,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1791,16 +1783,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1815,47 +1861,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1866,27 +1872,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1905,8 +1890,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1927,7 +1927,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1939,7 +1951,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1951,25 +2035,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1981,73 +2095,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2059,55 +2107,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2205,36 +2205,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2268,7 +2238,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2277,7 +2247,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2290,10 +2275,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
@@ -2311,137 +2311,136 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="16" fontId="12" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="14" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="13" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="5" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="15" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="20" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="14" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="10" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="25" fontId="22" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="19" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="10" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="3" fontId="5" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="19" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="3" fontId="9" numFmtId="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="21" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="22" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="4" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="19" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="18" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
@@ -2859,8 +2858,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -2881,16 +2880,16 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3023,92 +3022,92 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
         <v>999999</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="29"/>
+      <c r="F14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>2</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3118,22 +3117,22 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
@@ -3141,8 +3140,8 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
@@ -3153,8 +3152,8 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3282,46 +3281,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3392,49 +3391,49 @@
       </c>
     </row>
     <row ht="29" r="8" spans="1:15">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3909,46 +3908,46 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4019,49 +4018,49 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4532,52 +4531,52 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4656,55 +4655,55 @@
       </c>
     </row>
     <row ht="29" r="8" spans="1:17">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4712,29 +4711,29 @@
       <c r="A9" t="s">
         <v>406</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>407</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>408</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>7183259386136510</v>
       </c>
     </row>
@@ -4750,7 +4749,7 @@
       <c r="A12" t="s">
         <v>411</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>412</v>
       </c>
     </row>
@@ -5201,7 +5200,7 @@
       <c r="D3" t="s">
         <v>421</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>422</v>
       </c>
     </row>
@@ -5368,16 +5367,16 @@
       <c r="A16" t="s">
         <v>432</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>1130</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>1131</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>1121</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="23">
         <v>1116</v>
       </c>
     </row>
@@ -5403,19 +5402,19 @@
       </c>
     </row>
     <row ht="29" r="18" spans="1:5">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>436</v>
       </c>
     </row>
@@ -5428,19 +5427,19 @@
       <c r="A20" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="25" t="str">
+      <c r="B20" s="24" t="str">
         <f>B14</f>
         <v>IDR</v>
       </c>
-      <c r="C20" s="25" t="str">
+      <c r="C20" s="24" t="str">
         <f>C14</f>
         <v>OCR BPKB</v>
       </c>
-      <c r="D20" s="25" t="str">
+      <c r="D20" s="24" t="str">
         <f>D14</f>
         <v>OCR STNK</v>
       </c>
-      <c r="E20" s="25"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
@@ -5484,714 +5483,714 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f>IF(C7="New",COUNTIFS($A$12:$A$23,"*$*",C12:C23,""),IF(C7="Service",COUNTIFS($A$9:$A$10,"*$*",C9:C10,""),IF(C7="Edit",COUNTIFS($A$9:$A$21,"*$*",C9:C21,""),0)))</f>
         <v>2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <f>IF(D7="New",COUNTIFS($A$12:$A$23,"*$*",D12:D23,""),IF(D7="Service",COUNTIFS($A$9:$A$10,"*$*",D9:D10,""),IF(D7="Edit",COUNTIFS($A$9:$A$21,"*$*",D9:D21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <f>IF(E7="New",COUNTIFS($A$12:$A$23,"*$*",E12:E23,""),IF(E7="Service",COUNTIFS($A$9:$A$10,"*$*",E9:E10,""),IF(E7="Edit",COUNTIFS($A$9:$A$21,"*$*",E9:E21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f>IF(F7="New",COUNTIFS($A$12:$A$23,"*$*",F12:F23,""),IF(F7="Service",COUNTIFS($A$9:$A$10,"*$*",F9:F10,""),IF(F7="Edit",COUNTIFS($A$9:$A$21,"*$*",F9:F21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f>IF(G7="New",COUNTIFS($A$12:$A$23,"*$*",G12:G23,""),IF(G7="Service",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),IF(G7="Edit",COUNTIFS($A$9:$A$21,"*$*",G9:G21,""),IF(G7="ChargeType",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),0))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>450</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="1" spans="1:7">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>456</v>
       </c>
     </row>
     <row customFormat="1" r="11" s="1" spans="1:7">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>202304426</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>465</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10">
         <v>202304277</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="10"/>
+      <c r="B15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>467</v>
       </c>
       <c r="B16" t="s">
         <v>468</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" t="s">
         <v>469</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="6"/>
     </row>
     <row customFormat="1" r="17" s="1" spans="1:7">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row ht="29" r="18" spans="1:7">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="12" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="10" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="6"/>
     </row>
     <row customFormat="1" r="20" s="1" spans="1:7">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>476</v>
       </c>
       <c r="B21" t="s">
         <v>477</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="7" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>479</v>
       </c>
       <c r="B22" t="s">
         <v>480</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="7" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="G23" s="7"/>
+      <c r="G23" s="6"/>
     </row>
     <row customFormat="1" r="24" s="1" spans="1:7">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="15"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="15"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
     </row>
     <row ht="29" r="27" spans="1:7">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>491</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="17"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
         <v>496</v>
       </c>
     </row>
     <row customFormat="1" r="30" spans="1:7">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="s">
         <v>498</v>
       </c>
     </row>
     <row customFormat="1" r="31" s="1" spans="1:3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" spans="3:3">
-      <c r="C54" s="23"/>
+      <c r="C54" s="22"/>
     </row>
     <row r="55" spans="3:3">
-      <c r="C55" s="23"/>
+      <c r="C55" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
-      <formula1>"Edit, New"</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10 E10 F10 G10" type="list">
       <formula1>"Active, Inactive"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
+      <formula1>"Edit, New"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -6204,8 +6203,8 @@
   <sheetPr/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -6227,7 +6226,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6242,13 +6241,13 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6303,13 +6302,13 @@
       <c r="A10" t="s">
         <v>544</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
@@ -6354,13 +6353,13 @@
       <c r="A15" t="s">
         <v>551</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
@@ -6447,7 +6446,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -6511,7 +6510,7 @@
       </c>
     </row>
     <row customFormat="1" r="11" s="1" spans="1:1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>558</v>
       </c>
     </row>
@@ -6586,10 +6585,10 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6716,16 +6715,16 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6750,16 +6749,16 @@
       <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="23">
         <v>123456788012</v>
       </c>
     </row>
@@ -6784,16 +6783,16 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6865,7 +6864,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D2" t="s">
@@ -6894,25 +6893,25 @@
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7280,7 +7279,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>115</v>
       </c>
       <c r="B20" t="s">
@@ -7408,32 +7407,32 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -7629,43 +7628,43 @@
       <c r="A3" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -7732,7 +7731,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -7768,7 +7767,7 @@
       <c r="L8" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>155</v>
       </c>
       <c r="N8" t="s">
@@ -8282,61 +8281,61 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="3" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8427,7 +8426,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
@@ -8478,10 +8477,10 @@
       <c r="Q8" t="s">
         <v>229</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="3" t="s">
         <v>155</v>
       </c>
       <c r="T8" t="s">
@@ -9102,58 +9101,58 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -9240,61 +9239,61 @@
       </c>
     </row>
     <row ht="29" r="8" spans="1:19">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="3" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9876,52 +9875,52 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -10000,55 +9999,55 @@
       </c>
     </row>
     <row ht="29" r="8" spans="1:17">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10056,52 +10055,52 @@
       <c r="A9" t="s">
         <v>300</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10658,55 +10657,55 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -10789,58 +10788,58 @@
       </c>
     </row>
     <row ht="29" r="8" spans="1:18">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="3" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AT 73 Saldo, AT 77 Layanan Saya balikan Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,32 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="15" firstSheet="11" windowHeight="7070" windowWidth="18530"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" r:id="rId1" sheetId="1"/>
-    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
-    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
-    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
-    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
-    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
-    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
-    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
-    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
-    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
-    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
-    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
-    <sheet name="IsiSaldo" r:id="rId13" sheetId="13"/>
-    <sheet name="Tenant" r:id="rId14" sheetId="14"/>
-    <sheet name="Saldo" r:id="rId15" sheetId="15"/>
-    <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
+    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
+    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
+    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
+    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
+    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
+    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
+    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
+    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
+    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
+    <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
+    <sheet name="Tenant" sheetId="14" r:id="rId14"/>
+    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
+    <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="549">
   <si>
     <t>Status</t>
   </si>
@@ -1223,42 +1223,6 @@
     <t>Success, karena bpkb halaman 2 dan 3 sesuai requirement</t>
   </si>
   <si>
-    <t>Gagal karena tingkat blur yang mengganggu proses OCR</t>
-  </si>
-  <si>
-    <t>Gagal, karena pada foto halaman2 terdapat STNK di dalamnya</t>
-  </si>
-  <si>
-    <t>Gagal, karena bpkb dalam foto ada dua</t>
-  </si>
-  <si>
-    <t>50% kemungkinan berhasil karena versi lama mungkin cocok dengan OCR terkini</t>
-  </si>
-  <si>
-    <t>50% berhasil karena foto terlalu silau terkena flash</t>
-  </si>
-  <si>
-    <t>Gagal karena salah satu halaman memilki resolusi sangat tinggi</t>
-  </si>
-  <si>
-    <t>Gagal, API Key salah</t>
-  </si>
-  <si>
-    <t>Gagal karena salah satu halaman memiliki resolusi terlalu rendah</t>
-  </si>
-  <si>
-    <t>Dengan dikirim 1 parameter saja seharusnya success</t>
-  </si>
-  <si>
-    <t>Dengan dikirim parameter halaman 3 saja, maka kemungkinan bisa success</t>
-  </si>
-  <si>
-    <t>Gagal, karena tenant code salah</t>
-  </si>
-  <si>
-    <t>Gagal, karena tidak ada img untuk OCR</t>
-  </si>
-  <si>
     <t>$selfiephoto</t>
   </si>
   <si>
@@ -1712,6 +1676,9 @@
     <t>Username</t>
   </si>
   <si>
+    <t>;Table error/tidak muncul</t>
+  </si>
+  <si>
     <t>Success verifikasi</t>
   </si>
   <si>
@@ -1722,9 +1689,6 @@
   </si>
   <si>
     <t>Tipe API KEY</t>
-  </si>
-  <si>
-    <t>;Table error/tidak muncul</t>
   </si>
 </sst>
 </file>
@@ -1732,10 +1696,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="23">
@@ -1768,6 +1732,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1790,32 +1762,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1830,14 +1779,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1846,24 +1787,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1876,7 +1810,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1884,7 +1818,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1911,6 +1845,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1933,7 +1897,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1945,43 +1957,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1993,55 +1981,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2059,19 +1999,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2083,31 +2059,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2193,32 +2157,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2230,15 +2168,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2270,8 +2199,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2290,266 +2234,286 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="14" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="13" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="15" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="18" numFmtId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="12" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="10" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="21" numFmtId="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="19" fontId="20" numFmtId="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="19" fontId="15" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="22" numFmtId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="14" numFmtId="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="7"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
-    <cellStyle builtinId="10" name="Note" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2563,10 +2527,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2730,21 +2694,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2761,7 +2725,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2814,9 +2778,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -2824,11 +2788,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
+    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2870,7 +2834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:7">
+    <row r="3" ht="43.5" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2898,31 +2862,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3016,7 +2980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:1">
+    <row r="12" s="1" customFormat="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3111,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:1">
+    <row r="17" s="1" customFormat="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -3156,19 +3120,19 @@
       <c r="C21" s="24"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
+    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -3176,20 +3140,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.9090909090909" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="57.1818181818182" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="37.2727272727273" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="57.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="37.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="36.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="35.7272727272727" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3277,7 +3241,7 @@
         <v>197</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:15">
+    <row r="3" ht="29" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3341,31 +3305,31 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f ref="E4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
+        <f t="shared" ref="E4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3385,12 +3349,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:15">
+    <row r="8" ht="29" spans="1:15">
       <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
@@ -3531,7 +3495,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -3724,7 +3688,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -3822,15 +3786,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3838,18 +3802,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="35.3636363636364" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.6363636363636" collapsed="true"/>
+    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="35.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.6363636363636" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3904,7 +3868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:15">
+    <row r="3" ht="43.5" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3972,27 +3936,27 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f ref="F4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
+        <f t="shared" ref="F4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -4012,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -4158,7 +4122,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -4351,7 +4315,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -4412,7 +4376,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row r="24" s="1" customFormat="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -4434,36 +4398,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="75.9090909090909" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="35.1818181818182" collapsed="true"/>
+    <col min="1" max="1" width="21.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="35.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="35.8181818181818" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="34.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="34.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="33.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="34.1818181818182" customWidth="1"/>
+    <col min="9" max="9" width="36.5454545454545" customWidth="1"/>
+    <col min="10" max="10" width="75.9090909090909" customWidth="1"/>
+    <col min="11" max="11" width="35.7272727272727" customWidth="1"/>
+    <col min="12" max="12" width="45.1818181818182" customWidth="1"/>
+    <col min="13" max="16" width="35.7272727272727" customWidth="1"/>
+    <col min="17" max="17" width="35.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -4471,7 +4435,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -4519,66 +4483,33 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row ht="43.5" r="3" spans="1:17">
+    </row>
+    <row r="3" ht="29" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -4593,55 +4524,55 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f ref="D4:P4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f t="shared" ref="D4:P4" si="0">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>4</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="O4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q4">
@@ -4649,14 +4580,14 @@
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:17">
+    <row r="8" ht="29" spans="1:17">
       <c r="A8" s="25" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>289</v>
@@ -4709,10 +4640,10 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4731,7 +4662,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="B10" s="27">
         <v>7183259386136510</v>
@@ -4739,18 +4670,18 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="B11" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -4758,7 +4689,7 @@
         <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C13" t="s">
         <v>121</v>
@@ -4859,7 +4790,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>160</v>
       </c>
@@ -5076,7 +5007,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:1">
+    <row r="21" s="1" customFormat="1" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>175</v>
       </c>
@@ -5086,7 +5017,7 @@
         <v>312</v>
       </c>
       <c r="B22" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5113,7 +5044,7 @@
         <v>184</v>
       </c>
     </row>
-    <row customFormat="1" r="26" s="1" spans="1:1">
+    <row r="26" s="1" customFormat="1" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>189</v>
       </c>
@@ -5123,7 +5054,7 @@
         <v>316</v>
       </c>
       <c r="B27" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5131,22 +5062,22 @@
         <v>317</v>
       </c>
       <c r="B28" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="B9"/>
+    <ignoredError sqref="B9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -5154,9 +5085,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7272727272727" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="1" max="1" width="18.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="27" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5181,27 +5112,27 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="C2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row ht="29" r="3" spans="1:5">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" ht="29" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C3" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D3" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5225,43 +5156,43 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="B8" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="C8" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D8" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="E8" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="B9" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="C9" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D9" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="E9" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5269,16 +5200,16 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="C10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="E10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5286,38 +5217,38 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="C11" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="D11" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="E11" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="B12" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="C12" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D12" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="E12" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -5334,7 +5265,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B14" t="s">
         <v>269</v>
@@ -5348,7 +5279,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -5365,7 +5296,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B16" s="23">
         <v>1130</v>
@@ -5382,7 +5313,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B17" t="str">
         <f>CONCATENATE("Isiulang ",B14)</f>
@@ -5401,26 +5332,26 @@
         <v>Isiulang </v>
       </c>
     </row>
-    <row ht="29" r="18" spans="1:5">
+    <row r="18" ht="29" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row customFormat="1" r="19" s="1" spans="1:1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5458,15 +5389,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -5474,12 +5405,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.1818181818182" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.3636363636364" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.8181818181818" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="32.2727272727273" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="36.8181818181818" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="1" max="1" width="30.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="32.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.1818181818182" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5507,25 +5438,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5533,27 +5464,27 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="B4" s="6">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
@@ -5600,30 +5531,30 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row customFormat="1" r="8" s="1" spans="1:7">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -5634,45 +5565,45 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row customFormat="1" r="11" s="1" spans="1:7">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -5683,49 +5614,49 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="B14" s="10">
         <v>202304426</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -5736,7 +5667,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>34</v>
@@ -5751,22 +5682,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="B16" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:7">
+    <row r="17" s="1" customFormat="1" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -5775,39 +5706,39 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row ht="29" r="18" spans="1:7">
+    <row r="18" ht="29" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="11" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="9" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:7">
+    <row r="20" s="1" customFormat="1" spans="1:7">
       <c r="A20" s="7" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -5818,52 +5749,52 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="B21" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="6" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="B22" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="6" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:7">
+    <row r="24" s="1" customFormat="1" spans="1:7">
       <c r="A24" s="7" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -5873,67 +5804,67 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
-    <row ht="29" r="27" spans="1:7">
+    <row r="27" ht="29" spans="1:7">
       <c r="A27" s="6" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="6" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5941,12 +5872,12 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row customFormat="1" r="30" spans="1:7">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" spans="1:7">
       <c r="A30" s="6" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -5954,74 +5885,74 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row customFormat="1" r="31" s="1" spans="1:3">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:3">
       <c r="A31" s="19" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="6" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>128</v>
@@ -6030,16 +5961,16 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>121</v>
@@ -6048,7 +5979,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>124</v>
@@ -6057,25 +5988,25 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="6" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>126</v>
@@ -6084,82 +6015,82 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="6" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C52" s="6"/>
     </row>
@@ -6183,25 +6114,25 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10 E10 F10 G10" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
       <formula1>"Active, Inactive"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
       <formula1>"Edit, New"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -6209,10 +6140,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.8181818181818" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.2727272727273" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.0909090909091" collapsed="true"/>
+    <col min="1" max="1" width="22.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.0909090909091" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6234,21 +6165,21 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row ht="43.5" r="3" spans="1:4">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" ht="43.5" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>542</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6268,14 +6199,14 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B8" t="s">
         <v>121</v>
@@ -6289,7 +6220,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="B9" t="s">
         <v>159</v>
@@ -6300,27 +6231,27 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="B11" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B12" t="s">
         <v>159</v>
@@ -6331,7 +6262,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B13">
         <v>1234</v>
@@ -6342,7 +6273,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B14" t="str">
         <f>B8</f>
@@ -6351,19 +6282,19 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="B16" t="s">
         <v>159</v>
@@ -6372,9 +6303,9 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:1">
+    <row r="18" s="1" customFormat="1" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -6405,17 +6336,17 @@
         <v>35</v>
       </c>
     </row>
-    <row customFormat="1" r="23" s="1" spans="1:1">
+    <row r="23" s="1" customFormat="1" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="B24" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6423,36 +6354,36 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="40.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6463,12 +6394,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6476,7 +6407,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6484,13 +6415,13 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f>COUNTIFS($A$8:$A$14,"*$*",B8:B14,"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f>COUNTIFS($A$8:$A$13,"*$*",B8:B13,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6498,7 +6429,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6506,37 +6437,37 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
-      <c r="A11" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>559</v>
-      </c>
-      <c r="B12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>548</v>
+      </c>
+      <c r="B11" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
       <formula1>"PRODUCTION,TRIAL"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:B9"/>
@@ -6544,10 +6475,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6575,7 +6506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:5">
+    <row r="3" ht="29" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6613,7 +6544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -6797,18 +6728,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C16"/>
+    <ignoredError sqref="C16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -6816,16 +6747,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
+    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6857,7 +6788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:9">
+    <row r="2" ht="29" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6886,7 +6817,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:9">
+    <row r="3" ht="29" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6920,39 +6851,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -7186,7 +7117,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
@@ -7309,7 +7240,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -7320,15 +7251,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:B9"/>
@@ -7336,16 +7267,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7403,7 +7334,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:11">
+    <row r="3" ht="43.5" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7443,35 +7374,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>119</v>
       </c>
@@ -7536,34 +7467,34 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
-    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="51.5454545454545" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="43.7272727272727" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="35.2727272727273" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="36.8181818181818" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="51.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="43.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="36.8181818181818" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7624,7 +7555,7 @@
         <v>78</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:14">
+    <row r="3" ht="29" spans="1:14">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -7677,35 +7608,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -7725,7 +7656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -7862,7 +7793,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -8043,7 +7974,7 @@
         <v>174</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>175</v>
       </c>
@@ -8104,7 +8035,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row r="24" s="1" customFormat="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -8126,37 +8057,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="46.8181818181818" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="51.4545454545455" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="53.3636363636364" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.8181818181818" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="31.4545454545455" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="29.9090909090909" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="46.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="51.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="53.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.9090909090909" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -8277,7 +8208,7 @@
         <v>198</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:20">
+    <row r="3" ht="29" spans="1:20">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8344,67 +8275,67 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:Q4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:Q4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R4">
@@ -8420,7 +8351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
@@ -8611,7 +8542,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -8864,7 +8795,7 @@
         <v>167</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -8925,7 +8856,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row r="24" s="1" customFormat="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -8947,39 +8878,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane activePane="topLeft" topLeftCell="R1" xSplit="18280"/>
+      <pane xSplit="18280" topLeftCell="R1" activePane="topLeft"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
-    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.4545454545455" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="43.6363636363636" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="38.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="40.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="37.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="43.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.1818181818182" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9097,7 +9028,7 @@
         <v>240</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:19">
+    <row r="3" ht="43.5" spans="1:19">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9165,59 +9096,59 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9233,12 +9164,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:19">
+    <row r="8" ht="29" spans="1:19">
       <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
@@ -9415,7 +9346,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -9656,7 +9587,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -9717,7 +9648,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row r="24" s="1" customFormat="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -9739,15 +9670,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -9755,20 +9686,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.8181818181818" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="52.6363636363636" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="54.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="51.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.6363636363636" collapsed="true"/>
-    <col min="12" max="15" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="52.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="58" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="39.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="43" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.1818181818182" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -9871,7 +9802,7 @@
         <v>197</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:17">
+    <row r="3" ht="43.5" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9937,55 +9868,55 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f ref="D4:J4" si="0" t="shared">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
+        <f t="shared" ref="D4:J4" si="0">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
+        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9993,12 +9924,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:17">
+    <row r="8" ht="29" spans="1:17">
       <c r="A8" s="25" t="s">
         <v>288</v>
       </c>
@@ -10051,7 +9982,7 @@
         <v>155</v>
       </c>
     </row>
-    <row ht="29" r="9" spans="1:17">
+    <row r="9" ht="29" spans="1:17">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -10210,7 +10141,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:1">
+    <row r="12" s="1" customFormat="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>160</v>
       </c>
@@ -10427,7 +10358,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:1">
+    <row r="17" s="1" customFormat="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>175</v>
       </c>
@@ -10488,7 +10419,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="25" s="1" spans="1:1">
+    <row r="25" s="1" customFormat="1" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>189</v>
       </c>
@@ -10510,41 +10441,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane activePane="topLeft" topLeftCell="T1" xSplit="18280"/>
+      <pane xSplit="18280" topLeftCell="T1" activePane="topLeft"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.2727272727273" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.5454545454545" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="43.7272727272727" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.5454545454545" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="30.9090909090909" collapsed="true"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.2727272727273" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="37.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="40.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="43.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.5454545454545" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="30.9090909090909" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10653,7 +10584,7 @@
         <v>236</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:18">
+    <row r="3" ht="43.5" spans="1:18">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10714,59 +10645,59 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:O4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <f t="shared" ref="B4:O4" si="0">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -10782,12 +10713,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:18">
+    <row r="8" ht="29" spans="1:18">
       <c r="A8" s="25" t="s">
         <v>144</v>
       </c>
@@ -10955,7 +10886,7 @@
         <v>159</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
@@ -11184,7 +11115,7 @@
         <v>174</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
@@ -11245,7 +11176,7 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row r="24" s="1" customFormat="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>189</v>
       </c>
@@ -11267,7 +11198,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
APIAAS - Test Tracking Coverage
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -4,32 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="10" activeTab="13"/>
+    <workbookView activeTab="14" firstSheet="10" windowHeight="7070" windowWidth="18530"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" sheetId="1" r:id="rId1"/>
-    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
-    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
-    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
-    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
-    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
-    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
-    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
-    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
-    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
-    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
-    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
-    <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
-    <sheet name="Tenant" sheetId="14" r:id="rId14"/>
-    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
-    <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
+    <sheet name="Register" r:id="rId1" sheetId="1"/>
+    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
+    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
+    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
+    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
+    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
+    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
+    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
+    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
+    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
+    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
+    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
+    <sheet name="IsiSaldo" r:id="rId13" sheetId="13"/>
+    <sheet name="Tenant" r:id="rId14" sheetId="14"/>
+    <sheet name="Saldo" r:id="rId15" sheetId="15"/>
+    <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="573">
   <si>
     <t>Status</t>
   </si>
@@ -1768,11 +1768,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1805,68 +1805,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1881,7 +1827,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1897,6 +1875,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1904,10 +1896,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1920,9 +1920,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1934,17 +1942,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1963,7 +1963,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1975,37 +2119,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2017,133 +2131,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2229,41 +2229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2275,30 +2240,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2326,267 +2267,326 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="5" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="12" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="11" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="11" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="22" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="33">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="7"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="177" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
+    <cellStyle builtinId="10" name="Note" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2600,10 +2600,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2767,21 +2767,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2798,7 +2798,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2851,9 +2851,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -2861,11 +2861,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="20.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="21.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2907,7 +2907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:7">
+    <row ht="43.5" r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2935,31 +2935,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -3193,19 +3193,19 @@
       <c r="C21" s="24"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C14:D14 F14:G14" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -3213,20 +3213,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="57.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="37.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="35.7272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.9090909090909" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="57.1818181818182" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="37.2727272727273" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3314,7 +3314,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:15">
+    <row ht="29" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3378,31 +3378,31 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
+        <f ref="E4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3422,12 +3422,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:15">
+    <row ht="29" r="8" spans="1:15">
       <c r="A8" s="25" t="s">
         <v>146</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>233</v>
       </c>
@@ -3859,15 +3859,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3875,18 +3875,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="35.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="35.3636363636364" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.6363636363636" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3941,7 +3941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:15">
+    <row ht="43.5" r="3" spans="1:15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4009,27 +4009,27 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
+        <f ref="F4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>233</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -4471,15 +4471,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView topLeftCell="I8" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
@@ -4487,20 +4487,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="42.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="35.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="42.4545454545455" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="35.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -4591,7 +4591,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:17">
+    <row ht="29" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4651,56 +4651,56 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:P4" si="0">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f ref="D4:P4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="25" t="s">
         <v>411</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>162</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="21" s="1" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>177</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="26" s="1" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>191</v>
       </c>
@@ -5255,18 +5255,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B9" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="B9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -5274,9 +5274,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="5" width="27" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7272727272727" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5313,7 +5313,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>Isiulang </v>
       </c>
     </row>
-    <row r="18" ht="29" spans="1:5">
+    <row ht="29" r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>446</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="19" s="1" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>449</v>
       </c>
@@ -5591,28 +5591,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="30.1818181818182" customWidth="1"/>
-    <col min="2" max="2" width="42.3636363636364" customWidth="1"/>
-    <col min="3" max="3" width="21.8181818181818" customWidth="1"/>
-    <col min="4" max="5" width="32.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="36.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="26.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.8181818181818" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="32.2727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5752,7 +5752,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="8" s="1" spans="1:7">
       <c r="A8" s="7" t="s">
         <v>464</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="11" s="1" spans="1:7">
       <c r="A11" s="7" t="s">
         <v>470</v>
       </c>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="17" s="1" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>483</v>
       </c>
@@ -5906,7 +5906,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" ht="29" spans="1:7">
+    <row ht="29" r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>484</v>
       </c>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="20" s="1" spans="1:7">
       <c r="A20" s="7" t="s">
         <v>488</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:7">
+    <row customFormat="1" r="24" s="1" spans="1:7">
       <c r="A24" s="7" t="s">
         <v>498</v>
       </c>
@@ -6032,7 +6032,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" ht="29" spans="1:7">
+    <row ht="29" r="27" spans="1:7">
       <c r="A27" s="6" t="s">
         <v>503</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="30" customFormat="1" spans="1:7">
+    <row customFormat="1" r="30" spans="1:7">
       <c r="A30" s="6" t="s">
         <v>510</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" spans="1:3">
+    <row customFormat="1" r="31" s="1" spans="1:3">
       <c r="A31" s="19" t="s">
         <v>512</v>
       </c>
@@ -6314,36 +6314,36 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
+      <formula1>"Edit, New"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10 E10 F10 G10">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10 E10 F10 G10" type="list">
       <formula1>"Active, Inactive"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10">
-      <formula1>"Edit, New"</formula1>
-    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.8181818181818" customWidth="1"/>
-    <col min="2" max="2" width="31.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="29.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="26.0909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.8181818181818" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.7272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.2727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.0909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6360,7 +6360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:4">
+    <row ht="43.5" r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>449</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="18" s="1" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>566</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="23" s="1" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>191</v>
       </c>
@@ -6559,22 +6559,22 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6582,8 +6582,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.6363636363636" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6619,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>570</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="10" s="1" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>571</v>
       </c>
@@ -6655,19 +6655,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list">
       <formula1>"PRODUCTION,TRIAL"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -6675,10 +6675,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6709,7 +6709,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:5">
+    <row ht="29" r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -6931,18 +6931,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C16" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="E5" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
@@ -6950,16 +6950,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="40.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6991,7 +6991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="29" spans="1:9">
+    <row ht="29" r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:9">
+    <row ht="29" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7054,39 +7054,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
@@ -7443,7 +7443,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -7454,15 +7454,15 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -7470,16 +7470,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="11.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7537,7 +7537,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="101.5" spans="1:11">
+    <row ht="101.5" r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7577,35 +7577,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+        <f si="0" t="shared"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>121</v>
       </c>
@@ -7670,19 +7670,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -7690,14 +7690,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="52.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="5" max="10" width="49.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="51.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="43.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="35.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="36.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="51.5454545454545" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="35.2727272727273" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="36.8181818181818" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7758,7 +7758,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:14">
+    <row ht="29" r="3" spans="1:14">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -7811,35 +7811,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -7859,7 +7859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>177</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -8260,15 +8260,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25:B26"/>
@@ -8276,21 +8276,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="49.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="45.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="42.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="48.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="46.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="49.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="46.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="51.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="53.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="29.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="46.8181818181818" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="51.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="53.3636363636364" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.8181818181818" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="31.4545454545455" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="29.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -8411,7 +8411,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" ht="29" spans="1:20">
+    <row ht="29" r="3" spans="1:20">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8478,67 +8478,67 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:Q4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f ref="B4:Q4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="R4">
@@ -8554,7 +8554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -8998,7 +8998,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>233</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -9081,39 +9081,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="R1" activePane="topLeft"/>
+      <pane activePane="topLeft" topLeftCell="R1" xSplit="18280"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="38.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="10" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="40.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="43.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.4545454545455" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="43.6363636363636" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9231,7 +9231,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:19">
+    <row ht="43.5" r="3" spans="1:19">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9299,59 +9299,59 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9367,12 +9367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:19">
+    <row ht="29" r="8" spans="1:19">
       <c r="A8" s="25" t="s">
         <v>146</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>233</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -9873,15 +9873,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -9889,20 +9889,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="52.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="54.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="58" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="51.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="12" max="15" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="43" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.1818181818182" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.8181818181818" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="54.6363636363636" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.6363636363636" collapsed="true"/>
+    <col min="12" max="15" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.1818181818182" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -10005,7 +10005,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:17">
+    <row ht="43.5" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10071,55 +10071,55 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:J4" si="0">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
+        <f ref="D4:J4" si="0" t="shared">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
+        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -10127,12 +10127,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:17">
+    <row ht="29" r="8" spans="1:17">
       <c r="A8" s="25" t="s">
         <v>290</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" ht="29" spans="1:17">
+    <row ht="29" r="9" spans="1:17">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -10344,7 +10344,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>162</v>
       </c>
@@ -10561,7 +10561,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>177</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="25" s="1" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>191</v>
       </c>
@@ -10644,41 +10644,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane xSplit="18280" topLeftCell="T1" activePane="topLeft"/>
+      <pane activePane="topLeft" topLeftCell="T1" xSplit="18280"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.3636363636364" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="37.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="39.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="40.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="43.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="30.9090909090909" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.2727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.5454545454545" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="37.4545454545455" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.0909090909091" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.7272727272727" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.5454545454545" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.9090909090909" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10787,7 +10787,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" ht="43.5" spans="1:18">
+    <row ht="43.5" r="3" spans="1:18">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10848,59 +10848,59 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:O4" si="0">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <f ref="B4:O4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -10916,12 +10916,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:18">
+    <row ht="29" r="8" spans="1:18">
       <c r="A8" s="25" t="s">
         <v>146</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>162</v>
       </c>
@@ -11318,7 +11318,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>233</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -11401,7 +11401,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testing done ready for code review
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{5C7B2374-3CB4-4778-A413-75A880C5892A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="10" windowHeight="7070" windowWidth="18530"/>
+    <workbookView activeTab="13" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="Register" r:id="rId1" sheetId="1"/>
@@ -24,12 +30,12 @@
     <sheet name="Saldo" r:id="rId15" sheetId="15"/>
     <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="584">
   <si>
     <t>Status</t>
   </si>
@@ -1469,9 +1475,6 @@
     <t>Roemah Finance</t>
   </si>
   <si>
-    <t>WWFINANCE</t>
-  </si>
-  <si>
     <t>$Status</t>
   </si>
   <si>
@@ -1496,9 +1499,6 @@
     <t>ESIGN/ADINS</t>
   </si>
   <si>
-    <t>WWF</t>
-  </si>
-  <si>
     <t>$LabelRefNumber</t>
   </si>
   <si>
@@ -1511,12 +1511,6 @@
     <t>API Key</t>
   </si>
   <si>
-    <t>kyP4ih</t>
-  </si>
-  <si>
-    <t>EfXHMQ</t>
-  </si>
-  <si>
     <t>Batas Saldo</t>
   </si>
   <si>
@@ -1785,25 +1779,49 @@
   </si>
   <si>
     <t>Tipe API KEY</t>
+  </si>
+  <si>
+    <t>OCR BPKB;Liveness Face Compare;Verifikasi Dukcapil Tanpa Biometrik;OTP</t>
+  </si>
+  <si>
+    <t>FZ34jV</t>
+  </si>
+  <si>
+    <t>;Submit Gagal</t>
+  </si>
+  <si>
+    <t>Gagal search karena nama tenant terdaftar tidak kapital</t>
+  </si>
+  <si>
+    <t>WIKY WILLIS COMPANY</t>
+  </si>
+  <si>
+    <t>o63JZ8</t>
+  </si>
+  <si>
+    <t>WWC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1828,27 +1846,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1856,123 +1853,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1985,194 +1867,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2252,274 +1948,30 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="19" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="13" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="12" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="7" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="22" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="4" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="7"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
     <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -2530,90 +1982,47 @@
     </xf>
     <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="8"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="10"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="11"/>
-    <cellStyle builtinId="10" name="Note" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2871,25 +2280,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0909090909091" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.8181818181818" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.4545454545455" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.5454545454545" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="21.9090909090909" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.08984375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="21.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2983,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3077,149 +2486,148 @@
         <v>29</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="23">
         <v>999999</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>1</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>2</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-    </row>
-    <row r="20" spans="1:1">
+    <row r="19" spans="1:7">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
   </ignoredErrors>
@@ -3227,30 +2635,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.9090909090909" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.90625" collapsed="true"/>
     <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="57.1818181818182" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="37.2727272727273" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.36328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.08984375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.54296875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="57.1796875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="37.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="36.54296875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="35.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3300,7 +2707,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3446,13 +2853,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:15">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3592,7 +2999,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -3785,12 +3192,12 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>241</v>
       </c>
@@ -3798,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>186</v>
       </c>
@@ -3806,7 +3213,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>188</v>
       </c>
@@ -3814,7 +3221,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -3822,7 +3229,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>192</v>
       </c>
@@ -3830,7 +3237,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -3838,7 +3245,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -3866,7 +3273,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>199</v>
       </c>
@@ -3874,7 +3281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>200</v>
       </c>
@@ -3884,33 +3291,31 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.81640625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="35.3636363636364" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.6363636363636" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.36328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.08984375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.54296875" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="35.36328125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3960,7 +3365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4073,13 +3478,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -4219,7 +3624,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -4412,7 +3817,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -4473,7 +3878,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -4496,36 +3901,34 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.8181818181818" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.81640625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="34.2727272727273" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.3636363636364" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="42.4545454545455" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="35.1818181818182" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="36.1818181818182" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.36328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.08984375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="42.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="45.1796875" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="35.1796875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="36.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4584,7 +3987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4709,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f ref="D4:P4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f ref="D4:N4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
@@ -4769,13 +4172,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:18">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>422</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -4834,55 +4237,55 @@
       <c r="A9" t="s">
         <v>423</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="M9" s="26" t="s">
+      <c r="M9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="N9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="O9" s="26" t="s">
+      <c r="O9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="P9" s="26" t="s">
+      <c r="P9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="Q9" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="R9" s="26" t="s">
+      <c r="R9" s="19" t="s">
         <v>424</v>
       </c>
     </row>
@@ -4890,55 +4293,55 @@
       <c r="A10" t="s">
         <v>427</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="20">
         <v>718325938613651</v>
       </c>
-      <c r="F10" s="28">
-        <v>8.71832593861365e+16</v>
-      </c>
-      <c r="G10" s="27">
+      <c r="F10" s="21">
+        <v>8.7183259386136496E+16</v>
+      </c>
+      <c r="G10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="N10" s="27">
+      <c r="N10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="O10" s="27">
+      <c r="O10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="P10" s="27">
+      <c r="P10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="Q10" s="27">
+      <c r="Q10" s="20">
         <v>7183259386136510</v>
       </c>
-      <c r="R10" s="27">
+      <c r="R10" s="20">
         <v>7183259386136510</v>
       </c>
     </row>
@@ -5002,55 +4405,55 @@
       <c r="A12" t="s">
         <v>431</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="L12" s="29" t="s">
+      <c r="L12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="N12" s="29" t="s">
+      <c r="N12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="O12" s="29" t="s">
+      <c r="O12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="Q12" s="29" t="s">
+      <c r="Q12" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="R12" s="29" t="s">
+      <c r="R12" s="22" t="s">
         <v>432</v>
       </c>
     </row>
@@ -5166,7 +4569,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:18">
       <c r="A16" s="2" t="s">
         <v>169</v>
       </c>
@@ -5395,12 +4798,12 @@
         <v>176</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:1">
+    <row customFormat="1" r="21" s="1" spans="1:18">
       <c r="A21" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -5408,7 +4811,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -5416,7 +4819,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>317</v>
       </c>
@@ -5424,7 +4827,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>318</v>
       </c>
@@ -5432,12 +4835,12 @@
         <v>193</v>
       </c>
     </row>
-    <row customFormat="1" r="26" s="1" spans="1:1">
+    <row customFormat="1" r="26" s="1" spans="1:18">
       <c r="A26" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>325</v>
       </c>
@@ -5445,7 +4848,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>326</v>
       </c>
@@ -5455,7 +4858,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <headerFooter/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="B9"/>
   </ignoredErrors>
@@ -5463,17 +4865,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7272727272727" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="18.7265625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
     <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
   </cols>
@@ -5550,7 +4951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -5657,7 +5058,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>450</v>
       </c>
@@ -5692,16 +5093,16 @@
       <c r="A16" t="s">
         <v>452</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="16">
         <v>1130</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="16">
         <v>1139</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="16">
         <v>1124</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="16">
         <v>1116</v>
       </c>
     </row>
@@ -5723,27 +5124,27 @@
       </c>
       <c r="E17" t="str">
         <f>CONCATENATE("Isiulang ",E14)</f>
-        <v>Isiulang </v>
+        <v xml:space="preserve">Isiulang </v>
       </c>
     </row>
     <row ht="29" r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:1">
+    <row customFormat="1" r="19" s="1" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>457</v>
       </c>
@@ -5752,19 +5153,19 @@
       <c r="A20" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="24" t="str">
+      <c r="B20" s="17" t="str">
         <f>B14</f>
         <v>IDR</v>
       </c>
-      <c r="C20" s="24" t="str">
+      <c r="C20" s="17" t="str">
         <f>C14</f>
         <v>OCR BPKB</v>
       </c>
-      <c r="D20" s="24" t="str">
+      <c r="D20" s="17" t="str">
         <f>D14</f>
         <v>OCR STNK</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="17">
         <f>E14</f>
         <v>0</v>
       </c>
@@ -5791,758 +5192,751 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.1818181818182" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.3636363636364" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.8181818181818" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="32.2727272727273" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="36.8181818181818" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.1818181818182" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.36328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.81640625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="32.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C2" t="s">
         <v>439</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>459</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+    <row ht="29" r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f>IF(C7="New",COUNTIFS($A$12:$A$23,"*$*",C12:C23,""),IF(C7="Service",COUNTIFS($A$9:$A$10,"*$*",C9:C10,""),IF(C7="Edit",COUNTIFS($A$9:$A$21,"*$*",C9:C21,""),0)))</f>
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>IF(D7="New",COUNTIFS($A$12:$A$23,"*$*",D12:D23,""),IF(D7="Service",COUNTIFS($A$9:$A$10,"*$*",D9:D10,""),IF(D7="Edit",COUNTIFS($A$9:$A$21,"*$*",D9:D21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f>IF(E7="New",COUNTIFS($A$12:$A$23,"*$*",E12:E23,""),IF(E7="Service",COUNTIFS($A$9:$A$10,"*$*",E9:E10,""),IF(E7="Edit",COUNTIFS($A$9:$A$21,"*$*",E9:E21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f>IF(F7="New",COUNTIFS($A$12:$A$23,"*$*",F12:F23,""),IF(F7="Service",COUNTIFS($A$9:$A$10,"*$*",F9:F10,""),IF(F7="Edit",COUNTIFS($A$9:$A$21,"*$*",F9:F21,""),0)))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>IF(G7="New",COUNTIFS($A$12:$A$23,"*$*",G12:G23,""),IF(G7="Service",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),IF(G7="Edit",COUNTIFS($A$9:$A$21,"*$*",G9:G21,""),IF(G7="ChargeType",COUNTIFS($A$9:$A$10,"*$*",G9:G10,""),0))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>471</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="1" spans="1:7">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="1" spans="1:7">
+      <c r="A11" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row customFormat="1" r="11" s="1" spans="1:7">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="B14" s="5">
+        <v>202304426</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>484</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
+        <v>202304277</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B16" t="s">
+        <v>578</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" t="s">
+        <v>582</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row customFormat="1" r="17" s="1" spans="1:7">
+      <c r="A17" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row ht="43.5" r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row customFormat="1" r="20" s="1" spans="1:7">
+      <c r="A20" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B21" t="s">
+        <v>494</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B22" t="s">
+        <v>497</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row customFormat="1" r="24" s="1" spans="1:7">
+      <c r="A24" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row ht="29" r="27" spans="1:7">
+      <c r="A27" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row customFormat="1" r="31" s="1" spans="1:7">
+      <c r="A31" s="27" t="s">
+        <v>516</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B14" s="10">
-        <v>202304426</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>486</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10">
-        <v>202304277</v>
-      </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="B16" t="s">
-        <v>489</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" t="s">
-        <v>490</v>
-      </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row customFormat="1" r="17" s="1" spans="1:7">
-      <c r="A17" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row ht="29" r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row customFormat="1" r="20" s="1" spans="1:7">
-      <c r="A20" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="B21" t="s">
-        <v>498</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="B22" t="s">
-        <v>501</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="G23" s="6"/>
-    </row>
-    <row customFormat="1" r="24" s="1" spans="1:7">
-      <c r="A24" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="6" t="s">
-        <v>507</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>508</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>510</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row ht="29" r="27" spans="1:7">
-      <c r="A27" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>515</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row customFormat="1" r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
+      <c r="B33" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>519</v>
       </c>
     </row>
-    <row customFormat="1" r="31" s="1" spans="1:3">
-      <c r="A31" s="19" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="B32" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="C33" s="6" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="5" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="C34" s="6" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="5" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="C35" s="6" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="5" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="5" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="6" t="s">
+      <c r="B39" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
+      <c r="B40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="6" t="s">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="6" t="s">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B43" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="6" t="s">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>546</v>
       </c>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="6" t="s">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="6" t="s">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="6" t="s">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="6" t="s">
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="6" t="s">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>556</v>
-      </c>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
-        <v>557</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="C52" s="6"/>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" s="22"/>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" s="22"/>
+      <c r="C53" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10 E10 F10 G10" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10:G10" type="list" xr:uid="{00000000-0002-0000-0D00-000001000000}">
       <formula1>"Active, Inactive"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list" xr:uid="{00000000-0002-0000-0D00-000002000000}">
       <formula1>"Edit, New"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.8181818181818" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.7272727272727" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.2727272727273" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.0909090909091" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6559,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6572,13 +5966,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>562</v>
+        <v>556</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6598,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>457</v>
       </c>
@@ -6617,9 +6011,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B9" t="s">
         <v>168</v>
@@ -6630,38 +6024,38 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>560</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>562</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>564</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>565</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>566</v>
-      </c>
-      <c r="B11" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>568</v>
-      </c>
-      <c r="B12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>569</v>
       </c>
       <c r="B13">
         <v>1234</v>
@@ -6670,9 +6064,9 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B14" t="str">
         <f>B8</f>
@@ -6681,19 +6075,19 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>571</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:3">
+        <v>567</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B16" t="s">
         <v>168</v>
@@ -6702,9 +6096,9 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:1">
+    <row customFormat="1" r="18" s="1" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -6735,20 +6129,20 @@
         <v>35</v>
       </c>
     </row>
-    <row customFormat="1" r="23" s="1" spans="1:1">
+    <row customFormat="1" r="23" s="1" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -6758,31 +6152,29 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list" xr:uid="{00000000-0002-0000-0E00-000001000000}">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.6363636363636" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6798,7 +6190,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6806,7 +6198,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6818,9 +6210,9 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6839,14 +6231,14 @@
         <v>55</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:1">
+    <row customFormat="1" r="10" s="1" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
@@ -6854,30 +6246,28 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>"PRODUCTION,TRIAL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.3636363636364" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.4545454545455" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.36328125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="40.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6888,7 +6278,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -6946,7 +6336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -7030,7 +6420,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -7048,16 +6438,16 @@
       <c r="A14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="16" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7082,16 +6472,16 @@
       <c r="A16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="16">
         <v>123456789012</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="16">
         <v>123456788012</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="16">
         <v>123456788012</v>
       </c>
     </row>
@@ -7116,22 +6506,21 @@
       <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="17" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="C16"/>
   </ignoredErrors>
@@ -7139,26 +6528,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="E5" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1818181818182" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.3636363636364" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.36328125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="27.9090909090909" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.8181818181818" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7272727272727" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.1818181818182" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="40.6363636363636" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.8181818181818" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.90625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.6328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.1796875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.6328125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7219,7 +6607,7 @@
         <v>86</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:9">
+    <row ht="43.5" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7285,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -7519,7 +6907,7 @@
         <v>117</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>119</v>
       </c>
@@ -7612,7 +7000,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="18" t="s">
         <v>123</v>
       </c>
       <c r="B20" t="s">
@@ -7642,7 +7030,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -7654,34 +7042,32 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4545454545455" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.7272727272727" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.3636363636364" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.36328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6328125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6363636363636" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.7272727272727" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="11.6363636363636" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="11.6328125" collapsed="true"/>
     <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7710,7 +7096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7767,7 +7153,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -7804,12 +7190,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -7838,7 +7224,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -7869,34 +7255,32 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="52.8181818181818" collapsed="true"/>
-    <col min="5" max="10" customWidth="true" width="49.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="51.5454545454545" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="43.7272727272727" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="35.2727272727273" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="36.8181818181818" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="45.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="52.81640625" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="49.1796875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="51.54296875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="43.7265625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="35.26953125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="36.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7943,7 +7327,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -8058,13 +7442,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" t="s">
@@ -8195,7 +7579,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -8376,7 +7760,7 @@
         <v>183</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>184</v>
       </c>
@@ -8437,7 +7821,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -8460,36 +7844,34 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.3636363636364" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="49.8181818181818" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" width="45.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="42.3636363636364" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="48.9090909090909" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="46.4545454545455" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="49.2727272727273" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="46.8181818181818" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="51.4545454545455" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="53.3636363636364" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.8181818181818" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="31.4545454545455" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="29.9090909090909" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.36328125" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="45.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.81640625" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="45.1796875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="42.36328125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="48.90625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="46.453125" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="49.26953125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="46.81640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="51.453125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="53.36328125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.81640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="31.453125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="29.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -8554,7 +7936,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -8610,7 +7992,7 @@
         <v>207</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:20">
+    <row ht="43.5" r="3" spans="1:20">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8753,13 +8135,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" t="s">
@@ -8944,7 +8326,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -9197,7 +8579,7 @@
         <v>176</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -9258,7 +8640,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -9281,38 +8663,36 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane activePane="topLeft" topLeftCell="R1" xSplit="18280"/>
+      <pane topLeftCell="R1" xSplit="18280"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.1818181818182" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.0909090909091" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.6363636363636" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="38.4545454545455" collapsed="true"/>
-    <col min="10" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.2727272727273" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.4545454545455" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="43.6363636363636" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="42.08984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.36328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="38.453125" collapsed="true"/>
+    <col min="10" max="13" customWidth="true" width="39.1796875" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.26953125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="37.54296875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.453125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="43.6328125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="34.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9374,7 +8754,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9566,13 +8946,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:19">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -9748,7 +9128,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:19">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -9989,7 +9369,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -10050,7 +9430,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -10073,35 +9453,33 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.8181818181818" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="52.6363636363636" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="54.6363636363636" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="54.6328125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="51.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0909090909091" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.5454545454545" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="35.7272727272727" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.6363636363636" collapsed="true"/>
-    <col min="12" max="15" customWidth="true" width="39.1818181818182" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="51.6328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.08984375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.6328125" collapsed="true"/>
+    <col min="12" max="15" customWidth="true" width="39.1796875" collapsed="true"/>
     <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.1818181818182" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -10157,7 +9535,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10204,7 +9582,7 @@
         <v>206</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:17">
+    <row ht="58" r="3" spans="1:17">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10326,13 +9704,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:17">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:17">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>297</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -10543,7 +9921,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:1">
+    <row customFormat="1" r="12" s="1" spans="1:17">
       <c r="A12" s="2" t="s">
         <v>169</v>
       </c>
@@ -10760,7 +10138,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:1">
+    <row customFormat="1" r="17" s="1" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>184</v>
       </c>
@@ -10821,7 +10199,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="25" s="1" spans="1:1">
+    <row customFormat="1" r="25" s="1" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>198</v>
       </c>
@@ -10844,40 +10222,38 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane activePane="topLeft" topLeftCell="T1" xSplit="18280"/>
+      <pane topLeftCell="T1" xSplit="18280"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.3636363636364" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.2727272727273" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.1818181818182" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.5454545454545" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.5454545454545" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6363636363636" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.3636363636364" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="37.4545454545455" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="39.1818181818182" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.0909090909091" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="43.7272727272727" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.5454545454545" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="30.9090909090909" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.6328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.36328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="40.08984375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.1796875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="37.453125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="40.08984375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="39.1796875" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="40.08984375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="43.7265625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="34.54296875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10936,7 +10312,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11115,13 +10491,13 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:1">
+    <row customFormat="1" r="7" s="1" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:18">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -11288,7 +10664,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:1">
+    <row customFormat="1" r="11" s="1" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -11517,7 +10893,7 @@
         <v>183</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:1">
+    <row customFormat="1" r="16" s="1" spans="1:18">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -11578,7 +10954,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:1">
+    <row customFormat="1" r="24" s="1" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -11601,6 +10977,5 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Codacy Review for Keywords
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{5C7B2374-3CB4-4778-A413-75A880C5892A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AE9ABF71-1854-4D2D-9A49-8CEAA8D3790F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView activeTab="11" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="Register" r:id="rId1" sheetId="1"/>
@@ -1809,19 +1809,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1951,14 +1944,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -1966,12 +1959,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
     <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -1988,7 +1981,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -2000,14 +1993,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3908,8 +3900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -5199,7 +5191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -5689,11 +5681,11 @@
       </c>
     </row>
     <row customFormat="1" r="31" s="1" spans="1:7">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>516</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">

</xml_diff>

<commit_message>
Codacy Review for Keywords + 3/4 TC
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{AE9ABF71-1854-4D2D-9A49-8CEAA8D3790F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7731B7-E072-4364-A199-FD7524EA2385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" r:id="rId1" sheetId="1"/>
-    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
-    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
-    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
-    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
-    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
-    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
-    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
-    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
-    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
-    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
-    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
-    <sheet name="IsiSaldo" r:id="rId13" sheetId="13"/>
-    <sheet name="Tenant" r:id="rId14" sheetId="14"/>
-    <sheet name="Saldo" r:id="rId15" sheetId="15"/>
-    <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
+    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
+    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
+    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
+    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
+    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
+    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
+    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
+    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
+    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
+    <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
+    <sheet name="Tenant" sheetId="14" r:id="rId14"/>
+    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
+    <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="584">
   <si>
     <t>Status</t>
   </si>
@@ -1943,72 +1943,72 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="29">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2025,10 +2025,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2192,21 +2192,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2223,7 +2223,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2277,8 +2277,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -2286,11 +2286,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.08984375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="21.90625" collapsed="true"/>
+    <col min="1" max="1" width="20.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="21.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2332,7 +2332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2360,31 +2360,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:G4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:G4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:7">
+    <row r="12" spans="1:7" s="1" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:7">
+    <row r="17" spans="1:7" s="1" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -2618,17 +2618,17 @@
       <c r="C21" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="F14:G14 C14:D14"/>
+    <ignoredError sqref="F14:G14 C14:D14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -2636,20 +2636,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.90625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.36328125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.08984375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="57.1796875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="37.26953125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="35.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.90625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.36328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.08984375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="57.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="37.26953125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="35.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2737,7 +2737,7 @@
         <v>206</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="29">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2801,31 +2801,31 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f ref="E4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
+        <f t="shared" ref="E4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",E8:E21,"")</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -2845,12 +2845,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:15">
+    <row r="7" spans="1:15" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="29">
       <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:15">
+    <row r="11" spans="1:15" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:15">
+    <row r="16" spans="1:15" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -3282,13 +3282,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:P26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3296,18 +3296,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="34.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.36328125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.08984375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="35.36328125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.6328125" collapsed="true"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="34.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.36328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.08984375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="35.36328125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.6328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3362,7 +3362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3430,27 +3430,27 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f ref="F4:K4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
+        <f t="shared" ref="F4:K4" si="0">COUNTIFS($A$8:$A$21,"*$*",F8:F21,"")</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3470,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:15">
+    <row r="7" spans="1:15" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:15">
+    <row r="11" spans="1:15" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:15">
+    <row r="16" spans="1:15" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:2">
+    <row r="24" spans="1:2" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -3892,35 +3892,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:S28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="34.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.36328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.08984375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="42.453125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="45.1796875" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="35.1796875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="36.1796875" collapsed="true"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.36328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.08984375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="42.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.1796875" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="35.1796875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="36.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4035,7 +4035,7 @@
         <v>86</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="29">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -4104,47 +4104,47 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f ref="D4:N4" si="0" t="shared">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
+        <f t="shared" ref="D4:N4" si="0">COUNTIFS($A$8:$A$38,"*$*",D8:D38,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
@@ -4164,12 +4164,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:18">
+    <row r="7" spans="1:18" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="29">
       <c r="A8" s="18" t="s">
         <v>422</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:18">
+    <row r="16" spans="1:18" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>169</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>176</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:18">
+    <row r="21" spans="1:18" s="1" customFormat="1">
       <c r="A21" s="2" t="s">
         <v>184</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>193</v>
       </c>
     </row>
-    <row customFormat="1" r="26" s="1" spans="1:18">
+    <row r="26" spans="1:18" s="1" customFormat="1">
       <c r="A26" s="2" t="s">
         <v>198</v>
       </c>
@@ -4849,16 +4849,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="B9"/>
+    <ignoredError sqref="B9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -4866,9 +4866,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="27" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4905,7 +4905,7 @@
         <v>439</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="29">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:5">
+    <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v xml:space="preserve">Isiulang </v>
       </c>
     </row>
-    <row ht="29" r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="29">
       <c r="A18" s="3" t="s">
         <v>454</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>456</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:5">
+    <row r="19" spans="1:5" s="1" customFormat="1">
       <c r="A19" s="2" t="s">
         <v>457</v>
       </c>
@@ -5183,13 +5183,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:H53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -5197,12 +5197,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.1796875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.36328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.81640625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="32.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="36.81640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.1796875" collapsed="true"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="32.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5251,7 +5251,7 @@
         <v>460</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="29">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>471</v>
       </c>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:7">
+    <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="6" t="s">
         <v>472</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>476</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:7">
+    <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="6" t="s">
         <v>477</v>
       </c>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:7">
+    <row r="17" spans="1:7" s="1" customFormat="1">
       <c r="A17" s="6" t="s">
         <v>487</v>
       </c>
@@ -5498,7 +5498,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row ht="43.5" r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="43.5">
       <c r="A18" s="5" t="s">
         <v>488</v>
       </c>
@@ -5528,7 +5528,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:7">
+    <row r="20" spans="1:7" s="1" customFormat="1">
       <c r="A20" s="6" t="s">
         <v>492</v>
       </c>
@@ -5584,7 +5584,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:7">
+    <row r="24" spans="1:7" s="1" customFormat="1">
       <c r="A24" s="6" t="s">
         <v>502</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="11"/>
     </row>
-    <row ht="29" r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="29">
       <c r="A27" s="5" t="s">
         <v>507</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>515</v>
       </c>
     </row>
-    <row customFormat="1" r="31" s="1" spans="1:7">
+    <row r="31" spans="1:7" s="1" customFormat="1">
       <c r="A31" s="26" t="s">
         <v>516</v>
       </c>
@@ -5900,24 +5900,24 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:G7" type="list" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:G7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>"Edit, Service, New,ChargeType"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10 D10:G10" type="list" xr:uid="{00000000-0002-0000-0D00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 D10:G10" xr:uid="{00000000-0002-0000-0D00-000001000000}">
       <formula1>"Active, Inactive"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C9:C10" type="list" xr:uid="{00000000-0002-0000-0D00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10" xr:uid="{00000000-0002-0000-0D00-000002000000}">
       <formula1>"Edit, New"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -5925,10 +5925,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.08984375" collapsed="true"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5953,7 +5953,7 @@
         <v>459</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:4">
+    <row r="7" spans="1:4" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>457</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:4">
+    <row r="18" spans="1:4" s="1" customFormat="1">
       <c r="A18" s="2" t="s">
         <v>570</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row customFormat="1" r="23" s="1" spans="1:4">
+    <row r="23" spans="1:4" s="1" customFormat="1">
       <c r="A23" s="2" t="s">
         <v>198</v>
       </c>
@@ -6144,20 +6144,20 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 C12 D12" type="list" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16 C16 D16" type="list" xr:uid="{00000000-0002-0000-0E00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16" xr:uid="{00000000-0002-0000-0E00-000001000000}">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6165,8 +6165,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.6328125" collapsed="true"/>
+    <col min="1" max="1" width="20.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.6328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6202,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:2">
+    <row r="7" spans="1:2" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>574</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>55</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:2">
+    <row r="10" spans="1:2" s="1" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>575</v>
       </c>
@@ -6238,17 +6238,17 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>"PRODUCTION,TRIAL"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -6256,10 +6256,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.36328125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="40.6328125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.453125" collapsed="true"/>
+    <col min="1" max="1" width="20.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="40.6328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6290,7 +6290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="29">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:5">
+    <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -6512,33 +6512,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C16"/>
+    <ignoredError sqref="C16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1796875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="27.90625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.81640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7265625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.6328125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.1796875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="40.6328125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.81640625" collapsed="true"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.90625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7265625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.6328125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.1796875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40.6328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6546,7 +6546,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -6570,13 +6570,10 @@
         <v>1</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="29">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>85</v>
       </c>
@@ -6599,7 +6596,7 @@
         <v>86</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6633,39 +6630,39 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
+        <f t="shared" ref="B4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",B8:B22,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -6899,7 +6896,7 @@
         <v>117</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:9">
+    <row r="16" spans="1:9" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>119</v>
       </c>
@@ -7022,7 +7019,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21:K21" type="list" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:K21" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,
 OCR REK KORAN BCA
 ,OCR STNK,
@@ -7033,12 +7030,12 @@
 "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7047,16 +7044,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.6328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.36328125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.6328125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6328125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="11.6328125" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="20.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.36328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="11.6328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7114,7 +7111,7 @@
         <v>86</v>
       </c>
     </row>
-    <row ht="101.5" r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="101.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7154,35 +7151,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:I4" si="0" t="shared">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
+        <f t="shared" ref="C4:I4" si="0">COUNTIFS($A$8:$A$22,"*$*",C8:C22,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>128</v>
       </c>
@@ -7247,17 +7244,17 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:L8" type="list" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:L8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"OCR BPKB,OCR REK KORAN MANDIRI,LIVENESS + FACECOMPARE,OCR KK,OCR REK KORAN BCA,OCR STNK,FACECOMPARE,OCR KTP,OCR NPWP,LIVENESS"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -7265,14 +7262,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="45.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="52.81640625" collapsed="true"/>
-    <col min="5" max="10" customWidth="true" width="49.1796875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="51.54296875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="43.7265625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="35.26953125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="36.81640625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="45.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52.81640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="49.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="51.54296875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="43.7265625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.26953125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="36.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7333,7 +7330,7 @@
         <v>86</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="29">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -7386,35 +7383,35 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -7434,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:14">
+    <row r="7" spans="1:14" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
@@ -7571,7 +7568,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:14">
+    <row r="11" spans="1:14" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -7752,7 +7749,7 @@
         <v>183</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:14">
+    <row r="16" spans="1:14" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>184</v>
       </c>
@@ -7813,7 +7810,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:2">
+    <row r="24" spans="1:2" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -7835,12 +7832,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7849,21 +7846,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.36328125" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="45.1796875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="49.81640625" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" width="45.1796875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="42.36328125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="48.90625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="46.453125" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="49.26953125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="46.81640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="51.453125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="53.36328125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.81640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="31.453125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="29.90625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="45.1796875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="45.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="42.36328125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="48.90625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="46.453125" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="49.26953125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="46.81640625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="51.453125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="53.36328125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.81640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.453125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7984,7 +7981,7 @@
         <v>207</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:20">
+    <row r="3" spans="1:20" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8051,67 +8048,67 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:Q4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
+        <f t="shared" ref="B4:Q4" si="0">COUNTIFS($A$8:$A$20,"*$*",B8:B20,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R4">
@@ -8127,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:20">
+    <row r="7" spans="1:20" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
@@ -8318,7 +8315,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:20">
+    <row r="11" spans="1:20" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -8571,7 +8568,7 @@
         <v>176</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:20">
+    <row r="16" spans="1:20" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -8632,7 +8629,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:2">
+    <row r="24" spans="1:2" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -8654,37 +8651,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:T26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane topLeftCell="R1" xSplit="18280"/>
+      <pane xSplit="18280" topLeftCell="R1"/>
       <selection activeCell="R13" sqref="R13"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.08984375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.6328125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.36328125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="38.453125" collapsed="true"/>
-    <col min="10" max="13" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.26953125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="37.54296875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.453125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="43.6328125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.08984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.6328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.6328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.36328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="38.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="40.26953125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="37.54296875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.453125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="43.6328125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -8802,7 +8799,7 @@
         <v>249</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8870,59 +8867,59 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f ref="C4:J4" si="0" t="shared">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
+        <f t="shared" ref="C4:J4" si="0">COUNTIFS($A$8:$A$20,"*$*",C8:C20,"")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
+        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$20,"*$*",K8:K20,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -8938,12 +8935,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:19">
+    <row r="7" spans="1:19" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:19">
+    <row r="8" spans="1:19" ht="29">
       <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
@@ -9120,7 +9117,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:19">
+    <row r="11" spans="1:19" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -9361,7 +9358,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:19">
+    <row r="16" spans="1:19" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -9422,7 +9419,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:2">
+    <row r="24" spans="1:2" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -9444,13 +9441,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:R27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -9458,20 +9455,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="52.6328125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="54.6328125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="58.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="51.6328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.08984375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="35.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.6328125" collapsed="true"/>
-    <col min="12" max="15" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.1796875" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="52.6328125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.6328125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="58" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.6328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.08984375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.7265625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.6328125" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="43" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -9574,7 +9571,7 @@
         <v>206</v>
       </c>
     </row>
-    <row ht="58" r="3" spans="1:17">
+    <row r="3" spans="1:17" ht="58">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9640,55 +9637,55 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f ref="D4:J4" si="0" t="shared">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
+        <f t="shared" ref="D4:J4" si="0">COUNTIFS($A$8:$A$37,"*$*",D8:D37,"")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f ref="K4:P4" si="1" t="shared">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
+        <f t="shared" ref="K4:P4" si="1">COUNTIFS($A$8:$A$37,"*$*",K8:K37,"")</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f si="1" t="shared"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4">
@@ -9696,12 +9693,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:17">
+    <row r="7" spans="1:17" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:17">
+    <row r="8" spans="1:17" ht="29">
       <c r="A8" s="18" t="s">
         <v>297</v>
       </c>
@@ -9754,7 +9751,7 @@
         <v>164</v>
       </c>
     </row>
-    <row ht="29" r="9" spans="1:17">
+    <row r="9" spans="1:17" ht="29">
       <c r="A9" t="s">
         <v>309</v>
       </c>
@@ -9913,7 +9910,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:17">
+    <row r="12" spans="1:17" s="1" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>169</v>
       </c>
@@ -10130,7 +10127,7 @@
         <v>178</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:2">
+    <row r="17" spans="1:2" s="1" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>184</v>
       </c>
@@ -10191,7 +10188,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="25" s="1" spans="1:2">
+    <row r="25" spans="1:2" s="1" customFormat="1">
       <c r="A25" s="2" t="s">
         <v>198</v>
       </c>
@@ -10213,39 +10210,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:S26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane topLeftCell="T1" xSplit="18280"/>
+      <pane xSplit="18280" topLeftCell="T1"/>
       <selection activeCell="S9" sqref="S9"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="37.6328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.36328125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="40.08984375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="37.453125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="40.08984375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="40.08984375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="43.7265625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="30.90625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.26953125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.6328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.36328125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.08984375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="37.453125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.08984375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="40.08984375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="43.7265625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="30.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10354,7 +10351,7 @@
         <v>245</v>
       </c>
     </row>
-    <row ht="43.5" r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="43.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10415,59 +10412,59 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f ref="B4:O4" si="0" t="shared">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
+        <f t="shared" ref="B4:O4" si="0">COUNTIFS($A$8:$A$21,"*$*",B8:B21,"")</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -10483,12 +10480,12 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:18">
+    <row r="7" spans="1:18" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="29">
       <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
@@ -10656,7 +10653,7 @@
         <v>168</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:18">
+    <row r="11" spans="1:18" s="1" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -10885,7 +10882,7 @@
         <v>183</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:18">
+    <row r="16" spans="1:18" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -10946,7 +10943,7 @@
         <v>197</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:2">
+    <row r="24" spans="1:2" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>198</v>
       </c>
@@ -10968,6 +10965,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
APIAAS - User Management - Role Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7731B7-E072-4364-A199-FD7524EA2385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706B954-B6A1-49FB-9EB9-85218EF53422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -29,13 +29,14 @@
     <sheet name="Tenant" sheetId="14" r:id="rId14"/>
     <sheet name="Saldo" sheetId="15" r:id="rId15"/>
     <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
+    <sheet name="Role" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="621">
   <si>
     <t>Status</t>
   </si>
@@ -1253,6 +1254,519 @@
     <t>OCR Rek. Koran BCA</t>
   </si>
   <si>
+    <t>Success, semua parameter terpenuhi dan valid</t>
+  </si>
+  <si>
+    <t>Success tanpa parameter optional</t>
+  </si>
+  <si>
+    <t>Fullname menggunakan nama bebas</t>
+  </si>
+  <si>
+    <t>IDnumber kurang dari 16 digit</t>
+  </si>
+  <si>
+    <t>IDNumber lebih dari 16 digit</t>
+  </si>
+  <si>
+    <t>Nomor telepon kurang dari 11 digit(9)</t>
+  </si>
+  <si>
+    <t>Nomor telepon lebih dari 11 digit (13)</t>
+  </si>
+  <si>
+    <t>Isi tanggal lahir dengan format hari yang salah</t>
+  </si>
+  <si>
+    <t>Isi tanggal lahir dengan format bulan yang salah</t>
+  </si>
+  <si>
+    <t>Isi tanggal lahir dengan format tahun yang salah</t>
+  </si>
+  <si>
+    <t>Hit menggunakan tenant code yang salah</t>
+  </si>
+  <si>
+    <t>Hit menggunakan tenant key yang salah</t>
+  </si>
+  <si>
+    <t>$selfiephoto</t>
+  </si>
+  <si>
+    <t>$mobilephone</t>
+  </si>
+  <si>
+    <t>+62812345678</t>
+  </si>
+  <si>
+    <t>+628123456</t>
+  </si>
+  <si>
+    <t>+6281234567835</t>
+  </si>
+  <si>
+    <t>$idNumber</t>
+  </si>
+  <si>
+    <t>$fullName</t>
+  </si>
+  <si>
+    <t>UserGDAB</t>
+  </si>
+  <si>
+    <t>User1234</t>
+  </si>
+  <si>
+    <t>$tanggalLahir</t>
+  </si>
+  <si>
+    <t>1980-01-01</t>
+  </si>
+  <si>
+    <t>1980-01-1</t>
+  </si>
+  <si>
+    <t>1980-1-01</t>
+  </si>
+  <si>
+    <t>980-01-01</t>
+  </si>
+  <si>
+    <t>Verifikasi Identitas Dukcapil</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Success tambah saldo IDR</t>
+  </si>
+  <si>
+    <t>Success tambah saldo OCR KTP</t>
+  </si>
+  <si>
+    <t>Success tambah saldo OCR KK</t>
+  </si>
+  <si>
+    <t>Gagal topup karena tipe saldo kosong</t>
+  </si>
+  <si>
+    <t>$Username Billing</t>
+  </si>
+  <si>
+    <t>ADMESIGN</t>
+  </si>
+  <si>
+    <t>$Password Billing</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>$Tenant</t>
+  </si>
+  <si>
+    <t>$Vendor</t>
+  </si>
+  <si>
+    <t>$Tipe Saldo</t>
+  </si>
+  <si>
+    <t>$Tambah Saldo</t>
+  </si>
+  <si>
+    <t>$Nomor tagihan</t>
+  </si>
+  <si>
+    <t>$Catatan</t>
+  </si>
+  <si>
+    <t>$Tanggal Pembelian (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Filter Saldo</t>
+  </si>
+  <si>
+    <t>Reason Failed</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Success create tenant</t>
+  </si>
+  <si>
+    <t>Mandatory tidak lengkap</t>
+  </si>
+  <si>
+    <t>Success edit services</t>
+  </si>
+  <si>
+    <t>Success Edit Tenant</t>
+  </si>
+  <si>
+    <t>Success ubah charge type</t>
+  </si>
+  <si>
+    <t>Is Mandatory Complete</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>ChargeType</t>
+  </si>
+  <si>
+    <t>Search Tenant</t>
+  </si>
+  <si>
+    <t>$NamaTenant</t>
+  </si>
+  <si>
+    <t>Roemah Finance</t>
+  </si>
+  <si>
+    <t>$Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Tenant</t>
+  </si>
+  <si>
+    <t>Sumber Jaya Makmur Finance</t>
+  </si>
+  <si>
+    <t>WOM Finance</t>
+  </si>
+  <si>
+    <t>$KodeTenant</t>
+  </si>
+  <si>
+    <t>SJM</t>
+  </si>
+  <si>
+    <t>ESIGN/ADINS</t>
+  </si>
+  <si>
+    <t>$LabelRefNumber</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>Auto Generate API Key</t>
+  </si>
+  <si>
+    <t>API Key</t>
+  </si>
+  <si>
+    <t>Batas Saldo</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>OCR BPKB;Liveness Face Compare;Verifikasi Dukcapil Tanpa Biometrik;Id Forgery</t>
+  </si>
+  <si>
+    <t>200;300;400;100</t>
+  </si>
+  <si>
+    <t>100;200;300;400</t>
+  </si>
+  <si>
+    <t>Penerima Email Reminder</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>williswy@ad-ins.com;williswy@gmail.com</t>
+  </si>
+  <si>
+    <t>wwf@ad-ins.com;wwf@gmail.com</t>
+  </si>
+  <si>
+    <t>$Email User Admin</t>
+  </si>
+  <si>
+    <t>williswy@ad-ins.com</t>
+  </si>
+  <si>
+    <t>wwf@ad-ins.com</t>
+  </si>
+  <si>
+    <t>$Kode Akses User Admin</t>
+  </si>
+  <si>
+    <t>password1111</t>
+  </si>
+  <si>
+    <t>password1234</t>
+  </si>
+  <si>
+    <t>Services Setting</t>
+  </si>
+  <si>
+    <t>ServicesCheck</t>
+  </si>
+  <si>
+    <t>OTP;DOC;SDT;SMS</t>
+  </si>
+  <si>
+    <t>VendorCheck</t>
+  </si>
+  <si>
+    <t>DJP;ESG;INDR;DIGI</t>
+  </si>
+  <si>
+    <t>ServicesUncheck</t>
+  </si>
+  <si>
+    <t>OCR_KTP;OCR_REKKORAN_BCA;OCR_REKKORAN_MANDIRI;OCR_STNK</t>
+  </si>
+  <si>
+    <t>VendorUncheck</t>
+  </si>
+  <si>
+    <t>VIDA;VIDA;ESG;DIGI</t>
+  </si>
+  <si>
+    <t>ESG;ESG;ESG;ESG</t>
+  </si>
+  <si>
+    <t>Balance ChargeType Check</t>
+  </si>
+  <si>
+    <t>OCR_KTP;OCR_NPWP</t>
+  </si>
+  <si>
+    <t>Balance ChargeType Uncheck</t>
+  </si>
+  <si>
+    <t>OCR_KK;DOC</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>DJP</t>
+  </si>
+  <si>
+    <t>VRF</t>
+  </si>
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>INDR</t>
+  </si>
+  <si>
+    <t>DUKCAPIL_NOBIO</t>
+  </si>
+  <si>
+    <t>Verifikasi Dukcapil Tanpa Biometrik</t>
+  </si>
+  <si>
+    <t>ESG</t>
+  </si>
+  <si>
+    <t>OCR_BUKU_TABUNGAN_MANDIRI</t>
+  </si>
+  <si>
+    <t>OCR BUKU TABUNGAN MANDIRI</t>
+  </si>
+  <si>
+    <t>DIGI</t>
+  </si>
+  <si>
+    <t>OCR_KTP</t>
+  </si>
+  <si>
+    <t>OCR_NPWP</t>
+  </si>
+  <si>
+    <t>OCR NPWP</t>
+  </si>
+  <si>
+    <t>OCR_BPKB</t>
+  </si>
+  <si>
+    <t>OCR_KK</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>SMS Notif</t>
+  </si>
+  <si>
+    <t>SDT</t>
+  </si>
+  <si>
+    <t>Stamp Duty</t>
+  </si>
+  <si>
+    <t>OCR_STNK</t>
+  </si>
+  <si>
+    <t>LIVENESS_FACECOMPARE</t>
+  </si>
+  <si>
+    <t>Liveness Face Compare</t>
+  </si>
+  <si>
+    <t>CDE</t>
+  </si>
+  <si>
+    <t>Credit Decision Engine</t>
+  </si>
+  <si>
+    <t>VALIDASI_SAMSAT</t>
+  </si>
+  <si>
+    <t>Validasi Samsat</t>
+  </si>
+  <si>
+    <t>FACE_COMPARE</t>
+  </si>
+  <si>
+    <t>Face Compare</t>
+  </si>
+  <si>
+    <t>LIVENESS</t>
+  </si>
+  <si>
+    <t>Liveness</t>
+  </si>
+  <si>
+    <t>ROBO_SLIK</t>
+  </si>
+  <si>
+    <t>Robot Slik</t>
+  </si>
+  <si>
+    <t>IDFORGERY_OCRKTP</t>
+  </si>
+  <si>
+    <t>ID Forgery + OCR KTP</t>
+  </si>
+  <si>
+    <t>ID_FORGERY</t>
+  </si>
+  <si>
+    <t>ID Forgery</t>
+  </si>
+  <si>
+    <t>DUKCAPIL_VIDA</t>
+  </si>
+  <si>
+    <t>Success search with all criteria and all function active</t>
+  </si>
+  <si>
+    <t>Success search dengan field pengguna dan nama dokumen tidak terisi</t>
+  </si>
+  <si>
+    <t>Success search dengan mengisi field mandatory saja</t>
+  </si>
+  <si>
+    <t>Tipe Transaksi</t>
+  </si>
+  <si>
+    <t>Tanggal Transaksi Dari</t>
+  </si>
+  <si>
+    <t>2023-05-01</t>
+  </si>
+  <si>
+    <t>Pengguna</t>
+  </si>
+  <si>
+    <t>ADMIN ESIGN</t>
+  </si>
+  <si>
+    <t>Hasil Proses</t>
+  </si>
+  <si>
+    <t>Ref Number</t>
+  </si>
+  <si>
+    <t>Nama Dokumen</t>
+  </si>
+  <si>
+    <t>Tanggal Transaksi hingga</t>
+  </si>
+  <si>
+    <t>2023-05-03</t>
+  </si>
+  <si>
+    <t>Kantor</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Success verifikasi</t>
+  </si>
+  <si>
+    <t>Data Login</t>
+  </si>
+  <si>
+    <t>API KEY controller</t>
+  </si>
+  <si>
+    <t>Tipe API KEY</t>
+  </si>
+  <si>
+    <t>OCR BPKB;Liveness Face Compare;Verifikasi Dukcapil Tanpa Biometrik;OTP</t>
+  </si>
+  <si>
+    <t>Gagal search karena nama tenant terdaftar tidak kapital</t>
+  </si>
+  <si>
+    <t>WIKY WILLIS COMPANY</t>
+  </si>
+  <si>
+    <t>WWC</t>
+  </si>
+  <si>
+    <t>kEZDJp</t>
+  </si>
+  <si>
+    <t>-;Submit Gagal</t>
+  </si>
+  <si>
+    <t>-;Mandatory is incomplete</t>
+  </si>
+  <si>
+    <t>-;Fungsi pencarian gagal, no result</t>
+  </si>
+  <si>
+    <t>apV55o</t>
+  </si>
+  <si>
+    <t>;FailedStoreDB</t>
+  </si>
+  <si>
     <t>;ID Number length must be 16</t>
   </si>
   <si>
@@ -1265,103 +1779,7 @@
     <t>;selfiePhoto</t>
   </si>
   <si>
-    <t>Success, semua parameter terpenuhi dan valid</t>
-  </si>
-  <si>
-    <t>Success tanpa parameter optional</t>
-  </si>
-  <si>
-    <t>Fullname menggunakan nama bebas</t>
-  </si>
-  <si>
-    <t>IDnumber kurang dari 16 digit</t>
-  </si>
-  <si>
-    <t>IDNumber lebih dari 16 digit</t>
-  </si>
-  <si>
-    <t>Nomor telepon kurang dari 11 digit(9)</t>
-  </si>
-  <si>
-    <t>Nomor telepon lebih dari 11 digit (13)</t>
-  </si>
-  <si>
-    <t>Isi tanggal lahir dengan format hari yang salah</t>
-  </si>
-  <si>
-    <t>Isi tanggal lahir dengan format bulan yang salah</t>
-  </si>
-  <si>
-    <t>Isi tanggal lahir dengan format tahun yang salah</t>
-  </si>
-  <si>
-    <t>Hit menggunakan tenant code yang salah</t>
-  </si>
-  <si>
-    <t>Hit menggunakan tenant key yang salah</t>
-  </si>
-  <si>
-    <t>Hit tidak menggunakan foto melainkan file text</t>
-  </si>
-  <si>
-    <t>Failed menggunakan foto blur</t>
-  </si>
-  <si>
-    <t>Failed menggunakan foto dengan resolusi rendah</t>
-  </si>
-  <si>
-    <t>Failed menggunakan foto putih bersih</t>
-  </si>
-  <si>
-    <t>Failed menggunakan foto dengan resolusi terlalu tinggi</t>
-  </si>
-  <si>
-    <t>$selfiephoto</t>
-  </si>
-  <si>
-    <t>$mobilephone</t>
-  </si>
-  <si>
-    <t>+62812345678</t>
-  </si>
-  <si>
-    <t>+628123456</t>
-  </si>
-  <si>
-    <t>+6281234567835</t>
-  </si>
-  <si>
-    <t>$idNumber</t>
-  </si>
-  <si>
-    <t>$fullName</t>
-  </si>
-  <si>
-    <t>UserGDAB</t>
-  </si>
-  <si>
-    <t>User1234</t>
-  </si>
-  <si>
-    <t>$tanggalLahir</t>
-  </si>
-  <si>
-    <t>1980-01-01</t>
-  </si>
-  <si>
-    <t>1980-01-1</t>
-  </si>
-  <si>
-    <t>1980-1-01</t>
-  </si>
-  <si>
-    <t>980-01-01</t>
-  </si>
-  <si>
-    <t>Verifikasi Identitas Dukcapil</t>
-  </si>
-  <si>
-    <t>CF</t>
+    <t>2023-05-16</t>
   </si>
   <si>
     <t>;Done well</t>
@@ -1370,436 +1788,130 @@
     <t>;Mandatory is incomplete</t>
   </si>
   <si>
-    <t>Success tambah saldo IDR</t>
-  </si>
-  <si>
-    <t>Success tambah saldo OCR KTP</t>
-  </si>
-  <si>
-    <t>Success tambah saldo OCR KK</t>
-  </si>
-  <si>
-    <t>Gagal topup karena tipe saldo kosong</t>
-  </si>
-  <si>
-    <t>$Username Billing</t>
-  </si>
-  <si>
-    <t>ADMESIGN</t>
-  </si>
-  <si>
-    <t>$Password Billing</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>$Tenant</t>
-  </si>
-  <si>
-    <t>$Vendor</t>
-  </si>
-  <si>
-    <t>$Tipe Saldo</t>
-  </si>
-  <si>
-    <t>$Tambah Saldo</t>
-  </si>
-  <si>
-    <t>$Nomor tagihan</t>
-  </si>
-  <si>
-    <t>$Catatan</t>
-  </si>
-  <si>
-    <t>$Tanggal Pembelian (YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t>2023-05-02</t>
-  </si>
-  <si>
-    <t>2023-05-05</t>
-  </si>
-  <si>
-    <t>Filter Saldo</t>
-  </si>
-  <si>
-    <t>Reason Failed</t>
-  </si>
-  <si>
     <t>;Fungsi pencarian gagal, no result</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Success create tenant</t>
-  </si>
-  <si>
-    <t>Mandatory tidak lengkap</t>
-  </si>
-  <si>
-    <t>Success edit services</t>
-  </si>
-  <si>
-    <t>Success Edit Tenant</t>
-  </si>
-  <si>
-    <t>Success ubah charge type</t>
-  </si>
-  <si>
-    <t>Is Mandatory Complete</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>ChargeType</t>
-  </si>
-  <si>
-    <t>Search Tenant</t>
-  </si>
-  <si>
-    <t>$NamaTenant</t>
-  </si>
-  <si>
-    <t>Roemah Finance</t>
-  </si>
-  <si>
-    <t>$Status</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Tenant</t>
-  </si>
-  <si>
-    <t>Sumber Jaya Makmur Finance</t>
-  </si>
-  <si>
-    <t>WOM Finance</t>
-  </si>
-  <si>
-    <t>$KodeTenant</t>
-  </si>
-  <si>
-    <t>SJM</t>
-  </si>
-  <si>
-    <t>ESIGN/ADINS</t>
-  </si>
-  <si>
-    <t>$LabelRefNumber</t>
-  </si>
-  <si>
-    <t>OTP</t>
-  </si>
-  <si>
-    <t>Auto Generate API Key</t>
-  </si>
-  <si>
-    <t>API Key</t>
-  </si>
-  <si>
-    <t>Batas Saldo</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>OCR BPKB;Liveness Face Compare;Verifikasi Dukcapil Tanpa Biometrik;Id Forgery</t>
-  </si>
-  <si>
-    <t>200;300;400;100</t>
-  </si>
-  <si>
-    <t>100;200;300;400</t>
-  </si>
-  <si>
-    <t>Penerima Email Reminder</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>williswy@ad-ins.com;williswy@gmail.com</t>
-  </si>
-  <si>
-    <t>wwf@ad-ins.com;wwf@gmail.com</t>
-  </si>
-  <si>
-    <t>$Email User Admin</t>
-  </si>
-  <si>
-    <t>williswy@ad-ins.com</t>
-  </si>
-  <si>
-    <t>wwf@ad-ins.com</t>
-  </si>
-  <si>
-    <t>$Kode Akses User Admin</t>
-  </si>
-  <si>
-    <t>password1111</t>
-  </si>
-  <si>
-    <t>password1234</t>
-  </si>
-  <si>
-    <t>Services Setting</t>
-  </si>
-  <si>
-    <t>ServicesCheck</t>
-  </si>
-  <si>
-    <t>OTP;DOC;SDT;SMS</t>
-  </si>
-  <si>
-    <t>VendorCheck</t>
-  </si>
-  <si>
-    <t>DJP;ESG;INDR;DIGI</t>
-  </si>
-  <si>
-    <t>ServicesUncheck</t>
-  </si>
-  <si>
-    <t>OCR_KTP;OCR_REKKORAN_BCA;OCR_REKKORAN_MANDIRI;OCR_STNK</t>
-  </si>
-  <si>
-    <t>VendorUncheck</t>
-  </si>
-  <si>
-    <t>VIDA;VIDA;ESG;DIGI</t>
-  </si>
-  <si>
-    <t>ESG;ESG;ESG;ESG</t>
-  </si>
-  <si>
-    <t>Balance ChargeType Check</t>
-  </si>
-  <si>
-    <t>OCR_KTP;OCR_NPWP</t>
-  </si>
-  <si>
-    <t>Balance ChargeType Uncheck</t>
-  </si>
-  <si>
-    <t>OCR_KK;DOC</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>DJP</t>
-  </si>
-  <si>
-    <t>VRF</t>
-  </si>
-  <si>
-    <t>Verification</t>
-  </si>
-  <si>
-    <t>INDR</t>
-  </si>
-  <si>
-    <t>DUKCAPIL_NOBIO</t>
-  </si>
-  <si>
-    <t>Verifikasi Dukcapil Tanpa Biometrik</t>
-  </si>
-  <si>
-    <t>ESG</t>
-  </si>
-  <si>
-    <t>OCR_BUKU_TABUNGAN_MANDIRI</t>
-  </si>
-  <si>
-    <t>OCR BUKU TABUNGAN MANDIRI</t>
-  </si>
-  <si>
-    <t>DIGI</t>
-  </si>
-  <si>
-    <t>OCR_KTP</t>
-  </si>
-  <si>
-    <t>OCR_NPWP</t>
-  </si>
-  <si>
-    <t>OCR NPWP</t>
-  </si>
-  <si>
-    <t>OCR_BPKB</t>
-  </si>
-  <si>
-    <t>OCR_KK</t>
-  </si>
-  <si>
-    <t>SMS</t>
-  </si>
-  <si>
-    <t>SMS Notif</t>
-  </si>
-  <si>
-    <t>SDT</t>
-  </si>
-  <si>
-    <t>Stamp Duty</t>
-  </si>
-  <si>
-    <t>OCR_STNK</t>
-  </si>
-  <si>
-    <t>LIVENESS_FACECOMPARE</t>
-  </si>
-  <si>
-    <t>Liveness Face Compare</t>
-  </si>
-  <si>
-    <t>CDE</t>
-  </si>
-  <si>
-    <t>Credit Decision Engine</t>
-  </si>
-  <si>
-    <t>VALIDASI_SAMSAT</t>
-  </si>
-  <si>
-    <t>Validasi Samsat</t>
-  </si>
-  <si>
-    <t>FACE_COMPARE</t>
-  </si>
-  <si>
-    <t>Face Compare</t>
-  </si>
-  <si>
-    <t>LIVENESS</t>
-  </si>
-  <si>
-    <t>Liveness</t>
-  </si>
-  <si>
-    <t>ROBO_SLIK</t>
-  </si>
-  <si>
-    <t>Robot Slik</t>
-  </si>
-  <si>
-    <t>IDFORGERY_OCRKTP</t>
-  </si>
-  <si>
-    <t>ID Forgery + OCR KTP</t>
-  </si>
-  <si>
-    <t>ID_FORGERY</t>
-  </si>
-  <si>
-    <t>ID Forgery</t>
-  </si>
-  <si>
-    <t>DUKCAPIL_VIDA</t>
-  </si>
-  <si>
-    <t>Success search with all criteria and all function active</t>
-  </si>
-  <si>
-    <t>Success search dengan field pengguna dan nama dokumen tidak terisi</t>
-  </si>
-  <si>
-    <t>Success search dengan mengisi field mandatory saja</t>
-  </si>
-  <si>
-    <t>Tipe Transaksi</t>
-  </si>
-  <si>
-    <t>Tanggal Transaksi Dari</t>
-  </si>
-  <si>
-    <t>2023-05-01</t>
-  </si>
-  <si>
-    <t>Pengguna</t>
-  </si>
-  <si>
-    <t>ADMIN ESIGN</t>
-  </si>
-  <si>
-    <t>Hasil Proses</t>
-  </si>
-  <si>
-    <t>Ref Number</t>
-  </si>
-  <si>
-    <t>Nama Dokumen</t>
-  </si>
-  <si>
-    <t>Tanggal Transaksi hingga</t>
-  </si>
-  <si>
-    <t>2023-05-03</t>
-  </si>
-  <si>
-    <t>Kantor</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>;Table error/tidak muncul</t>
   </si>
   <si>
-    <t>Success verifikasi</t>
-  </si>
-  <si>
-    <t>Data Login</t>
-  </si>
-  <si>
-    <t>API KEY controller</t>
-  </si>
-  <si>
-    <t>Tipe API KEY</t>
-  </si>
-  <si>
-    <t>OCR BPKB;Liveness Face Compare;Verifikasi Dukcapil Tanpa Biometrik;OTP</t>
-  </si>
-  <si>
-    <t>FZ34jV</t>
-  </si>
-  <si>
-    <t>;Submit Gagal</t>
-  </si>
-  <si>
-    <t>Gagal search karena nama tenant terdaftar tidak kapital</t>
-  </si>
-  <si>
-    <t>WIKY WILLIS COMPANY</t>
-  </si>
-  <si>
-    <t>o63JZ8</t>
-  </si>
-  <si>
-    <t>WWC</t>
+    <t>Hit menggunakan file dengan extension selain .jpg, .jpeg, .png</t>
+  </si>
+  <si>
+    <t>Hit API menggunakan foto blur dengan intensitas tinggi</t>
+  </si>
+  <si>
+    <t>Hit menggunakan foto putih bersih</t>
+  </si>
+  <si>
+    <t>Hit menggunaka foto dengan resolusi diatas 3840x2160</t>
+  </si>
+  <si>
+    <t>Use Verifikasi Identitas Dukcapil</t>
+  </si>
+  <si>
+    <t>Success hit, lalu cek mutasi menggunakan tipe transaksi Use, bukan All</t>
+  </si>
+  <si>
+    <t>Success create role baru</t>
+  </si>
+  <si>
+    <t>SEDAYU@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>P@ssw0rd123</t>
+  </si>
+  <si>
+    <t>Filter Role</t>
+  </si>
+  <si>
+    <t>Nama Role</t>
+  </si>
+  <si>
+    <t>Status Role</t>
+  </si>
+  <si>
+    <t>Edit Role</t>
+  </si>
+  <si>
+    <t>SUPERVISOR</t>
+  </si>
+  <si>
+    <t>$Nama Role</t>
+  </si>
+  <si>
+    <t>$Edit Status Role</t>
+  </si>
+  <si>
+    <t>New Role</t>
+  </si>
+  <si>
+    <t>$Add RoleName</t>
+  </si>
+  <si>
+    <t>Setting Role</t>
+  </si>
+  <si>
+    <t>API_DOCUMENTATION</t>
+  </si>
+  <si>
+    <t>API_KEY</t>
+  </si>
+  <si>
+    <t>BALANCE</t>
+  </si>
+  <si>
+    <t>COUPON</t>
+  </si>
+  <si>
+    <t>DASHBOARD</t>
+  </si>
+  <si>
+    <t>LIST_SERVICE_PRICE</t>
+  </si>
+  <si>
+    <t>API Documentation</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>OCR Monitoring Dashboard</t>
+  </si>
+  <si>
+    <t>List Service Price</t>
+  </si>
+  <si>
+    <t>API_KEY;BALANCE;LIST_SERVICE_PRICE</t>
+  </si>
+  <si>
+    <t>$MenuChecked</t>
+  </si>
+  <si>
+    <t>$MenuUnchecked</t>
+  </si>
+  <si>
+    <t>Username Login</t>
+  </si>
+  <si>
+    <t>Password Login</t>
+  </si>
+  <si>
+    <t>Menu Code</t>
+  </si>
+  <si>
+    <t>NEWROLEX1</t>
+  </si>
+  <si>
+    <t>Success edit role</t>
+  </si>
+  <si>
+    <t>Success ChargeType</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -1809,12 +1921,33 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1844,6 +1977,27 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1944,14 +2098,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1959,12 +2113,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1981,7 +2135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1993,13 +2147,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2630,7 +2796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3898,10 +4064,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -3921,9 +4088,10 @@
     <col min="13" max="16" width="35.7265625" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="35.1796875" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="36.1796875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="35.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3970,16 +4138,19 @@
         <v>1</v>
       </c>
       <c r="P1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>44</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3993,22 +4164,22 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>401</v>
+        <v>572</v>
       </c>
       <c r="F2" t="s">
-        <v>401</v>
+        <v>572</v>
       </c>
       <c r="G2" t="s">
-        <v>402</v>
+        <v>573</v>
       </c>
       <c r="H2" t="s">
         <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>403</v>
+        <v>574</v>
       </c>
       <c r="J2" t="s">
-        <v>403</v>
+        <v>574</v>
       </c>
       <c r="K2" t="s">
         <v>206</v>
@@ -4020,78 +4191,72 @@
         <v>206</v>
       </c>
       <c r="N2" t="s">
-        <v>404</v>
+        <v>575</v>
       </c>
       <c r="O2" t="s">
         <v>86</v>
       </c>
-      <c r="P2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>86</v>
-      </c>
-      <c r="R2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="29">
+    </row>
+    <row r="3" spans="1:19" ht="33.5" customHeight="1">
       <c r="A3" t="s">
         <v>139</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>416</v>
-      </c>
       <c r="N3" s="3" t="s">
-        <v>417</v>
+        <v>581</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>418</v>
+        <v>582</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>419</v>
+        <v>335</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>420</v>
+        <v>583</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>584</v>
+      </c>
+      <c r="S3" s="27" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -4163,15 +4328,19 @@
         <f>COUNTIFS($A$8:$A$38,"*$*",R8:R38,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" s="1" customFormat="1">
+      <c r="S4">
+        <f>COUNTIFS($A$8:$A$38,"*$*",S8:S38,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="29">
+    <row r="8" spans="1:19" ht="29">
       <c r="A8" s="18" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>298</v>
@@ -4224,66 +4393,72 @@
       <c r="R8" s="3" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="S8" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>415</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="B10" s="20">
         <v>7183259386136510</v>
@@ -4336,176 +4511,188 @@
       <c r="R10" s="20">
         <v>7183259386136510</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" s="20">
+        <v>7183259386136510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="F11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="G11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="H11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="I11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="J11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="L11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="M11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="N11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="O11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="P11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="Q11" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="R11" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>420</v>
+      </c>
+      <c r="S11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="Q12" s="22" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="R12" s="22" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>423</v>
+      </c>
+      <c r="S12" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="C13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="D13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="E13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="F13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="H13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="I13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="J13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="K13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="L13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="M13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="N13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="O13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="P13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="Q13" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="R13" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>427</v>
+      </c>
+      <c r="S13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>167</v>
       </c>
@@ -4560,8 +4747,11 @@
       <c r="R14" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" s="1" customFormat="1">
+      <c r="S14" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>169</v>
       </c>
@@ -4800,7 +4990,7 @@
         <v>321</v>
       </c>
       <c r="B22" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -4850,6 +5040,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B9" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4860,8 +5051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -4893,16 +5084,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>438</v>
+        <v>577</v>
       </c>
       <c r="C2" t="s">
-        <v>438</v>
+        <v>577</v>
       </c>
       <c r="D2" t="s">
-        <v>438</v>
+        <v>577</v>
       </c>
       <c r="E2" t="s">
-        <v>439</v>
+        <v>578</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29">
@@ -4910,16 +5101,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C3" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="D3" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4950,36 +5141,36 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B8" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="C8" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="D8" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="E8" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="C9" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="D9" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="E9" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5018,7 +5209,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -5035,7 +5226,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
@@ -5052,7 +5243,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="B14" t="s">
         <v>278</v>
@@ -5066,7 +5257,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -5083,24 +5274,24 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B16" s="16">
-        <v>1130</v>
+        <v>1411</v>
       </c>
       <c r="C16" s="16">
-        <v>1139</v>
+        <v>1412</v>
       </c>
       <c r="D16" s="16">
-        <v>1124</v>
+        <v>1413</v>
       </c>
       <c r="E16" s="16">
-        <v>1116</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="B17" t="str">
         <f>CONCATENATE("Isiulang ",B14)</f>
@@ -5121,24 +5312,24 @@
     </row>
     <row r="18" spans="1:5" ht="29">
       <c r="A18" s="3" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>455</v>
+        <v>576</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>456</v>
+        <v>576</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>456</v>
+        <v>576</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>456</v>
+        <v>576</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1">
       <c r="A19" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5183,6 +5374,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5191,8 +5383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -5219,7 +5411,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -5230,25 +5422,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B2" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="C2" t="s">
-        <v>439</v>
+        <v>568</v>
       </c>
       <c r="D2" t="s">
-        <v>459</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>460</v>
+        <v>569</v>
+      </c>
+      <c r="E2" t="s">
+        <v>571</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29">
@@ -5256,27 +5448,27 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="B4" s="5">
         <f>IF(B7="New",COUNTIFS($A$12:$A$23,"*$*",B12:B23,""),IF(B7="Service",COUNTIFS($A$9:$A$10,"*$*",B9:B10,""),IF(B7="Edit",COUNTIFS($A$9:$A$21,"*$*",B9:B21,""),0)))</f>
@@ -5323,30 +5515,30 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -5357,45 +5549,45 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="6" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -5406,49 +5598,49 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B14" s="5">
         <v>202304426</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -5459,7 +5651,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>34</v>
@@ -5474,22 +5666,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B16" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1">
       <c r="A17" s="6" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -5500,37 +5692,37 @@
     </row>
     <row r="18" spans="1:7" ht="43.5">
       <c r="A18" s="5" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="8" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -5541,52 +5733,52 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="B21" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="5" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B22" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="5" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1">
       <c r="A24" s="6" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -5594,69 +5786,69 @@
       <c r="E24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="29">
       <c r="A25" s="5" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>504</v>
+        <v>490</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>494</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="29">
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>508</v>
+        <v>490</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>490</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -5664,12 +5856,12 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -5677,74 +5869,74 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1">
-      <c r="A31" s="26" t="s">
-        <v>516</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="34" t="s">
+        <v>502</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>137</v>
@@ -5753,16 +5945,16 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>130</v>
@@ -5771,7 +5963,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>133</v>
@@ -5780,25 +5972,25 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>135</v>
@@ -5807,82 +5999,82 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="C52" s="5"/>
     </row>
@@ -5920,7 +6112,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -5950,7 +6142,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>459</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5">
@@ -5958,13 +6150,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5986,12 +6178,12 @@
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="B8" t="s">
         <v>130</v>
@@ -6005,7 +6197,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="B9" t="s">
         <v>168</v>
@@ -6016,27 +6208,27 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="B11" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="B12" t="s">
         <v>168</v>
@@ -6047,7 +6239,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="B13">
         <v>1234</v>
@@ -6058,7 +6250,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="B14" t="str">
         <f>B8</f>
@@ -6067,19 +6259,19 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="B16" t="s">
         <v>168</v>
@@ -6090,7 +6282,7 @@
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -6128,7 +6320,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="B24" t="s">
         <v>53</v>
@@ -6144,10 +6336,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 C12 D12" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"All,OCR Process is successful,OCR Process result is False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 C16 D16" xr:uid="{00000000-0002-0000-0E00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:D16" xr:uid="{00000000-0002-0000-0E00-000001000000}">
       <formula1>"All,HEAD OFFICE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6160,7 +6352,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -6182,7 +6374,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6190,7 +6382,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6204,7 +6396,7 @@
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6225,12 +6417,12 @@
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1">
       <c r="A10" s="2" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
@@ -6243,6 +6435,312 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6F7591-4557-47F0-84A5-A61172818A15}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>587</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>618</v>
+      </c>
+      <c r="D3" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4">
+        <f>IF(B7="New", COUNTIFS($A$19, "*$*", B19, ""), IF(B7="Edit", COUNTIFS($A$16:$A$17, "$", B16:B17, ""), IF(B7="Settings", COUNTIFS($A$21:$A$22, "$", B21:B22, ""), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>IF(C7="New", COUNTIFS($A$19, "*$*", C19, ""), IF(C7="Edit", COUNTIFS($A$16:$A$17, "$", C16:C17, ""), IF(C7="Settings", COUNTIFS($A$21:$A$22, "$", C21:C22, ""), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>IF(D7="New", COUNTIFS($A$19, "*$*", D19, ""), IF(D7="Edit", COUNTIFS($A$16:$A$17, "$", D16:D17, ""), IF(D7="Settings", COUNTIFS($A$21:$A$22, "$", D21:D22, ""), 0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="30" customFormat="1">
+      <c r="A9" s="30" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="29" t="s">
+        <v>614</v>
+      </c>
+      <c r="B10" t="s">
+        <v>588</v>
+      </c>
+      <c r="C10" t="s">
+        <v>588</v>
+      </c>
+      <c r="D10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="29" t="s">
+        <v>615</v>
+      </c>
+      <c r="B11" t="s">
+        <v>589</v>
+      </c>
+      <c r="C11" t="s">
+        <v>589</v>
+      </c>
+      <c r="D11" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="30" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="29" t="s">
+        <v>591</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>594</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>594</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="29" t="s">
+        <v>592</v>
+      </c>
+      <c r="B14" t="s">
+        <v>462</v>
+      </c>
+      <c r="C14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D14" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1">
+      <c r="A15" s="30" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="29" t="s">
+        <v>595</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>594</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>594</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="29" t="s">
+        <v>596</v>
+      </c>
+      <c r="B17" t="s">
+        <v>462</v>
+      </c>
+      <c r="C17" t="s">
+        <v>462</v>
+      </c>
+      <c r="D17" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="30" customFormat="1">
+      <c r="A18" s="30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="29" t="s">
+        <v>598</v>
+      </c>
+      <c r="B19" t="s">
+        <v>617</v>
+      </c>
+      <c r="C19" t="s">
+        <v>617</v>
+      </c>
+      <c r="D19" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1">
+      <c r="A20" s="30" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29">
+      <c r="A21" s="29" t="s">
+        <v>612</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>611</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>611</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="29" t="s">
+        <v>613</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>602</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>602</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1">
+      <c r="A24" s="30" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="28" t="s">
+        <v>600</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:D7" xr:uid="{C823D92C-5C50-4109-94F8-767C8D796365}">
+      <formula1>"Edit, Settings, New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:D14 B17:D17" xr:uid="{F71850C3-0E93-492F-B4B5-CC1D6A2203C8}">
+      <formula1>"All,Active,Inactive"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6523,7 +7021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -7256,7 +7754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -7840,7 +8338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
@@ -9449,8 +9947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -10218,9 +10716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane xSplit="18280" topLeftCell="T1"/>
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="I3" sqref="I3"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
APIAAS User Management - User AT100 Done
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706B954-B6A1-49FB-9EB9-85218EF53422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D820C2-D793-4E15-BEC4-DA82CEF04FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="Saldo" sheetId="15" r:id="rId15"/>
     <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
     <sheet name="Role" sheetId="17" r:id="rId17"/>
+    <sheet name="User" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="653">
   <si>
     <t>Status</t>
   </si>
@@ -1912,6 +1913,102 @@
   </si>
   <si>
     <t>Settings</t>
+  </si>
+  <si>
+    <t>Misalkan yang di check : API_KEY dan BALANCE, maka sisanya harus masuk ke kolom uncheck</t>
+  </si>
+  <si>
+    <t>** untuk penggunaan Uncheck Menu diusahakan kebalikan dari yang di check</t>
+  </si>
+  <si>
+    <t>Filter User</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>$Email</t>
+  </si>
+  <si>
+    <t>$FirstName</t>
+  </si>
+  <si>
+    <t>$LastName</t>
+  </si>
+  <si>
+    <t>$Password</t>
+  </si>
+  <si>
+    <t>$Role</t>
+  </si>
+  <si>
+    <t>Edit User</t>
+  </si>
+  <si>
+    <t>$Firstname</t>
+  </si>
+  <si>
+    <t>$Status Aktivasi</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Success create user baru</t>
+  </si>
+  <si>
+    <t>FRENCENT.KINSELTON@AD-INS.COM</t>
+  </si>
+  <si>
+    <t>KINGJOJO@GM.COM</t>
+  </si>
+  <si>
+    <t>KING</t>
+  </si>
+  <si>
+    <t>JOJO</t>
+  </si>
+  <si>
+    <t>P@ssword123</t>
+  </si>
+  <si>
+    <t>3NEWROLE2</t>
+  </si>
+  <si>
+    <t>ResendController</t>
+  </si>
+  <si>
+    <t>ShouldResendVerif?</t>
+  </si>
+  <si>
+    <t>New(Add) User</t>
+  </si>
+  <si>
+    <t>Success edit user baru</t>
+  </si>
+  <si>
+    <t>KEGAR@GM.COM</t>
+  </si>
+  <si>
+    <t>KEVIN</t>
+  </si>
+  <si>
+    <t>EDGAR</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Ramsay</t>
+  </si>
+  <si>
+    <t>3NEWROLE9</t>
+  </si>
+  <si>
+    <t>Sukses Resend verif email saja</t>
+  </si>
+  <si>
+    <t>;Button Resend tidak muncul</t>
   </si>
 </sst>
 </file>
@@ -1921,12 +2018,33 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1996,6 +2114,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2098,14 +2222,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2113,12 +2237,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2135,7 +2259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2147,25 +2271,33 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2173,7 +2305,78 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -5374,7 +5577,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5873,11 +6076,11 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="38" t="s">
         <v>502</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
@@ -6442,8 +6645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6F7591-4557-47F0-84A5-A61172818A15}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6451,7 +6654,7 @@
     <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24.36328125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6492,15 +6695,15 @@
         <v>452</v>
       </c>
       <c r="B4">
-        <f>IF(B7="New", COUNTIFS($A$19, "*$*", B19, ""), IF(B7="Edit", COUNTIFS($A$16:$A$17, "$", B16:B17, ""), IF(B7="Settings", COUNTIFS($A$21:$A$22, "$", B21:B22, ""), 0)))</f>
+        <f>IF(B7="New",COUNTIFS($A$19,"*$*",B19,""),IF(B7="Edit",COUNTIFS($A$13:$A$17,"$",B13:B17,""),IF(B7="Settings",COUNTIFS($A$21:$A$22,"$",B21:B22,""),IF(B7="Settings",COUNTIFS($A$13:$A$14,"$",B13:B14,""),0))))</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>IF(C7="New", COUNTIFS($A$19, "*$*", C19, ""), IF(C7="Edit", COUNTIFS($A$16:$A$17, "$", C16:C17, ""), IF(C7="Settings", COUNTIFS($A$21:$A$22, "$", C21:C22, ""), 0)))</f>
+        <f t="shared" ref="C4:D4" si="0">IF(C7="New",COUNTIFS($A$19,"*$*",C19,""),IF(C7="Edit",COUNTIFS($A$13:$A$17,"$",C13:C17,""),IF(C7="Settings",COUNTIFS($A$21:$A$22,"$",C21:C22,""),IF(C7="Settings",COUNTIFS($A$13:$A$14,"$",C13:C14,""),0))))</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>IF(D7="New", COUNTIFS($A$19, "*$*", D19, ""), IF(D7="Edit", COUNTIFS($A$16:$A$17, "$", D16:D17, ""), IF(D7="Settings", COUNTIFS($A$21:$A$22, "$", D21:D22, ""), 0)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6665,7 +6868,7 @@
       <c r="C22" s="29" t="s">
         <v>602</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="34" t="s">
         <v>602</v>
       </c>
     </row>
@@ -6689,6 +6892,9 @@
       <c r="B26" s="28" t="s">
         <v>606</v>
       </c>
+      <c r="C26" s="34" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
@@ -6697,6 +6903,9 @@
       <c r="B27" s="28" t="s">
         <v>472</v>
       </c>
+      <c r="C27" s="34" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
@@ -6731,12 +6940,400 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A16:XFD17">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>OR(A$7="Settings",A$7="New")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:XFD19">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>OR(A$7="Settings",A$7="Edit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:XFD22">
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>OR(A$7="Edit",A$7="New")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:XFD14">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>A$7="New"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:D7" xr:uid="{C823D92C-5C50-4109-94F8-767C8D796365}">
       <formula1>"Edit, Settings, New"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:D14 B17:D17" xr:uid="{F71850C3-0E93-492F-B4B5-CC1D6A2203C8}">
       <formula1>"All,Active,Inactive"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0F381-544A-4B69-ADA2-FCE56D2FAA0F}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>634</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>644</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4">
+        <f>IF(B7="New",COUNTIFS($A$17:$A$21,"*$*",B17:B21,""),IF(B7="Edit",COUNTIFS($A$23:$A$26,"$",B23:B26,""),0))</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="0">IF(C7="New",COUNTIFS($A$17:$A$21,"*$*",C17:C21,""),IF(C7="Edit",COUNTIFS($A$23:$A$26,"$",C23:C26,""),0))</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="30" t="s">
+        <v>559</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="29" t="s">
+        <v>614</v>
+      </c>
+      <c r="B10" t="s">
+        <v>588</v>
+      </c>
+      <c r="C10" t="s">
+        <v>588</v>
+      </c>
+      <c r="D10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="29" t="s">
+        <v>615</v>
+      </c>
+      <c r="B11" t="s">
+        <v>589</v>
+      </c>
+      <c r="C11" t="s">
+        <v>589</v>
+      </c>
+      <c r="D11" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="30" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29">
+      <c r="A13" t="s">
+        <v>479</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>461</v>
+      </c>
+      <c r="B14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>624</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1">
+      <c r="A16" s="30" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="35" t="s">
+        <v>625</v>
+      </c>
+      <c r="B17" t="s">
+        <v>645</v>
+      </c>
+      <c r="C17" t="s">
+        <v>636</v>
+      </c>
+      <c r="D17" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="35" t="s">
+        <v>626</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>646</v>
+      </c>
+      <c r="C18" t="s">
+        <v>637</v>
+      </c>
+      <c r="D18" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="35" t="s">
+        <v>627</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>647</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>638</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="B20" t="s">
+        <v>639</v>
+      </c>
+      <c r="C20" t="s">
+        <v>639</v>
+      </c>
+      <c r="D20" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="35" t="s">
+        <v>629</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1">
+      <c r="A22" s="30" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="35" t="s">
+        <v>631</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>648</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>648</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="35" t="s">
+        <v>627</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="35" t="s">
+        <v>629</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>650</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>650</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="35" t="s">
+        <v>632</v>
+      </c>
+      <c r="B26" t="s">
+        <v>633</v>
+      </c>
+      <c r="C26" t="s">
+        <v>633</v>
+      </c>
+      <c r="D26" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1">
+      <c r="A27" s="30" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="35" t="s">
+        <v>642</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <conditionalFormatting sqref="A13:XFD13">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>A$7="New"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:XFD21">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>A$7="Edit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>A$7="Verification"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:XFD26">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>A$7="New"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>A$7="Verification"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:XFD15">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>A$7="New"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:D14" xr:uid="{7726A9FE-EE87-4157-AAC4-293F5CF8F796}">
+      <formula1>"All,Active,Inactive,Unverified"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:D26" xr:uid="{23A658F0-579B-4EEE-887A-7CC539F710B6}">
+      <formula1>"Active, Inactive"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:D28" xr:uid="{2E925797-1F27-42D7-B0B2-C0E35BB3EBEF}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:D7" xr:uid="{A873D311-6C7B-4DCC-BE02-B8A1DB4929FB}">
+      <formula1>"New,Edit,Verification"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Next Codacy Review(2) + Progress up to AT 100 User Management-User
</commit_message>
<xml_diff>
--- a/Excel/2. APIAAS.xlsx
+++ b/Excel/2. APIAAS.xlsx
@@ -1,44 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{45D02DF8-3B67-4703-8069-956E1313A626}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3037B500-8458-4611-9C1D-1BD5E91283CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="11" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" r:id="rId1" sheetId="1"/>
-    <sheet name="Edit Profile" r:id="rId2" sheetId="2"/>
-    <sheet name="API KEY" r:id="rId3" sheetId="3"/>
-    <sheet name="Dokumentasi API" r:id="rId4" sheetId="4"/>
-    <sheet name="OCR KTP" r:id="rId5" sheetId="5"/>
-    <sheet name="OCR KK" r:id="rId6" sheetId="6"/>
-    <sheet name="OCR STNK" r:id="rId7" sheetId="7"/>
-    <sheet name="OCR BPKB" r:id="rId8" sheetId="8"/>
-    <sheet name="OCR NPWP" r:id="rId9" sheetId="9"/>
-    <sheet name="OCR RK Mandiri" r:id="rId10" sheetId="10"/>
-    <sheet name="OCR RK BCA" r:id="rId11" sheetId="11"/>
-    <sheet name="Dukcapil(NonBiom)" r:id="rId12" sheetId="12"/>
-    <sheet name="IsiSaldo" r:id="rId13" sheetId="13"/>
-    <sheet name="Tenant" r:id="rId14" sheetId="14"/>
-    <sheet name="Saldo" r:id="rId15" sheetId="15"/>
-    <sheet name="LayananSaya" r:id="rId16" sheetId="16"/>
-    <sheet name="Role" r:id="rId17" sheetId="17"/>
-    <sheet name="User" r:id="rId18" sheetId="18"/>
-    <sheet name="Cleansing Object" r:id="rId19" sheetId="19"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="API KEY" sheetId="3" r:id="rId3"/>
+    <sheet name="Dokumentasi API" sheetId="4" r:id="rId4"/>
+    <sheet name="OCR KTP" sheetId="5" r:id="rId5"/>
+    <sheet name="OCR KK" sheetId="6" r:id="rId6"/>
+    <sheet name="OCR STNK" sheetId="7" r:id="rId7"/>
+    <sheet name="OCR BPKB" sheetId="8" r:id="rId8"/>
+    <sheet name="OCR NPWP" sheetId="9" r:id="rId9"/>
+    <sheet name="OCR RK Mandiri" sheetId="10" r:id="rId10"/>
+    <sheet name="OCR RK BCA" sheetId="11" r:id="rId11"/>
+    <sheet name="Dukcapil(NonBiom)" sheetId="12" r:id="rId12"/>
+    <sheet name="IsiSaldo" sheetId="13" r:id="rId13"/>
+    <sheet name="Tenant" sheetId="14" r:id="rId14"/>
+    <sheet name="Saldo" sheetId="15" r:id="rId15"/>
+    <sheet name="LayananSaya" sheetId="16" r:id="rId16"/>
+    <sheet name="Role" sheetId="17" r:id="rId17"/>
+    <sheet name="User" sheetId="18" r:id="rId18"/>
+    <sheet name="Cleansing Object" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="890">
   <si>
     <t>Status</t>
   </si>
@@ -2646,6 +2646,83 @@
   </si>
   <si>
     <t>-;Done well</t>
+  </si>
+  <si>
+    <t>Add role dengan role name kosong</t>
+  </si>
+  <si>
+    <t>Add role dengan role name sudah ada di tenant yg sama</t>
+  </si>
+  <si>
+    <t>DXSUPERVROLEACCESS</t>
+  </si>
+  <si>
+    <t>Add role dengan kata pertama role name melebihi 15 huruf dan hanya 1 kata 
+(18 huruf)</t>
+  </si>
+  <si>
+    <t>DXSUPERVROLEACCESS SUPERUSER</t>
+  </si>
+  <si>
+    <t>Edit role dengan role name kosong</t>
+  </si>
+  <si>
+    <t>Edit role dengan role name sudah ada di tenant yg sama</t>
+  </si>
+  <si>
+    <t>SUPERVISOR_TESTING</t>
+  </si>
+  <si>
+    <t>NEWROLETESTING</t>
+  </si>
+  <si>
+    <t>3NEWROLE5</t>
+  </si>
+  <si>
+    <t>Edit role dengan role name sudah ada di tenant yg berbeda</t>
+  </si>
+  <si>
+    <t>2ROLEBARU2</t>
+  </si>
+  <si>
+    <t>ROLE SUPERQC</t>
+  </si>
+  <si>
+    <t>Edit role dengan ganti role name tapi tidak mengubah kata pertama</t>
+  </si>
+  <si>
+    <t>ROLE USERQC</t>
+  </si>
+  <si>
+    <t>ROLE SUPQC</t>
+  </si>
+  <si>
+    <t>ROLES USERQE</t>
+  </si>
+  <si>
+    <t>Edit role dengan ganti role name dan mengubah keseluruhan kata</t>
+  </si>
+  <si>
+    <t>Add role dengan kata pertama role name melebihi 15 huruf 
+(18 huruf) dan ada 2 kata</t>
+  </si>
+  <si>
+    <t>Edit role dengan kata pertama role name melebihi 15 huruf dan hanya 1 kata ; ubah kata pertama role name</t>
+  </si>
+  <si>
+    <t>Edit role dengan kata pertama role name melebihi 15 huruf dan hanya 1 kata ; tidak ubah kata pertama role name</t>
+  </si>
+  <si>
+    <t>Edit role dengan kata pertama role name melebihi 15 huruf dan ada 2 kata ; ubah kata pertama role name</t>
+  </si>
+  <si>
+    <t>Edit role dengan kata pertama role name melebihi 15 huruf dan ada 2 kata ; tidak ubah kata pertama role name</t>
+  </si>
+  <si>
+    <t>DXSUPERVROLEACESS SUPERUSER</t>
+  </si>
+  <si>
+    <t>DXSUPERVROLEACESS SUPER</t>
   </si>
 </sst>
 </file>
@@ -2655,12 +2732,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2885,118 +2969,143 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="56">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" ap